<commit_message>
v1.3 modify SRS after get comments
modify navigation SRS get comments on version 1.2 of SRS
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_SRS.xlsx
+++ b/LH_REQUIREMENTS/LH_SRS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="127">
   <si>
     <t>Feature</t>
   </si>
@@ -263,18 +263,12 @@
     <t>SRS-NAV-001</t>
   </si>
   <si>
-    <t>The system shall allow users to navigate between four predefined content categories.</t>
-  </si>
-  <si>
     <t>LH-CRS-NAVIGATION-002</t>
   </si>
   <si>
     <t>SRS-NAV-002</t>
   </si>
   <si>
-    <t>The system shall include a header navigation bar with tabs for each section and dropdowns for subsections.</t>
-  </si>
-  <si>
     <t>LH-CRS-NAVIGATION-003</t>
   </si>
   <si>
@@ -377,9 +371,6 @@
     <t>The system shall allow only .mp3 audio files to be uploaded. If another format (e.g., .wav) is selected, display the message: "Only MP3 format is allowed."</t>
   </si>
   <si>
-    <t>The message should be shown in a bigger area like next to the password field or in a popup</t>
-  </si>
-  <si>
     <t>The system shall ensure that the username is unique. If a duplicate username is detected, an error message shall be displayed, saying : This username is already used</t>
   </si>
   <si>
@@ -417,6 +408,21 @@
   </si>
   <si>
     <t>modify SRS after last version of SIQ and reviewers comments on version 1.1 of SRS</t>
+  </si>
+  <si>
+    <t>The message of all password requirements during registration be shown in a appropriate area next to the password field when user clicks on password field</t>
+  </si>
+  <si>
+    <t>The system include a header navigation bar with tabs for each section and clickable dropdowns for subsections.</t>
+  </si>
+  <si>
+    <t>The system allow users to navigate between four predefined content categories  ( ‘Sports’, ‘Scientific’,'Health','Economy').</t>
+  </si>
+  <si>
+    <t>v1.3</t>
+  </si>
+  <si>
+    <t>modify SRS get comments on version 1.2 of SRS</t>
   </si>
 </sst>
 </file>
@@ -679,6 +685,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -688,28 +700,22 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -995,7 +1001,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1025,7 +1031,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="30">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="34" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="21" t="s">
@@ -1042,7 +1048,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="30">
-      <c r="A3" s="33"/>
+      <c r="A3" s="35"/>
       <c r="B3" s="16" t="s">
         <v>12</v>
       </c>
@@ -1057,7 +1063,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="45">
-      <c r="A4" s="33"/>
+      <c r="A4" s="35"/>
       <c r="B4" s="21" t="s">
         <v>15</v>
       </c>
@@ -1071,8 +1077,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30">
-      <c r="A5" s="33"/>
+    <row r="5" spans="1:5" ht="45">
+      <c r="A5" s="35"/>
       <c r="B5" s="16" t="s">
         <v>17</v>
       </c>
@@ -1080,14 +1086,14 @@
         <v>18</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="60">
-      <c r="A6" s="33"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="21" t="s">
         <v>19</v>
       </c>
@@ -1095,14 +1101,14 @@
         <v>20</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30">
-      <c r="A7" s="33"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="30" t="s">
         <v>21</v>
       </c>
@@ -1117,84 +1123,84 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="45">
-      <c r="A8" s="33"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="30"/>
       <c r="C8" s="10" t="s">
         <v>56</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45">
-      <c r="A9" s="33"/>
-      <c r="B9" s="40" t="s">
+      <c r="A9" s="35"/>
+      <c r="B9" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30">
+      <c r="A10" s="35"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45">
+      <c r="A11" s="35"/>
+      <c r="B11" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="45">
+      <c r="A12" s="35"/>
+      <c r="B12" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30">
-      <c r="A10" s="33"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="45">
-      <c r="A11" s="33"/>
-      <c r="B11" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11" s="10" t="s">
+      <c r="C12" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="E12" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="45">
+      <c r="A13" s="36"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="45">
-      <c r="A12" s="33"/>
-      <c r="B12" s="40" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="45">
-      <c r="A13" s="34"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>90</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>92</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>8</v>
@@ -1202,7 +1208,7 @@
     </row>
     <row r="14" spans="1:5" s="13" customFormat="1" ht="15.75">
       <c r="A14" s="26" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B14" s="25" t="s">
         <v>62</v>
@@ -1220,13 +1226,13 @@
     <row r="15" spans="1:5" s="13" customFormat="1" ht="45">
       <c r="A15" s="27"/>
       <c r="B15" s="37" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>8</v>
@@ -1236,10 +1242,10 @@
       <c r="A16" s="27"/>
       <c r="B16" s="38"/>
       <c r="C16" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>8</v>
@@ -1249,10 +1255,10 @@
       <c r="A17" s="28"/>
       <c r="B17" s="39"/>
       <c r="C17" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E17" s="10" t="s">
         <v>8</v>
@@ -1324,11 +1330,11 @@
       <c r="A22" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="40" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>24</v>
@@ -1339,12 +1345,12 @@
     </row>
     <row r="23" spans="1:5" ht="45">
       <c r="A23" s="31"/>
-      <c r="B23" s="42"/>
+      <c r="B23" s="41"/>
       <c r="C23" s="12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E23" s="12" t="s">
         <v>8</v>
@@ -1352,12 +1358,12 @@
     </row>
     <row r="24" spans="1:5" ht="45">
       <c r="A24" s="31"/>
-      <c r="B24" s="42"/>
+      <c r="B24" s="41"/>
       <c r="C24" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>8</v>
@@ -1365,12 +1371,12 @@
     </row>
     <row r="25" spans="1:5" ht="45">
       <c r="A25" s="31"/>
-      <c r="B25" s="36"/>
+      <c r="B25" s="42"/>
       <c r="C25" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>8</v>
@@ -1385,7 +1391,7 @@
         <v>26</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>8</v>
@@ -1400,7 +1406,7 @@
         <v>28</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>8</v>
@@ -1415,7 +1421,7 @@
         <v>30</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E28" s="10" t="s">
         <v>8</v>
@@ -1430,7 +1436,7 @@
         <v>32</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E29" s="11" t="s">
         <v>8</v>
@@ -1445,7 +1451,7 @@
         <v>34</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E30" s="10" t="s">
         <v>8</v>
@@ -1485,16 +1491,16 @@
     </row>
     <row r="33" spans="1:7" ht="31.5">
       <c r="A33" s="17" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C33" s="11" t="s">
         <v>65</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E33" s="11" t="s">
         <v>8</v>
@@ -1504,16 +1510,16 @@
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1">
       <c r="A34" s="29" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>66</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>8</v>
@@ -1524,7 +1530,7 @@
     <row r="35" spans="1:7" ht="15" customHeight="1">
       <c r="A35" s="29"/>
       <c r="B35" s="16" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C35" s="11" t="s">
         <v>67</v>
@@ -1538,7 +1544,7 @@
       <c r="F35" s="15"/>
       <c r="G35" s="15"/>
     </row>
-    <row r="36" spans="1:7" ht="30">
+    <row r="36" spans="1:7" ht="45">
       <c r="A36" s="26" t="s">
         <v>70</v>
       </c>
@@ -1549,7 +1555,7 @@
         <v>72</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
       <c r="E36" s="10" t="s">
         <v>8</v>
@@ -1558,13 +1564,13 @@
     <row r="37" spans="1:7" ht="30">
       <c r="A37" s="27"/>
       <c r="B37" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C37" s="11" t="s">
-        <v>75</v>
-      </c>
       <c r="D37" s="11" t="s">
-        <v>76</v>
+        <v>123</v>
       </c>
       <c r="E37" s="11" t="s">
         <v>8</v>
@@ -1573,13 +1579,13 @@
     <row r="38" spans="1:7" ht="30">
       <c r="A38" s="28"/>
       <c r="B38" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D38" s="12" t="s">
         <v>77</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>79</v>
       </c>
       <c r="E38" s="10" t="s">
         <v>8</v>
@@ -1617,7 +1623,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1658,23 +1664,31 @@
     </row>
     <row r="3" spans="1:4" ht="56.25">
       <c r="A3" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D3" s="5">
         <v>45765</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.75">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="7"/>
+    <row r="4" spans="1:4" ht="37.5">
+      <c r="A4" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" s="5">
+        <v>45766</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="18.75">
       <c r="A5" s="3"/>

</xml_diff>

<commit_message>
v1.4 modify and add more SRS
1/modify "SRS-PUB-004" with more details
2/add more SRS to admin constrains "SRS-ADM-003"
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_SRS.xlsx
+++ b/LH_REQUIREMENTS/LH_SRS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LH_SRS" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="131">
   <si>
     <t>Feature</t>
   </si>
@@ -362,9 +362,6 @@
     <t>The system shall validate audio file size before upload and reject files exceeding 20MB, with the message: "Max size: 20MB."</t>
   </si>
   <si>
-    <t>The system shall count words in articles in real-time and prevent submission if the article exceeds 1000 words</t>
-  </si>
-  <si>
     <t>The system shall allow only .mp4 video files to be uploaded. If an unsupported format (e.g., .avi) is selected, display: "Only MP4 format is allowed."</t>
   </si>
   <si>
@@ -423,6 +420,22 @@
   </si>
   <si>
     <t>modify SRS get comments on version 1.2 of SRS</t>
+  </si>
+  <si>
+    <t>SRS-ADM-003</t>
+  </si>
+  <si>
+    <t>The system shall count words in articles in real-time and an error message  of "article body exceeds 1000 words"will be displayed and  prevent submission if the article exceeds 1000 words</t>
+  </si>
+  <si>
+    <t>v1.4</t>
+  </si>
+  <si>
+    <t>1/modify "SRS-PUB-004" with more details
+2/add more srs to admin constrains "SRS-ADM-003"</t>
+  </si>
+  <si>
+    <t>an error message of "user not found, please try a valid username or ID" must be shown when trying to delete not existing user</t>
   </si>
 </sst>
 </file>
@@ -594,7 +607,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -612,9 +625,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -998,608 +1008,622 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" style="23" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" style="23" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" style="22" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" style="22" customWidth="1"/>
     <col min="4" max="4" width="53.42578125" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19.5">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30">
-      <c r="A3" s="35"/>
-      <c r="B3" s="16" t="s">
+      <c r="A3" s="34"/>
+      <c r="B3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45">
-      <c r="A4" s="35"/>
-      <c r="B4" s="21" t="s">
+      <c r="A4" s="34"/>
+      <c r="B4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45">
-      <c r="A5" s="35"/>
-      <c r="B5" s="16" t="s">
+      <c r="A5" s="34"/>
+      <c r="B5" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="E5" s="11" t="s">
+      <c r="D5" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="60">
-      <c r="A6" s="35"/>
-      <c r="B6" s="21" t="s">
+      <c r="A6" s="34"/>
+      <c r="B6" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30">
+      <c r="A7" s="34"/>
+      <c r="B7" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45">
+      <c r="A8" s="34"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="30">
-      <c r="A7" s="35"/>
-      <c r="B7" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="45">
-      <c r="A8" s="35"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="10" t="s">
+      <c r="E8" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45">
+      <c r="A9" s="34"/>
+      <c r="B9" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30">
+      <c r="A10" s="34"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45">
+      <c r="A11" s="34"/>
+      <c r="B11" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="45">
+      <c r="A12" s="34"/>
+      <c r="B12" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="45">
+      <c r="A13" s="35"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="12" customFormat="1" ht="15.75">
+      <c r="A14" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="12" customFormat="1" ht="45">
+      <c r="A15" s="26"/>
+      <c r="B15" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="12" customFormat="1" ht="30">
+      <c r="A16" s="26"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="12" customFormat="1" ht="30">
+      <c r="A17" s="27"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30">
+      <c r="A18" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30">
+      <c r="A19" s="28"/>
+      <c r="B19" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30">
+      <c r="A20" s="28"/>
+      <c r="B20" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75">
+      <c r="A21" s="28"/>
+      <c r="B21" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" customHeight="1">
+      <c r="A22" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="45">
+      <c r="A23" s="30"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="45">
+      <c r="A24" s="30"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="45">
+      <c r="A25" s="30"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="45">
+      <c r="A26" s="30"/>
+      <c r="B26" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="45">
+      <c r="A27" s="30"/>
+      <c r="B27" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="60">
+      <c r="A28" s="30"/>
+      <c r="B28" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="45">
+      <c r="A29" s="30"/>
+      <c r="B29" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="45">
+      <c r="A30" s="30"/>
+      <c r="B30" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="30">
+      <c r="A31" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30">
+      <c r="A32" s="28"/>
+      <c r="B32" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="31.5">
+      <c r="A33" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45">
-      <c r="A9" s="35"/>
-      <c r="B9" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30">
-      <c r="A10" s="35"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="45">
-      <c r="A11" s="35"/>
-      <c r="B11" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="45">
-      <c r="A12" s="35"/>
-      <c r="B12" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="45">
-      <c r="A13" s="36"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="13" customFormat="1" ht="15.75">
-      <c r="A14" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="13" customFormat="1" ht="45">
-      <c r="A15" s="27"/>
-      <c r="B15" s="37" t="s">
-        <v>119</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="13" customFormat="1" ht="30">
-      <c r="A16" s="27"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="13" customFormat="1" ht="30">
-      <c r="A17" s="28"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30">
-      <c r="A18" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="30">
-      <c r="A19" s="29"/>
-      <c r="B19" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30">
-      <c r="A20" s="29"/>
-      <c r="B20" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75">
-      <c r="A21" s="29"/>
-      <c r="B21" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="30" customHeight="1">
-      <c r="A22" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="45">
-      <c r="A23" s="31"/>
-      <c r="B23" s="41"/>
-      <c r="C23" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="45">
-      <c r="A24" s="31"/>
-      <c r="B24" s="41"/>
-      <c r="C24" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="45">
-      <c r="A25" s="31"/>
-      <c r="B25" s="42"/>
-      <c r="C25" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="45">
-      <c r="A26" s="31"/>
-      <c r="B26" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="45">
-      <c r="A27" s="31"/>
-      <c r="B27" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="30">
-      <c r="A28" s="31"/>
-      <c r="B28" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="45">
-      <c r="A29" s="31"/>
-      <c r="B29" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="45">
-      <c r="A30" s="31"/>
-      <c r="B30" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="30">
-      <c r="A31" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="30">
-      <c r="A32" s="29"/>
-      <c r="B32" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="31.5">
-      <c r="A33" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="B33" s="16" t="s">
+      <c r="E33" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+    </row>
+    <row r="34" spans="1:7" ht="30" customHeight="1">
+      <c r="A34" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+    </row>
+    <row r="35" spans="1:7" ht="15" customHeight="1">
+      <c r="A35" s="34"/>
+      <c r="B35" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="C33" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-    </row>
-    <row r="34" spans="1:7" ht="30" customHeight="1">
-      <c r="A34" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="B34" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-    </row>
-    <row r="35" spans="1:7" ht="15" customHeight="1">
-      <c r="A35" s="29"/>
-      <c r="B35" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D35" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E35" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-    </row>
-    <row r="36" spans="1:7" ht="45">
-      <c r="A36" s="26" t="s">
+      <c r="E35" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+    </row>
+    <row r="36" spans="1:7" ht="15" customHeight="1">
+      <c r="A36" s="35"/>
+      <c r="B36" s="41"/>
+      <c r="C36" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+    </row>
+    <row r="37" spans="1:7" ht="45">
+      <c r="A37" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="B36" s="20" t="s">
+      <c r="B37" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C37" s="9" t="s">
         <v>72</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="30">
-      <c r="A37" s="27"/>
-      <c r="B37" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>74</v>
       </c>
       <c r="D37" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="E37" s="11" t="s">
+      <c r="E37" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30">
-      <c r="A38" s="28"/>
-      <c r="B38" s="20" t="s">
+      <c r="A38" s="26"/>
+      <c r="B38" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="30">
+      <c r="A39" s="27"/>
+      <c r="B39" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C39" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D38" s="12" t="s">
+      <c r="D39" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E38" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="18"/>
-      <c r="B39" s="22"/>
+      <c r="E39" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="17"/>
+      <c r="B40" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="A36:A38"/>
+  <mergeCells count="13">
+    <mergeCell ref="A37:A39"/>
     <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A34:A35"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="A22:A30"/>
     <mergeCell ref="A31:A32"/>
@@ -1609,6 +1633,8 @@
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="A34:A36"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showDropDown="1" sqref="A34 A14"/>
@@ -1623,7 +1649,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1664,13 +1690,13 @@
     </row>
     <row r="3" spans="1:4" ht="56.25">
       <c r="A3" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>120</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>121</v>
       </c>
       <c r="D3" s="5">
         <v>45765</v>
@@ -1678,23 +1704,31 @@
     </row>
     <row r="4" spans="1:4" ht="37.5">
       <c r="A4" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>125</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>126</v>
       </c>
       <c r="D4" s="5">
         <v>45766</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18.75">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="7"/>
+    <row r="5" spans="1:4" ht="75">
+      <c r="A5" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="5">
+        <v>45773</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
v1.5 modify (SRS ID) Column according to naming convention
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_SRS.xlsx
+++ b/LH_REQUIREMENTS/LH_SRS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4080" windowHeight="6930"/>
   </bookViews>
   <sheets>
     <sheet name="LH_SRS" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="134">
   <si>
     <t>Feature</t>
   </si>
@@ -55,36 +55,21 @@
     <t>LH-CRS-REGISTRATION-001</t>
   </si>
   <si>
-    <t>SRS-REG-001</t>
-  </si>
-  <si>
     <t>LH-CRS-REGISTRATION-002</t>
   </si>
   <si>
-    <t>SRS-REG-002</t>
-  </si>
-  <si>
     <t>The system shall reject passwords shorter than 8 characters with an error message.</t>
   </si>
   <si>
     <t>LH-CRS-REGISTRATION-003</t>
   </si>
   <si>
-    <t>SRS-REG-003</t>
-  </si>
-  <si>
     <t>LH-CRS-REGISTRATION-004</t>
   </si>
   <si>
-    <t>SRS-REG-004</t>
-  </si>
-  <si>
     <t>LH-CRS-REGISTRATION-005</t>
   </si>
   <si>
-    <t>SRS-REG-005</t>
-  </si>
-  <si>
     <t>LH-CRS-REGISTRATION-006</t>
   </si>
   <si>
@@ -100,82 +85,49 @@
     <t>LH-CRS-PUBLISH-002</t>
   </si>
   <si>
-    <t>SRS-PUB-002</t>
-  </si>
-  <si>
     <t>LH-CRS-PUBLISH-003</t>
   </si>
   <si>
-    <t>SRS-PUB-003</t>
-  </si>
-  <si>
     <t>LH-CRS-PUBLISH-004</t>
   </si>
   <si>
-    <t>SRS-PUB-004</t>
-  </si>
-  <si>
     <t>LH-CRS-PUBLISH-005</t>
   </si>
   <si>
-    <t>SRS-PUB-005</t>
-  </si>
-  <si>
     <t>LH-CRS-PUBLISH-006</t>
   </si>
   <si>
-    <t>SRS-PUB-006</t>
-  </si>
-  <si>
     <t>Notifications</t>
   </si>
   <si>
     <t>LH-CRS-NOTIFICATIONS-001</t>
   </si>
   <si>
-    <t>SRS-NOT-001</t>
-  </si>
-  <si>
     <t>LH-CRS-NOTIFICATIONS-002</t>
   </si>
   <si>
-    <t>SRS-NOT-002</t>
-  </si>
-  <si>
     <t>Login</t>
   </si>
   <si>
     <t>LH-CRS-LOGIN-001</t>
   </si>
   <si>
-    <t>SRS-LOGIN-001</t>
-  </si>
-  <si>
     <t>The system shall provide a login form with email and password fields.</t>
   </si>
   <si>
     <t>LH-CRS-LOGIN-002</t>
   </si>
   <si>
-    <t>SRS-LOGIN-002</t>
-  </si>
-  <si>
     <t>The system shall verify user registration status before allowing login; reject unregistered emails.</t>
   </si>
   <si>
     <t>LH-CRS-LOGIN-003</t>
   </si>
   <si>
-    <t>SRS-LOGIN-003</t>
-  </si>
-  <si>
     <t>The system shall show a generic error: "Invalid credentials" for all login failures (no specifics).</t>
   </si>
   <si>
     <t>LH-CRS-LOGIN-004</t>
-  </si>
-  <si>
-    <t>SRS-LOGIN-004</t>
   </si>
   <si>
     <t>The system shall provide a registration form with fields for email, username, password and register button</t>
@@ -209,12 +161,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>SRS-REG-006.1</t>
-  </si>
-  <si>
-    <t>SRS-REG-006.2</t>
-  </si>
-  <si>
     <t>v1.1</t>
   </si>
   <si>
@@ -233,21 +179,9 @@
     <t>LH-CRS-ID-CONSTRAINS-001</t>
   </si>
   <si>
-    <t>SRS-ID-001</t>
-  </si>
-  <si>
     <t>User IDs shall be generated upon registration.</t>
   </si>
   <si>
-    <t>SRS-SYS-001</t>
-  </si>
-  <si>
-    <t>SRS-ADM-001</t>
-  </si>
-  <si>
-    <t>SRS-ADM-002</t>
-  </si>
-  <si>
     <t>admains can delete any user using its username or ID</t>
   </si>
   <si>
@@ -260,21 +194,12 @@
     <t>LH-CRS-NAVIGATION-001</t>
   </si>
   <si>
-    <t>SRS-NAV-001</t>
-  </si>
-  <si>
     <t>LH-CRS-NAVIGATION-002</t>
   </si>
   <si>
-    <t>SRS-NAV-002</t>
-  </si>
-  <si>
     <t>LH-CRS-NAVIGATION-003</t>
   </si>
   <si>
-    <t>SRS-NAV-003</t>
-  </si>
-  <si>
     <t>The system shall restrict content categories to exactly four (4) with no additions/deletions by users.</t>
   </si>
   <si>
@@ -287,45 +212,21 @@
     <t>LH-CRS-REGISTRATION-009</t>
   </si>
   <si>
-    <t>SRS-REG-007.1</t>
-  </si>
-  <si>
-    <t>SRS-REG-007.2</t>
-  </si>
-  <si>
     <t>The registration form shall require all mandatory fields (email, username, and password) to be filled out before submission</t>
   </si>
   <si>
     <t>The system shall display an error message if any mandatory field is left empty</t>
   </si>
   <si>
-    <t>SRS-REG-008</t>
-  </si>
-  <si>
     <t>The username shall adhere to the following constraints  (e.g., 4-20 characters,only contain letters and numbers  no special symbols like(!,@,#,$&lt;%,^,etc))</t>
   </si>
   <si>
     <t>The system shall prevent multiple registrations using the same email address. If a duplicate email is detected, an error message shall be displayed</t>
   </si>
   <si>
-    <t>SRS-REG-009.2</t>
-  </si>
-  <si>
-    <t>SRS-REG-009.1</t>
-  </si>
-  <si>
     <t>The system shall prevent multiple registrations using the same username. If a duplicate username is detected, an error message shall be displayed</t>
   </si>
   <si>
-    <t>SRS-ID-002.1</t>
-  </si>
-  <si>
-    <t>SRS-ID-002.2</t>
-  </si>
-  <si>
-    <t>SRS-ID-002.3</t>
-  </si>
-  <si>
     <t>The system shall automatically generate a unique user ID for each new registration in the format UXXX (ex:U001)</t>
   </si>
   <si>
@@ -338,24 +239,12 @@
     <t>Clicking the "Publish Article" button shall redirect the user to a form with fields for (Article title , Text body and publish button )</t>
   </si>
   <si>
-    <t>SRS-PUB-001.2</t>
-  </si>
-  <si>
-    <t>SRS-PUB-001.1</t>
-  </si>
-  <si>
     <t>Clicking the "Upload Video" button shall redirect the user to an interface supporting(Video title, add vedio and publish button)</t>
   </si>
   <si>
-    <t>SRS-PUB-001.3</t>
-  </si>
-  <si>
     <t>Clicking the "Record Audio" button shall open an embedded recorder with controls for(Start/stop recording and publish button)</t>
   </si>
   <si>
-    <t>SRS-PUB-001.4</t>
-  </si>
-  <si>
     <t>The system shall validate video file size before upload and reject files exceeding 100MB, with the message: "Max size: 100MB."</t>
   </si>
   <si>
@@ -420,9 +309,6 @@
   </si>
   <si>
     <t>modify SRS get comments on version 1.2 of SRS</t>
-  </si>
-  <si>
-    <t>SRS-ADM-003</t>
   </si>
   <si>
     <t>The system shall count words in articles in real-time and an error message  of "article body exceeds 1000 words"will be displayed and  prevent submission if the article exceeds 1000 words</t>
@@ -436,6 +322,129 @@
   </si>
   <si>
     <t>an error message of "user not found, please try a valid username or ID" must be shown when trying to delete not existing user</t>
+  </si>
+  <si>
+    <t>LH-SRS-REG-001</t>
+  </si>
+  <si>
+    <t>LH-SRS-REG-002</t>
+  </si>
+  <si>
+    <t>LH-SRS-REG-003</t>
+  </si>
+  <si>
+    <t>LH-SRS-REG-004</t>
+  </si>
+  <si>
+    <t>LH-SRS-REG-005</t>
+  </si>
+  <si>
+    <t>LH-SRS-REG-006.1</t>
+  </si>
+  <si>
+    <t>LH-SRS-REG-006.2</t>
+  </si>
+  <si>
+    <t>LH-SRS-REG-007.1</t>
+  </si>
+  <si>
+    <t>LH-SRS-REG-007.2</t>
+  </si>
+  <si>
+    <t>LH-SRS-REG-008</t>
+  </si>
+  <si>
+    <t>LH-SRS-REG-009.1</t>
+  </si>
+  <si>
+    <t>LH-SRS-REG-009.2</t>
+  </si>
+  <si>
+    <t>LH-SRS-ID-001</t>
+  </si>
+  <si>
+    <t>LH-SRS-ID-002.1</t>
+  </si>
+  <si>
+    <t>LH-SRS-ID-002.2</t>
+  </si>
+  <si>
+    <t>LH-SRS-ID-002.3</t>
+  </si>
+  <si>
+    <t>LH-SRS-LOGIN-001</t>
+  </si>
+  <si>
+    <t>LH-SRS-LOGIN-002</t>
+  </si>
+  <si>
+    <t>LH-SRS-LOGIN-003</t>
+  </si>
+  <si>
+    <t>LH-SRS-LOGIN-004</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUB-001.1</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUB-001.2</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUB-001.3</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUB-001.4</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUB-002</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUB-003</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUB-004</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUB-005</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUB-006</t>
+  </si>
+  <si>
+    <t>LH-SRS-NOT-001</t>
+  </si>
+  <si>
+    <t>LH-SRS-NOT-002</t>
+  </si>
+  <si>
+    <t>LH-SRS-SYS-001</t>
+  </si>
+  <si>
+    <t>LH-SRS-ADM-001</t>
+  </si>
+  <si>
+    <t>LH-SRS-ADM-002</t>
+  </si>
+  <si>
+    <t>LH-SRS-ADM-003</t>
+  </si>
+  <si>
+    <t>LH-SRS-NAV-001</t>
+  </si>
+  <si>
+    <t>LH-SRS-NAV-002</t>
+  </si>
+  <si>
+    <t>LH-SRS-NAV-003</t>
+  </si>
+  <si>
+    <t>v1.5</t>
+  </si>
+  <si>
+    <t>Hala Eldaly</t>
+  </si>
+  <si>
+    <t>modify (SRS ID) Column according to naming convention</t>
   </si>
 </sst>
 </file>
@@ -1010,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1034,7 +1043,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>1</v>
@@ -1048,10 +1057,10 @@
         <v>10</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>8</v>
@@ -1060,13 +1069,13 @@
     <row r="3" spans="1:5" ht="30">
       <c r="A3" s="34"/>
       <c r="B3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>14</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>8</v>
@@ -1075,13 +1084,13 @@
     <row r="4" spans="1:5" ht="45">
       <c r="A4" s="34"/>
       <c r="B4" s="20" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>16</v>
+        <v>95</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>8</v>
@@ -1090,13 +1099,13 @@
     <row r="5" spans="1:5" ht="45">
       <c r="A5" s="34"/>
       <c r="B5" s="15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>18</v>
+        <v>96</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>121</v>
+        <v>84</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>8</v>
@@ -1105,13 +1114,13 @@
     <row r="6" spans="1:5" ht="60">
       <c r="A6" s="34"/>
       <c r="B6" s="20" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>20</v>
+        <v>97</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>108</v>
+        <v>71</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>8</v>
@@ -1120,13 +1129,13 @@
     <row r="7" spans="1:5" ht="30">
       <c r="A7" s="34"/>
       <c r="B7" s="29" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>8</v>
@@ -1136,10 +1145,10 @@
       <c r="A8" s="34"/>
       <c r="B8" s="29"/>
       <c r="C8" s="9" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>109</v>
+        <v>72</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>8</v>
@@ -1148,13 +1157,13 @@
     <row r="9" spans="1:5" ht="45">
       <c r="A9" s="34"/>
       <c r="B9" s="31" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>8</v>
@@ -1164,10 +1173,10 @@
       <c r="A10" s="34"/>
       <c r="B10" s="32"/>
       <c r="C10" s="9" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>8</v>
@@ -1176,13 +1185,13 @@
     <row r="11" spans="1:5" ht="45">
       <c r="A11" s="34"/>
       <c r="B11" s="24" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>8</v>
@@ -1191,13 +1200,13 @@
     <row r="12" spans="1:5" ht="45">
       <c r="A12" s="34"/>
       <c r="B12" s="31" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>8</v>
@@ -1207,10 +1216,10 @@
       <c r="A13" s="35"/>
       <c r="B13" s="32"/>
       <c r="C13" s="9" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>8</v>
@@ -1218,16 +1227,16 @@
     </row>
     <row r="14" spans="1:5" s="12" customFormat="1" ht="15.75">
       <c r="A14" s="25" t="s">
-        <v>117</v>
+        <v>80</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>8</v>
@@ -1236,13 +1245,13 @@
     <row r="15" spans="1:5" s="12" customFormat="1" ht="45">
       <c r="A15" s="26"/>
       <c r="B15" s="36" t="s">
-        <v>118</v>
+        <v>81</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>8</v>
@@ -1252,10 +1261,10 @@
       <c r="A16" s="26"/>
       <c r="B16" s="37"/>
       <c r="C16" s="10" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>8</v>
@@ -1265,10 +1274,10 @@
       <c r="A17" s="27"/>
       <c r="B17" s="38"/>
       <c r="C17" s="9" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>8</v>
@@ -1276,16 +1285,16 @@
     </row>
     <row r="18" spans="1:5" ht="30">
       <c r="A18" s="28" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>42</v>
+        <v>109</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>8</v>
@@ -1294,13 +1303,13 @@
     <row r="19" spans="1:5" ht="30">
       <c r="A19" s="28"/>
       <c r="B19" s="20" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>45</v>
+        <v>110</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>8</v>
@@ -1309,13 +1318,13 @@
     <row r="20" spans="1:5" ht="30">
       <c r="A20" s="28"/>
       <c r="B20" s="15" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>48</v>
+        <v>111</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="E20" s="10" t="s">
         <v>8</v>
@@ -1324,13 +1333,13 @@
     <row r="21" spans="1:5" ht="15.75">
       <c r="A21" s="28"/>
       <c r="B21" s="20" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>51</v>
+        <v>112</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>8</v>
@@ -1338,16 +1347,16 @@
     </row>
     <row r="22" spans="1:5" ht="30" customHeight="1">
       <c r="A22" s="30" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B22" s="39" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>8</v>
@@ -1357,10 +1366,10 @@
       <c r="A23" s="30"/>
       <c r="B23" s="40"/>
       <c r="C23" s="11" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
       <c r="E23" s="11" t="s">
         <v>8</v>
@@ -1370,10 +1379,10 @@
       <c r="A24" s="30"/>
       <c r="B24" s="40"/>
       <c r="C24" s="10" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="E24" s="10" t="s">
         <v>8</v>
@@ -1383,10 +1392,10 @@
       <c r="A25" s="30"/>
       <c r="B25" s="41"/>
       <c r="C25" s="11" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>8</v>
@@ -1395,13 +1404,13 @@
     <row r="26" spans="1:5" ht="45">
       <c r="A26" s="30"/>
       <c r="B26" s="20" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>26</v>
+        <v>117</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>104</v>
+        <v>67</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>8</v>
@@ -1410,13 +1419,13 @@
     <row r="27" spans="1:5" ht="45">
       <c r="A27" s="30"/>
       <c r="B27" s="15" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>28</v>
+        <v>118</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>105</v>
+        <v>68</v>
       </c>
       <c r="E27" s="10" t="s">
         <v>8</v>
@@ -1425,13 +1434,13 @@
     <row r="28" spans="1:5" ht="60">
       <c r="A28" s="30"/>
       <c r="B28" s="20" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>30</v>
+        <v>119</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>127</v>
+        <v>89</v>
       </c>
       <c r="E28" s="9" t="s">
         <v>8</v>
@@ -1440,13 +1449,13 @@
     <row r="29" spans="1:5" ht="45">
       <c r="A29" s="30"/>
       <c r="B29" s="15" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>32</v>
+        <v>120</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>106</v>
+        <v>69</v>
       </c>
       <c r="E29" s="10" t="s">
         <v>8</v>
@@ -1455,13 +1464,13 @@
     <row r="30" spans="1:5" ht="45">
       <c r="A30" s="30"/>
       <c r="B30" s="20" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>34</v>
+        <v>121</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="E30" s="9" t="s">
         <v>8</v>
@@ -1469,16 +1478,16 @@
     </row>
     <row r="31" spans="1:5" ht="30">
       <c r="A31" s="28" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>37</v>
+        <v>122</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="E31" s="10" t="s">
         <v>8</v>
@@ -1487,13 +1496,13 @@
     <row r="32" spans="1:5" ht="30">
       <c r="A32" s="28"/>
       <c r="B32" s="20" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>39</v>
+        <v>123</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="E32" s="9" t="s">
         <v>8</v>
@@ -1501,16 +1510,16 @@
     </row>
     <row r="33" spans="1:7" ht="31.5">
       <c r="A33" s="16" t="s">
-        <v>116</v>
+        <v>79</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>114</v>
+        <v>77</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>110</v>
+        <v>73</v>
       </c>
       <c r="E33" s="10" t="s">
         <v>8</v>
@@ -1520,16 +1529,16 @@
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1">
       <c r="A34" s="33" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>66</v>
+        <v>125</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="E34" s="9" t="s">
         <v>8</v>
@@ -1540,13 +1549,13 @@
     <row r="35" spans="1:7" ht="15" customHeight="1">
       <c r="A35" s="34"/>
       <c r="B35" s="39" t="s">
-        <v>115</v>
+        <v>78</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>67</v>
+        <v>126</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="E35" s="10" t="s">
         <v>8</v>
@@ -1558,10 +1567,10 @@
       <c r="A36" s="35"/>
       <c r="B36" s="41"/>
       <c r="C36" s="10" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>130</v>
+        <v>92</v>
       </c>
       <c r="E36" s="10" t="s">
         <v>8</v>
@@ -1571,16 +1580,16 @@
     </row>
     <row r="37" spans="1:7" ht="45">
       <c r="A37" s="25" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>72</v>
+        <v>128</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>123</v>
+        <v>86</v>
       </c>
       <c r="E37" s="9" t="s">
         <v>8</v>
@@ -1589,13 +1598,13 @@
     <row r="38" spans="1:7" ht="30">
       <c r="A38" s="26"/>
       <c r="B38" s="23" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>74</v>
+        <v>129</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>122</v>
+        <v>85</v>
       </c>
       <c r="E38" s="10" t="s">
         <v>8</v>
@@ -1604,13 +1613,13 @@
     <row r="39" spans="1:7" ht="30">
       <c r="A39" s="27"/>
       <c r="B39" s="19" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>76</v>
+        <v>130</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="E39" s="9" t="s">
         <v>8</v>
@@ -1646,10 +1655,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1676,13 +1685,13 @@
     </row>
     <row r="2" spans="1:4" ht="56.25">
       <c r="A2" s="3" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="D2" s="5">
         <v>45760</v>
@@ -1690,13 +1699,13 @@
     </row>
     <row r="3" spans="1:4" ht="56.25">
       <c r="A3" s="3" t="s">
-        <v>119</v>
+        <v>82</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>120</v>
+        <v>83</v>
       </c>
       <c r="D3" s="5">
         <v>45765</v>
@@ -1704,13 +1713,13 @@
     </row>
     <row r="4" spans="1:4" ht="37.5">
       <c r="A4" s="3" t="s">
-        <v>124</v>
+        <v>87</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>125</v>
+        <v>88</v>
       </c>
       <c r="D4" s="5">
         <v>45766</v>
@@ -1718,15 +1727,29 @@
     </row>
     <row r="5" spans="1:4" ht="75">
       <c r="A5" s="3" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>129</v>
+        <v>91</v>
       </c>
       <c r="D5" s="5">
+        <v>45773</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="37.5">
+      <c r="A6" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D6" s="5">
         <v>45773</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v2.0 adjusted login SRS based on CRS
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_SRS.xlsx
+++ b/LH_REQUIREMENTS/LH_SRS.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4C2ED2-5B78-40A7-9DC6-9649A1F328CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4080" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LH_SRS" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="148">
   <si>
     <t>Feature</t>
   </si>
@@ -112,22 +113,10 @@
     <t>LH-CRS-LOGIN-001</t>
   </si>
   <si>
-    <t>The system shall provide a login form with email and password fields.</t>
-  </si>
-  <si>
     <t>LH-CRS-LOGIN-002</t>
   </si>
   <si>
-    <t>The system shall verify user registration status before allowing login; reject unregistered emails.</t>
-  </si>
-  <si>
     <t>LH-CRS-LOGIN-003</t>
-  </si>
-  <si>
-    <t>The system shall show a generic error: "Invalid credentials" for all login failures (no specifics).</t>
-  </si>
-  <si>
-    <t>LH-CRS-LOGIN-004</t>
   </si>
   <si>
     <t>The system shall provide a registration form with fields for email, username, password and register button</t>
@@ -173,9 +162,6 @@
     <t>The system shall display unread notifications in a bell icon dropdown.</t>
   </si>
   <si>
-    <t>The system shall hash passwords</t>
-  </si>
-  <si>
     <t>LH-CRS-ID-CONSTRAINS-001</t>
   </si>
   <si>
@@ -445,12 +431,69 @@
   </si>
   <si>
     <t>modify (SRS ID) Column according to naming convention</t>
+  </si>
+  <si>
+    <t>The system shall allow users to log in using a valid email address and password combination.</t>
+  </si>
+  <si>
+    <t>Gehad Ashry</t>
+  </si>
+  <si>
+    <t>The system shall verify user registration status before allowing login; The email address must follow the format username@domain.com.</t>
+  </si>
+  <si>
+    <t>The password must match the one provided during user registration.</t>
+  </si>
+  <si>
+    <t>LH-SRS-LOGIN-005</t>
+  </si>
+  <si>
+    <t>The system shall verify that login credentials match a registered user present in the user database.</t>
+  </si>
+  <si>
+    <t>Only users with an active registration are permitted to access the system.</t>
+  </si>
+  <si>
+    <t>LH-SRS-LOGIN-006</t>
+  </si>
+  <si>
+    <t>In case of a failed login attempt, the system shall display a generic error message : "Invalid credentials" for all login failures (no specifics).</t>
+  </si>
+  <si>
+    <t>The system shall not disclose whether the error is due to an incorrect email, incorrect password, or missing inputs.</t>
+  </si>
+  <si>
+    <t>LH-SRS-LOGIN-007</t>
+  </si>
+  <si>
+    <t>The system shall store user passwords in a hashed format to prevent plain-text storage.</t>
+  </si>
+  <si>
+    <t>LH-SRS-LOGIN-008</t>
+  </si>
+  <si>
+    <t>A simple salting mechanism shall be applied to each password before hashing to increase uniqueness.</t>
+  </si>
+  <si>
+    <t>LH-SRS-LOGIN-009</t>
+  </si>
+  <si>
+    <t>The system shall not store raw (plain-text) passwords at any stage.</t>
+  </si>
+  <si>
+    <t>LH-SRS-LOGIN-010</t>
+  </si>
+  <si>
+    <t>v2.0</t>
+  </si>
+  <si>
+    <t>Adjusted the Login SRS to match CRS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -616,7 +659,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -656,35 +699,47 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -695,46 +750,22 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1016,18 +1047,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" style="22" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" style="22" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" style="21" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" style="21" customWidth="1"/>
     <col min="4" max="4" width="53.42578125" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1043,610 +1074,689 @@
         <v>3</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30">
-      <c r="A2" s="33" t="s">
+    <row r="2" spans="1:5" ht="47.25">
+      <c r="A2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="31.5">
+      <c r="A3" s="27"/>
+      <c r="B3" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="47.25">
+      <c r="A4" s="27"/>
+      <c r="B4" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="47.25">
+      <c r="A5" s="27"/>
+      <c r="B5" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="63">
+      <c r="A6" s="27"/>
+      <c r="B6" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="31.5">
+      <c r="A7" s="27"/>
+      <c r="B7" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30">
-      <c r="A3" s="34"/>
-      <c r="B3" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="10" t="s">
+      <c r="D7" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="47.25">
+      <c r="A8" s="27"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="45">
-      <c r="A4" s="34"/>
-      <c r="B4" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="9" t="s">
+      <c r="D8" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="47.25">
+      <c r="A9" s="27"/>
+      <c r="B9" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D9" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="31.5">
+      <c r="A10" s="27"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="63">
+      <c r="A11" s="27"/>
+      <c r="B11" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="47.25">
+      <c r="A12" s="27"/>
+      <c r="B12" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="47.25">
+      <c r="A13" s="28"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="12" customFormat="1" ht="23.25" customHeight="1">
+      <c r="A14" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45">
-      <c r="A5" s="34"/>
-      <c r="B5" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="E14" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="12" customFormat="1" ht="45">
+      <c r="A15" s="30"/>
+      <c r="B15" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="12" customFormat="1" ht="30">
+      <c r="A16" s="30"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="12" customFormat="1" ht="30">
+      <c r="A17" s="31"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30">
+      <c r="A18" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="45">
+      <c r="A19" s="27"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="28.5" customHeight="1">
+      <c r="A20" s="27"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30">
+      <c r="A21" s="27"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30">
+      <c r="A22" s="27"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="45">
+      <c r="A23" s="27"/>
+      <c r="B23" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="45">
+      <c r="A24" s="27"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30">
+      <c r="A25" s="27"/>
+      <c r="B25" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30">
+      <c r="A26" s="27"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="30">
+      <c r="A27" s="28"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" customHeight="1">
+      <c r="A28" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="45">
+      <c r="A29" s="33"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="45">
+      <c r="A30" s="33"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="45">
+      <c r="A31" s="33"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="45">
+      <c r="A32" s="33"/>
+      <c r="B32" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="45">
+      <c r="A33" s="33"/>
+      <c r="B33" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="60">
+      <c r="A34" s="33"/>
+      <c r="B34" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D34" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="60">
-      <c r="A6" s="34"/>
-      <c r="B6" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D6" s="9" t="s">
+      <c r="E34" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="45">
+      <c r="A35" s="33"/>
+      <c r="B35" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="45">
+      <c r="A36" s="34"/>
+      <c r="B36" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="30">
+      <c r="A37" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="30">
+      <c r="A38" s="28"/>
+      <c r="B38" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="31.5">
+      <c r="A39" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+    </row>
+    <row r="40" spans="1:7" ht="30" customHeight="1">
+      <c r="A40" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="30">
-      <c r="A7" s="34"/>
-      <c r="B7" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="45">
-      <c r="A8" s="34"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45">
-      <c r="A9" s="34"/>
-      <c r="B9" s="31" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30">
-      <c r="A10" s="34"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="45">
-      <c r="A11" s="34"/>
-      <c r="B11" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="45">
-      <c r="A12" s="34"/>
-      <c r="B12" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="45">
-      <c r="A13" s="35"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="12" customFormat="1" ht="15.75">
-      <c r="A14" s="25" t="s">
+      <c r="C40" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+    </row>
+    <row r="41" spans="1:7" ht="15" customHeight="1">
+      <c r="A41" s="27"/>
+      <c r="B41" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+    </row>
+    <row r="42" spans="1:7" ht="15" customHeight="1">
+      <c r="A42" s="28"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+    </row>
+    <row r="43" spans="1:7" ht="45">
+      <c r="A43" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="30">
+      <c r="A44" s="30"/>
+      <c r="B44" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D44" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B14" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="12" customFormat="1" ht="45">
-      <c r="A15" s="26"/>
-      <c r="B15" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="12" customFormat="1" ht="30">
-      <c r="A16" s="26"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="12" customFormat="1" ht="30">
-      <c r="A17" s="27"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30">
-      <c r="A18" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="30">
-      <c r="A19" s="28"/>
-      <c r="B19" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30">
-      <c r="A20" s="28"/>
-      <c r="B20" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75">
-      <c r="A21" s="28"/>
-      <c r="B21" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="30" customHeight="1">
-      <c r="A22" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="45">
-      <c r="A23" s="30"/>
-      <c r="B23" s="40"/>
-      <c r="C23" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="45">
-      <c r="A24" s="30"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="45">
-      <c r="A25" s="30"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="45">
-      <c r="A26" s="30"/>
-      <c r="B26" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="45">
-      <c r="A27" s="30"/>
-      <c r="B27" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="60">
-      <c r="A28" s="30"/>
-      <c r="B28" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="45">
-      <c r="A29" s="30"/>
-      <c r="B29" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="45">
-      <c r="A30" s="30"/>
-      <c r="B30" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="30">
-      <c r="A31" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="30">
-      <c r="A32" s="28"/>
-      <c r="B32" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="31.5">
-      <c r="A33" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-    </row>
-    <row r="34" spans="1:7" ht="30" customHeight="1">
-      <c r="A34" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="B34" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" s="9" t="s">
+      <c r="E44" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="30">
+      <c r="A45" s="31"/>
+      <c r="B45" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="D34" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-    </row>
-    <row r="35" spans="1:7" ht="15" customHeight="1">
-      <c r="A35" s="34"/>
-      <c r="B35" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-    </row>
-    <row r="36" spans="1:7" ht="15" customHeight="1">
-      <c r="A36" s="35"/>
-      <c r="B36" s="41"/>
-      <c r="C36" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-    </row>
-    <row r="37" spans="1:7" ht="45">
-      <c r="A37" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="B37" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="30">
-      <c r="A38" s="26"/>
-      <c r="B38" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="30">
-      <c r="A39" s="27"/>
-      <c r="B39" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="17"/>
-      <c r="B40" s="21"/>
+      <c r="D45" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="16"/>
+      <c r="B46" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="A18:A21"/>
+  <mergeCells count="16">
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="A18:A27"/>
+    <mergeCell ref="A43:A45"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A22:A30"/>
-    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A28:A36"/>
+    <mergeCell ref="A37:A38"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="B18:B22"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A34 A14"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A40 A14" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1654,11 +1764,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1685,13 +1795,13 @@
     </row>
     <row r="2" spans="1:4" ht="56.25">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D2" s="5">
         <v>45760</v>
@@ -1699,13 +1809,13 @@
     </row>
     <row r="3" spans="1:4" ht="56.25">
       <c r="A3" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D3" s="5">
         <v>45765</v>
@@ -1713,13 +1823,13 @@
     </row>
     <row r="4" spans="1:4" ht="37.5">
       <c r="A4" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D4" s="5">
         <v>45766</v>
@@ -1727,13 +1837,13 @@
     </row>
     <row r="5" spans="1:4" ht="75">
       <c r="A5" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D5" s="5">
         <v>45773</v>
@@ -1741,16 +1851,30 @@
     </row>
     <row r="6" spans="1:4" ht="37.5">
       <c r="A6" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D6" s="5">
         <v>45773</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="37.5">
+      <c r="A7" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="5">
+        <v>45780</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v2.5 Adjusted Publish Audio after review comments
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_SRS.xlsx
+++ b/LH_REQUIREMENTS/LH_SRS.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568C8723-A1B1-46CF-B949-072B6C7FD444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LH_SRS" sheetId="1" r:id="rId1"/>
@@ -219,12 +218,6 @@
     <t>LH-SRS-LOGIN-004</t>
   </si>
   <si>
-    <t>LH-SRS-NOT-001</t>
-  </si>
-  <si>
-    <t>LH-SRS-NOT-002</t>
-  </si>
-  <si>
     <t>LH-SRS-SYS-001</t>
   </si>
   <si>
@@ -547,13 +540,7 @@
     <t>LH-SRS-PUBLISHAUDIO-006</t>
   </si>
   <si>
-    <t>The system display an error message "Recording exceeds 5 minutes". if the recording exceeds 5 minutes and automatically stop the recording.</t>
-  </si>
-  <si>
     <t>LH-SRS-PUBLISHAUDIO-007</t>
-  </si>
-  <si>
-    <t>The system display the error message in a visible and non-dismissible format until recording stops.</t>
   </si>
   <si>
     <t>LH-SRS-PUBLISHAUDIO-008</t>
@@ -820,12 +807,24 @@
   <si>
     <t>Categories</t>
   </si>
+  <si>
+    <t>The system display the error message in a visible and non-dismissible format</t>
+  </si>
+  <si>
+    <t>The system display an error message "Recording exceeds 5 minutes". if the recording exceeds 5 minutes.</t>
+  </si>
+  <si>
+    <t>v2.5</t>
+  </si>
+  <si>
+    <t>Adjusted the Publish Audio after get comments</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -959,7 +958,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1019,31 +1018,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1111,64 +1090,61 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1450,24 +1426,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A72" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" style="13" customWidth="1"/>
-    <col min="3" max="3" width="26.44140625" style="13" customWidth="1"/>
-    <col min="4" max="4" width="53.44140625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="13"/>
+    <col min="1" max="1" width="19.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" style="13" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="53.42578125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="19.5">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1484,8 +1460,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="34" t="s">
+    <row r="2" spans="1:5" ht="30">
+      <c r="A2" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="11" t="s">
@@ -1495,14 +1471,14 @@
         <v>51</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="35"/>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30">
+      <c r="A3" s="27"/>
       <c r="B3" s="11" t="s">
         <v>11</v>
       </c>
@@ -1510,14 +1486,14 @@
         <v>52</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="35"/>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30">
+      <c r="A4" s="27"/>
       <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
@@ -1525,14 +1501,14 @@
         <v>53</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="35"/>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="27"/>
       <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
@@ -1540,14 +1516,14 @@
         <v>54</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="35"/>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30">
+      <c r="A6" s="27"/>
       <c r="B6" s="11" t="s">
         <v>14</v>
       </c>
@@ -1555,44 +1531,44 @@
         <v>55</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="35"/>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="27"/>
       <c r="B7" s="17" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="35"/>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="27"/>
       <c r="B8" s="17" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="35"/>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30">
+      <c r="A9" s="27"/>
       <c r="B9" s="11" t="s">
         <v>31</v>
       </c>
@@ -1600,29 +1576,29 @@
         <v>56</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="35"/>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="27"/>
       <c r="B10" s="17" t="s">
         <v>32</v>
       </c>
       <c r="C10" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>216</v>
-      </c>
       <c r="E10" s="11" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="37" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="23.25" customHeight="1">
+      <c r="A11" s="23" t="s">
         <v>41</v>
       </c>
       <c r="B11" s="10" t="s">
@@ -1638,9 +1614,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="39"/>
-      <c r="B12" s="24" t="s">
+    <row r="12" spans="1:5" ht="30">
+      <c r="A12" s="24"/>
+      <c r="B12" s="28" t="s">
         <v>42</v>
       </c>
       <c r="C12" s="10" t="s">
@@ -1653,9 +1629,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="39"/>
-      <c r="B13" s="25"/>
+    <row r="13" spans="1:5" ht="30">
+      <c r="A13" s="24"/>
+      <c r="B13" s="29"/>
       <c r="C13" s="10" t="s">
         <v>59</v>
       </c>
@@ -1666,9 +1642,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="38"/>
-      <c r="B14" s="26"/>
+    <row r="14" spans="1:5" ht="30">
+      <c r="A14" s="25"/>
+      <c r="B14" s="30"/>
       <c r="C14" s="10" t="s">
         <v>60</v>
       </c>
@@ -1679,8 +1655,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="34" t="s">
+    <row r="15" spans="1:5" ht="30">
+      <c r="A15" s="26" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="31" t="s">
@@ -1690,286 +1666,286 @@
         <v>61</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="35"/>
-      <c r="B16" s="33"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="45">
+      <c r="A16" s="27"/>
+      <c r="B16" s="32"/>
       <c r="C16" s="11" t="s">
         <v>62</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="35"/>
-      <c r="B17" s="33"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="28.5" customHeight="1">
+      <c r="A17" s="27"/>
+      <c r="B17" s="32"/>
       <c r="C17" s="11" t="s">
         <v>63</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="35"/>
-      <c r="B18" s="33"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30">
+      <c r="A18" s="27"/>
+      <c r="B18" s="32"/>
       <c r="C18" s="11" t="s">
         <v>64</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="35"/>
-      <c r="B19" s="32"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30">
+      <c r="A19" s="27"/>
+      <c r="B19" s="33"/>
       <c r="C19" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>80</v>
-      </c>
       <c r="E19" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="35"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="45">
+      <c r="A20" s="27"/>
       <c r="B20" s="31" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30">
+      <c r="A21" s="27"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="D20" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="35"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>83</v>
-      </c>
       <c r="E21" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="35"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30">
+      <c r="A22" s="27"/>
       <c r="B22" s="31" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30">
+      <c r="A23" s="27"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D23" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E22" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="35"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="11" t="s">
+      <c r="E23" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30">
+      <c r="A24" s="36"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D24" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="E23" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="36"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>89</v>
-      </c>
       <c r="E24" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="37" t="s">
-        <v>249</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30">
+      <c r="A25" s="23" t="s">
+        <v>245</v>
       </c>
       <c r="B25" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30">
+      <c r="A26" s="24"/>
+      <c r="B26" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="24"/>
+      <c r="B27" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30">
+      <c r="A28" s="24"/>
+      <c r="B28" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="D28" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="30">
+      <c r="A29" s="24"/>
+      <c r="B29" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D29" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30">
+      <c r="A30" s="24"/>
+      <c r="B30" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="D30" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="E25" s="10" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="39"/>
-      <c r="B26" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="39"/>
-      <c r="B27" s="10" t="s">
+      <c r="E30" s="10" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="30">
+      <c r="A31" s="24"/>
+      <c r="B31" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C31" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D31" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="E27" s="10" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="39"/>
-      <c r="B28" s="10" t="s">
+      <c r="E31" s="10" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30">
+      <c r="A32" s="24"/>
+      <c r="B32" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C32" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D32" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="E28" s="10" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="39"/>
-      <c r="B29" s="10" t="s">
+      <c r="E32" s="10" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="30">
+      <c r="A33" s="24"/>
+      <c r="B33" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C33" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D33" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="E29" s="10" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="39"/>
-      <c r="B30" s="10" t="s">
+      <c r="E33" s="10" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="30">
+      <c r="A34" s="25"/>
+      <c r="B34" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C34" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D34" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="E30" s="10" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="39"/>
-      <c r="B31" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="39"/>
-      <c r="B32" s="10" t="s">
-        <v>223</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>234</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="39"/>
-      <c r="B33" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="38"/>
-      <c r="B34" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>245</v>
-      </c>
       <c r="E34" s="10" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="30">
       <c r="A35" s="14" t="s">
         <v>40</v>
       </c>
@@ -1977,7 +1953,7 @@
         <v>39</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D35" s="11" t="s">
         <v>37</v>
@@ -1988,118 +1964,118 @@
       <c r="F35" s="15"/>
       <c r="G35" s="15"/>
     </row>
-    <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="37" t="s">
+    <row r="36" spans="1:7" ht="30" customHeight="1">
+      <c r="A36" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="23" t="s">
+      <c r="B36" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="30" customHeight="1">
+      <c r="A37" s="24"/>
+      <c r="B37" s="40"/>
+      <c r="C37" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="D37" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="C36" s="19" t="s">
+      <c r="E37" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="30" customHeight="1">
+      <c r="A38" s="24"/>
+      <c r="B38" s="40" t="s">
         <v>184</v>
       </c>
-      <c r="D36" s="21" t="s">
+      <c r="C38" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="E36" s="19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="39"/>
-      <c r="B37" s="23"/>
-      <c r="C37" s="19" t="s">
+      <c r="D38" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="D37" s="19" t="s">
+      <c r="E38" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="30" customHeight="1">
+      <c r="A39" s="24"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="19" t="s">
         <v>187</v>
       </c>
-      <c r="E37" s="19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="39"/>
-      <c r="B38" s="23" t="s">
+      <c r="D39" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="C38" s="19" t="s">
+      <c r="E39" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="30" customHeight="1">
+      <c r="A40" s="24"/>
+      <c r="B40" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="D38" s="21" t="s">
+      <c r="C40" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="E38" s="19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="39"/>
-      <c r="B39" s="23"/>
-      <c r="C39" s="19" t="s">
+      <c r="D40" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="D39" s="19" t="s">
+      <c r="E40" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="30" customHeight="1">
+      <c r="A41" s="24"/>
+      <c r="B41" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="E39" s="19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="39"/>
-      <c r="B40" s="22" t="s">
+      <c r="C41" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="C40" s="19" t="s">
+      <c r="D41" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="D40" s="21" t="s">
+      <c r="E41" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="15" customHeight="1">
+      <c r="A42" s="24"/>
+      <c r="B42" s="22" t="s">
         <v>195</v>
       </c>
-      <c r="E40" s="19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="39"/>
-      <c r="B41" s="22" t="s">
+      <c r="C42" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="D42" s="21" t="s">
         <v>197</v>
       </c>
-      <c r="D41" s="19" t="s">
-        <v>198</v>
-      </c>
-      <c r="E41" s="19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="39"/>
-      <c r="B42" s="22" t="s">
-        <v>199</v>
-      </c>
-      <c r="C42" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="D42" s="21" t="s">
-        <v>201</v>
-      </c>
       <c r="E42" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A43" s="34" t="s">
+    <row r="43" spans="1:7" ht="45">
+      <c r="A43" s="26" t="s">
         <v>25</v>
       </c>
       <c r="B43" s="11" t="s">
         <v>26</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D43" s="11" t="s">
         <v>46</v>
@@ -2108,13 +2084,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="35"/>
+    <row r="44" spans="1:7" ht="30">
+      <c r="A44" s="27"/>
       <c r="B44" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D44" s="11" t="s">
         <v>45</v>
@@ -2123,13 +2099,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="35"/>
+    <row r="45" spans="1:7" ht="30">
+      <c r="A45" s="27"/>
       <c r="B45" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D45" s="11" t="s">
         <v>29</v>
@@ -2138,502 +2114,502 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="37" t="s">
+    <row r="46" spans="1:7" ht="30">
+      <c r="A46" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="30">
+      <c r="A47" s="24"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="30">
+      <c r="A48" s="24"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="30">
+      <c r="A49" s="24"/>
+      <c r="B49" s="30"/>
+      <c r="C49" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="30">
+      <c r="A50" s="24"/>
+      <c r="B50" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="30">
+      <c r="A51" s="24"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="45">
+      <c r="A52" s="24"/>
+      <c r="B52" s="29"/>
+      <c r="C52" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="45">
+      <c r="A53" s="24"/>
+      <c r="B53" s="30"/>
+      <c r="C53" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="45">
+      <c r="A54" s="24"/>
+      <c r="B54" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="45">
+      <c r="A55" s="24"/>
+      <c r="B55" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="30">
+      <c r="A56" s="24"/>
+      <c r="B56" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="45">
+      <c r="A57" s="25"/>
+      <c r="B57" s="30"/>
+      <c r="C57" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="30">
+      <c r="A58" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="B58" s="37" t="s">
+        <v>157</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="E58" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="33">
+      <c r="A59" s="27"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="D59" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="E59" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="30">
+      <c r="A60" s="27"/>
+      <c r="B60" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="C60" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="E60" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="33">
+      <c r="A61" s="27"/>
+      <c r="B61" s="38"/>
+      <c r="C61" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="D61" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="E61" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="30">
+      <c r="A62" s="27"/>
+      <c r="B62" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="D62" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="E62" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="49.5">
+      <c r="A63" s="27"/>
+      <c r="B63" s="39"/>
+      <c r="C63" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="D63" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="E63" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="30">
+      <c r="A64" s="27"/>
+      <c r="B64" s="39"/>
+      <c r="C64" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="D64" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="E64" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="33">
+      <c r="A65" s="27"/>
+      <c r="B65" s="38"/>
+      <c r="C65" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="D65" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="E65" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="30">
+      <c r="A66" s="27"/>
+      <c r="B66" s="37" t="s">
+        <v>174</v>
+      </c>
+      <c r="C66" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="D66" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="E66" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="49.5">
+      <c r="A67" s="27"/>
+      <c r="B67" s="38"/>
+      <c r="C67" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="D67" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="E67" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="30">
+      <c r="A68" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="B46" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="D46" s="10" t="s">
+      <c r="B68" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="C68" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="D68" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="E68" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="30">
+      <c r="A69" s="41"/>
+      <c r="B69" s="29"/>
+      <c r="C69" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="D69" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="E46" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A47" s="39"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="D47" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A48" s="39"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A49" s="39"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="E49" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="39"/>
-      <c r="B50" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="D50" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A51" s="39"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="D51" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="E51" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A52" s="39"/>
-      <c r="B52" s="25"/>
-      <c r="C52" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="E52" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A53" s="39"/>
-      <c r="B53" s="26"/>
-      <c r="C53" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="D53" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="E53" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A54" s="39"/>
-      <c r="B54" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="E54" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A55" s="39"/>
-      <c r="B55" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="C55" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="D55" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="E55" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A56" s="39"/>
-      <c r="B56" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="C56" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="D56" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="E56" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A57" s="38"/>
-      <c r="B57" s="26"/>
-      <c r="C57" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="D57" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="E57" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="B58" s="40" t="s">
-        <v>159</v>
-      </c>
-      <c r="C58" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="D58" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="E58" s="18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="35"/>
-      <c r="B59" s="41"/>
-      <c r="C59" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="D59" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="E59" s="18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="35"/>
-      <c r="B60" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="C60" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="D60" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="E60" s="18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="35"/>
-      <c r="B61" s="41"/>
-      <c r="C61" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="D61" s="20" t="s">
-        <v>168</v>
-      </c>
-      <c r="E61" s="18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A62" s="35"/>
-      <c r="B62" s="40" t="s">
-        <v>169</v>
-      </c>
-      <c r="C62" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="D62" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="E62" s="18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="A63" s="35"/>
-      <c r="B63" s="42"/>
-      <c r="C63" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="D63" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="E63" s="18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A64" s="35"/>
-      <c r="B64" s="42"/>
-      <c r="C64" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="D64" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="E64" s="18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="35"/>
-      <c r="B65" s="41"/>
-      <c r="C65" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="D65" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="E65" s="18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A66" s="35"/>
-      <c r="B66" s="40" t="s">
-        <v>178</v>
-      </c>
-      <c r="C66" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="D66" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="E66" s="18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="A67" s="35"/>
-      <c r="B67" s="41"/>
-      <c r="C67" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="D67" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="E67" s="18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A68" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="B68" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="C68" s="16" t="s">
+      <c r="E69" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="30">
+      <c r="A70" s="41"/>
+      <c r="B70" s="29"/>
+      <c r="C70" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="D68" s="10" t="s">
+      <c r="D70" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="E70" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="30">
+      <c r="A71" s="41"/>
+      <c r="B71" s="29"/>
+      <c r="C71" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="D71" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="E68" s="10" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A69" s="28"/>
-      <c r="B69" s="25"/>
-      <c r="C69" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="D69" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="E69" s="10" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A70" s="28"/>
-      <c r="B70" s="25"/>
-      <c r="C70" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="D70" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="E70" s="10" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A71" s="28"/>
-      <c r="B71" s="25"/>
-      <c r="C71" s="16" t="s">
+      <c r="E71" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="45">
+      <c r="A72" s="41"/>
+      <c r="B72" s="29"/>
+      <c r="C72" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="D71" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="E71" s="10" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A72" s="28"/>
-      <c r="B72" s="25"/>
-      <c r="C72" s="16" t="s">
-        <v>137</v>
-      </c>
       <c r="D72" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E72" s="10" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A73" s="28"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="45">
+      <c r="A73" s="41"/>
       <c r="B73" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C73" s="16" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D73" s="10" t="s">
         <v>36</v>
       </c>
       <c r="E73" s="10" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A74" s="28"/>
-      <c r="B74" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="45">
+      <c r="A74" s="41"/>
+      <c r="B74" s="28" t="s">
+        <v>127</v>
       </c>
       <c r="C74" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="D74" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="E74" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="45">
+      <c r="A75" s="41"/>
+      <c r="B75" s="30"/>
+      <c r="C75" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="D75" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="45">
+      <c r="A76" s="41"/>
+      <c r="B76" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C76" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="D74" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="E74" s="10" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A75" s="28"/>
-      <c r="B75" s="26"/>
-      <c r="C75" s="16" t="s">
+      <c r="D76" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="E76" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="30">
+      <c r="A77" s="41"/>
+      <c r="B77" s="29"/>
+      <c r="C77" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="D75" s="10" t="s">
+      <c r="D77" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="30">
+      <c r="A78" s="41"/>
+      <c r="B78" s="30"/>
+      <c r="C78" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D78" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="E78" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="30">
+      <c r="A79" s="41"/>
+      <c r="B79" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="C79" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="E75" s="10" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A76" s="28"/>
-      <c r="B76" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="C76" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="D76" s="10" t="s">
+      <c r="D79" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="E76" s="10" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A77" s="28"/>
-      <c r="B77" s="25"/>
-      <c r="C77" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="D77" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="E77" s="10" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A78" s="28"/>
-      <c r="B78" s="26"/>
-      <c r="C78" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="D78" s="10" t="s">
+      <c r="E79" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="30">
+      <c r="A80" s="41"/>
+      <c r="B80" s="35"/>
+      <c r="C80" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="D80" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="E78" s="10" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A79" s="28"/>
-      <c r="B79" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="C79" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="D79" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="E79" s="10" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A80" s="28"/>
-      <c r="B80" s="30"/>
-      <c r="C80" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="D80" s="10" t="s">
-        <v>156</v>
-      </c>
       <c r="E80" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A25:A34"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B68:B72"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="B76:B78"/>
     <mergeCell ref="A68:A80"/>
     <mergeCell ref="B79:B80"/>
     <mergeCell ref="B20:B21"/>
@@ -2650,15 +2626,15 @@
     <mergeCell ref="B60:B61"/>
     <mergeCell ref="B62:B65"/>
     <mergeCell ref="B66:B67"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B68:B72"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="B76:B78"/>
+    <mergeCell ref="A25:A34"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B15:B19"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showDropDown="1" sqref="A36:A41 A11" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showDropDown="1" sqref="A36:A41 A11"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2666,22 +2642,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="45" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="40.5">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -2695,7 +2671,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="55.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="56.25">
       <c r="A2" s="3" t="s">
         <v>21</v>
       </c>
@@ -2709,7 +2685,7 @@
         <v>45760</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="55.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="56.25">
       <c r="A3" s="3" t="s">
         <v>43</v>
       </c>
@@ -2723,7 +2699,7 @@
         <v>45765</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="37.5">
       <c r="A4" s="3" t="s">
         <v>47</v>
       </c>
@@ -2737,7 +2713,7 @@
         <v>45766</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="74.400000000000006" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="75">
       <c r="A5" s="3" t="s">
         <v>49</v>
       </c>
@@ -2751,87 +2727,101 @@
         <v>45773</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="37.5">
       <c r="A6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>73</v>
       </c>
       <c r="D6" s="5">
         <v>45773</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="37.5">
       <c r="A7" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D7" s="5">
         <v>45780</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="37.5">
       <c r="A8" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D8" s="5">
         <v>45781</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="37.5">
       <c r="A9" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D9" s="5">
         <v>45784</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="37.5">
       <c r="A10" s="3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D10" s="5">
         <v>45785</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="37.200000000000003" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="37.5">
       <c r="A11" s="3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="D11" s="5">
+        <v>45786</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="37.5">
+      <c r="A12" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="D11" s="5">
+      <c r="B12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="D12" s="5">
         <v>45786</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v2.6 Update Admin Home feature
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_SRS.xlsx
+++ b/LH_REQUIREMENTS/LH_SRS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="272">
   <si>
     <t>Feature</t>
   </si>
@@ -819,12 +819,159 @@
   <si>
     <t>Adjusted the Publish Audio after get comments</t>
   </si>
+  <si>
+    <t>v2.6</t>
+  </si>
+  <si>
+    <t>Update Admin Home feature</t>
+  </si>
+  <si>
+    <t>Admin Home</t>
+  </si>
+  <si>
+    <t>LH-CRS-ADMINHOME-001</t>
+  </si>
+  <si>
+    <t>LH-CRS-ADMINHOME-002</t>
+  </si>
+  <si>
+    <t>LH-CRS-ADMINHOME-003</t>
+  </si>
+  <si>
+    <t>LH-SRS-ADMINHOME-001</t>
+  </si>
+  <si>
+    <t>LH-SRS-ADMINHOME-002</t>
+  </si>
+  <si>
+    <t>LH-SRS-ADMINHOME-003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system shall provide administrators with access to a dedicated Admin Home Page. This page shall display all posts from every category, including each post’s title and a short preview.
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The Admin Home Page shall include a dropdown menu 
+labeled </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Admin Tools"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, containing various 
+administrative actions.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The Admin Home Page shall display a personalized 
+welcome message for the logged-in administrator in
+ the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>top-right corner</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The Admin Home Page shall display the application </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>logo
+ in the top-left corner</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>LH-SRS-ADMINHOME-004</t>
+  </si>
+  <si>
+    <t>LH-SRS-ADMINHOME-005</t>
+  </si>
+  <si>
+    <t>LH-SRS-ADMINHOME-006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system shall dynamically fetch posts displayed on the Admin Home Page to reflect the latest updates across all categories.
+</t>
+  </si>
+  <si>
+    <t>If fetching posts fails, the system shall display a generic 
+error message indicating that loading failed.</t>
+  </si>
+  <si>
+    <t>Each action in the Admin Tools dropdown shall be clearly labeled, accessible, and secure (e.g., requiring 
+confirmation before execution).</t>
+  </si>
+  <si>
+    <t>LH-SRS-ADMINHOME-007</t>
+  </si>
+  <si>
+    <t>LH-SRS-ADMINHOME-008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Admin Tools dropdown shall include the following actions:
+Delete Post
+Delete User
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -915,6 +1062,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1022,7 +1177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1090,6 +1245,45 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1099,39 +1293,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1141,11 +1302,17 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1427,10 +1594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G80"/>
+  <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="G69" sqref="G69"/>
+    <sheetView topLeftCell="A81" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1461,7 +1628,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="30">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="33" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="11" t="s">
@@ -1478,7 +1645,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="30">
-      <c r="A3" s="27"/>
+      <c r="A3" s="34"/>
       <c r="B3" s="11" t="s">
         <v>11</v>
       </c>
@@ -1493,7 +1660,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="30">
-      <c r="A4" s="27"/>
+      <c r="A4" s="34"/>
       <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
@@ -1508,7 +1675,7 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="27"/>
+      <c r="A5" s="34"/>
       <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
@@ -1523,7 +1690,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="30">
-      <c r="A6" s="27"/>
+      <c r="A6" s="34"/>
       <c r="B6" s="11" t="s">
         <v>14</v>
       </c>
@@ -1538,7 +1705,7 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="27"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="17" t="s">
         <v>15</v>
       </c>
@@ -1553,7 +1720,7 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="27"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="17" t="s">
         <v>30</v>
       </c>
@@ -1568,7 +1735,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="30">
-      <c r="A9" s="27"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="11" t="s">
         <v>31</v>
       </c>
@@ -1583,7 +1750,7 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="27"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="17" t="s">
         <v>32</v>
       </c>
@@ -1598,7 +1765,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="23.25" customHeight="1">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="36" t="s">
         <v>41</v>
       </c>
       <c r="B11" s="10" t="s">
@@ -1615,8 +1782,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="30">
-      <c r="A12" s="24"/>
-      <c r="B12" s="28" t="s">
+      <c r="A12" s="37"/>
+      <c r="B12" s="24" t="s">
         <v>42</v>
       </c>
       <c r="C12" s="10" t="s">
@@ -1630,8 +1797,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="30">
-      <c r="A13" s="24"/>
-      <c r="B13" s="29"/>
+      <c r="A13" s="37"/>
+      <c r="B13" s="25"/>
       <c r="C13" s="10" t="s">
         <v>59</v>
       </c>
@@ -1643,8 +1810,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="30">
-      <c r="A14" s="25"/>
-      <c r="B14" s="30"/>
+      <c r="A14" s="38"/>
+      <c r="B14" s="26"/>
       <c r="C14" s="10" t="s">
         <v>60</v>
       </c>
@@ -1656,10 +1823,10 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="30">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="30" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="11" t="s">
@@ -1673,7 +1840,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="45">
-      <c r="A16" s="27"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="32"/>
       <c r="C16" s="11" t="s">
         <v>62</v>
@@ -1686,7 +1853,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="28.5" customHeight="1">
-      <c r="A17" s="27"/>
+      <c r="A17" s="34"/>
       <c r="B17" s="32"/>
       <c r="C17" s="11" t="s">
         <v>63</v>
@@ -1699,7 +1866,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="30">
-      <c r="A18" s="27"/>
+      <c r="A18" s="34"/>
       <c r="B18" s="32"/>
       <c r="C18" s="11" t="s">
         <v>64</v>
@@ -1712,8 +1879,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="30">
-      <c r="A19" s="27"/>
-      <c r="B19" s="33"/>
+      <c r="A19" s="34"/>
+      <c r="B19" s="31"/>
       <c r="C19" s="11" t="s">
         <v>76</v>
       </c>
@@ -1725,8 +1892,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="45">
-      <c r="A20" s="27"/>
-      <c r="B20" s="31" t="s">
+      <c r="A20" s="34"/>
+      <c r="B20" s="30" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="11" t="s">
@@ -1740,8 +1907,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="30">
-      <c r="A21" s="27"/>
-      <c r="B21" s="33"/>
+      <c r="A21" s="34"/>
+      <c r="B21" s="31"/>
       <c r="C21" s="11" t="s">
         <v>82</v>
       </c>
@@ -1753,8 +1920,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="30">
-      <c r="A22" s="27"/>
-      <c r="B22" s="31" t="s">
+      <c r="A22" s="34"/>
+      <c r="B22" s="30" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="11" t="s">
@@ -1768,7 +1935,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="30">
-      <c r="A23" s="27"/>
+      <c r="A23" s="34"/>
       <c r="B23" s="32"/>
       <c r="C23" s="11" t="s">
         <v>86</v>
@@ -1781,8 +1948,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="30">
-      <c r="A24" s="36"/>
-      <c r="B24" s="33"/>
+      <c r="A24" s="35"/>
+      <c r="B24" s="31"/>
       <c r="C24" s="11" t="s">
         <v>88</v>
       </c>
@@ -1794,7 +1961,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="30">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="36" t="s">
         <v>245</v>
       </c>
       <c r="B25" s="10" t="s">
@@ -1811,7 +1978,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="30">
-      <c r="A26" s="24"/>
+      <c r="A26" s="37"/>
       <c r="B26" s="10" t="s">
         <v>213</v>
       </c>
@@ -1826,7 +1993,7 @@
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="24"/>
+      <c r="A27" s="37"/>
       <c r="B27" s="10" t="s">
         <v>214</v>
       </c>
@@ -1841,7 +2008,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="30">
-      <c r="A28" s="24"/>
+      <c r="A28" s="37"/>
       <c r="B28" s="10" t="s">
         <v>215</v>
       </c>
@@ -1856,7 +2023,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="30">
-      <c r="A29" s="24"/>
+      <c r="A29" s="37"/>
       <c r="B29" s="10" t="s">
         <v>216</v>
       </c>
@@ -1871,7 +2038,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="30">
-      <c r="A30" s="24"/>
+      <c r="A30" s="37"/>
       <c r="B30" s="10" t="s">
         <v>217</v>
       </c>
@@ -1886,7 +2053,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="30">
-      <c r="A31" s="24"/>
+      <c r="A31" s="37"/>
       <c r="B31" s="10" t="s">
         <v>218</v>
       </c>
@@ -1901,7 +2068,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="30">
-      <c r="A32" s="24"/>
+      <c r="A32" s="37"/>
       <c r="B32" s="10" t="s">
         <v>219</v>
       </c>
@@ -1916,7 +2083,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="30">
-      <c r="A33" s="24"/>
+      <c r="A33" s="37"/>
       <c r="B33" s="10" t="s">
         <v>220</v>
       </c>
@@ -1931,7 +2098,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="30">
-      <c r="A34" s="25"/>
+      <c r="A34" s="38"/>
       <c r="B34" s="10" t="s">
         <v>221</v>
       </c>
@@ -1965,10 +2132,10 @@
       <c r="G35" s="15"/>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1">
-      <c r="A36" s="23" t="s">
+      <c r="A36" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="40" t="s">
+      <c r="B36" s="23" t="s">
         <v>179</v>
       </c>
       <c r="C36" s="19" t="s">
@@ -1982,8 +2149,8 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1">
-      <c r="A37" s="24"/>
-      <c r="B37" s="40"/>
+      <c r="A37" s="37"/>
+      <c r="B37" s="23"/>
       <c r="C37" s="19" t="s">
         <v>182</v>
       </c>
@@ -1995,8 +2162,8 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1">
-      <c r="A38" s="24"/>
-      <c r="B38" s="40" t="s">
+      <c r="A38" s="37"/>
+      <c r="B38" s="23" t="s">
         <v>184</v>
       </c>
       <c r="C38" s="19" t="s">
@@ -2010,8 +2177,8 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1">
-      <c r="A39" s="24"/>
-      <c r="B39" s="40"/>
+      <c r="A39" s="37"/>
+      <c r="B39" s="23"/>
       <c r="C39" s="19" t="s">
         <v>187</v>
       </c>
@@ -2023,7 +2190,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1">
-      <c r="A40" s="24"/>
+      <c r="A40" s="37"/>
       <c r="B40" s="22" t="s">
         <v>189</v>
       </c>
@@ -2038,7 +2205,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1">
-      <c r="A41" s="24"/>
+      <c r="A41" s="37"/>
       <c r="B41" s="22" t="s">
         <v>192</v>
       </c>
@@ -2053,7 +2220,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="15" customHeight="1">
-      <c r="A42" s="24"/>
+      <c r="A42" s="37"/>
       <c r="B42" s="22" t="s">
         <v>195</v>
       </c>
@@ -2068,7 +2235,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="45">
-      <c r="A43" s="26" t="s">
+      <c r="A43" s="33" t="s">
         <v>25</v>
       </c>
       <c r="B43" s="11" t="s">
@@ -2085,7 +2252,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="30">
-      <c r="A44" s="27"/>
+      <c r="A44" s="34"/>
       <c r="B44" s="11" t="s">
         <v>27</v>
       </c>
@@ -2100,7 +2267,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="30">
-      <c r="A45" s="27"/>
+      <c r="A45" s="34"/>
       <c r="B45" s="11" t="s">
         <v>28</v>
       </c>
@@ -2115,10 +2282,10 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="30">
-      <c r="A46" s="23" t="s">
+      <c r="A46" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="B46" s="28" t="s">
+      <c r="B46" s="24" t="s">
         <v>94</v>
       </c>
       <c r="C46" s="10" t="s">
@@ -2132,8 +2299,8 @@
       </c>
     </row>
     <row r="47" spans="1:7" ht="30">
-      <c r="A47" s="24"/>
-      <c r="B47" s="29"/>
+      <c r="A47" s="37"/>
+      <c r="B47" s="25"/>
       <c r="C47" s="10" t="s">
         <v>97</v>
       </c>
@@ -2145,8 +2312,8 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="30">
-      <c r="A48" s="24"/>
-      <c r="B48" s="29"/>
+      <c r="A48" s="37"/>
+      <c r="B48" s="25"/>
       <c r="C48" s="10" t="s">
         <v>99</v>
       </c>
@@ -2158,8 +2325,8 @@
       </c>
     </row>
     <row r="49" spans="1:5" ht="30">
-      <c r="A49" s="24"/>
-      <c r="B49" s="30"/>
+      <c r="A49" s="37"/>
+      <c r="B49" s="26"/>
       <c r="C49" s="10" t="s">
         <v>101</v>
       </c>
@@ -2171,8 +2338,8 @@
       </c>
     </row>
     <row r="50" spans="1:5" ht="30">
-      <c r="A50" s="24"/>
-      <c r="B50" s="28" t="s">
+      <c r="A50" s="37"/>
+      <c r="B50" s="24" t="s">
         <v>103</v>
       </c>
       <c r="C50" s="10" t="s">
@@ -2186,8 +2353,8 @@
       </c>
     </row>
     <row r="51" spans="1:5" ht="30">
-      <c r="A51" s="24"/>
-      <c r="B51" s="29"/>
+      <c r="A51" s="37"/>
+      <c r="B51" s="25"/>
       <c r="C51" s="10" t="s">
         <v>106</v>
       </c>
@@ -2199,8 +2366,8 @@
       </c>
     </row>
     <row r="52" spans="1:5" ht="45">
-      <c r="A52" s="24"/>
-      <c r="B52" s="29"/>
+      <c r="A52" s="37"/>
+      <c r="B52" s="25"/>
       <c r="C52" s="10" t="s">
         <v>108</v>
       </c>
@@ -2212,8 +2379,8 @@
       </c>
     </row>
     <row r="53" spans="1:5" ht="45">
-      <c r="A53" s="24"/>
-      <c r="B53" s="30"/>
+      <c r="A53" s="37"/>
+      <c r="B53" s="26"/>
       <c r="C53" s="10" t="s">
         <v>110</v>
       </c>
@@ -2225,7 +2392,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" ht="45">
-      <c r="A54" s="24"/>
+      <c r="A54" s="37"/>
       <c r="B54" s="9" t="s">
         <v>112</v>
       </c>
@@ -2240,7 +2407,7 @@
       </c>
     </row>
     <row r="55" spans="1:5" ht="45">
-      <c r="A55" s="24"/>
+      <c r="A55" s="37"/>
       <c r="B55" s="9" t="s">
         <v>115</v>
       </c>
@@ -2255,8 +2422,8 @@
       </c>
     </row>
     <row r="56" spans="1:5" ht="30">
-      <c r="A56" s="24"/>
-      <c r="B56" s="28" t="s">
+      <c r="A56" s="37"/>
+      <c r="B56" s="24" t="s">
         <v>118</v>
       </c>
       <c r="C56" s="10" t="s">
@@ -2270,8 +2437,8 @@
       </c>
     </row>
     <row r="57" spans="1:5" ht="45">
-      <c r="A57" s="25"/>
-      <c r="B57" s="30"/>
+      <c r="A57" s="38"/>
+      <c r="B57" s="26"/>
       <c r="C57" s="10" t="s">
         <v>120</v>
       </c>
@@ -2283,10 +2450,10 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="30">
-      <c r="A58" s="26" t="s">
+      <c r="A58" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="B58" s="37" t="s">
+      <c r="B58" s="39" t="s">
         <v>157</v>
       </c>
       <c r="C58" s="18" t="s">
@@ -2300,8 +2467,8 @@
       </c>
     </row>
     <row r="59" spans="1:5" ht="33">
-      <c r="A59" s="27"/>
-      <c r="B59" s="38"/>
+      <c r="A59" s="34"/>
+      <c r="B59" s="40"/>
       <c r="C59" s="18" t="s">
         <v>160</v>
       </c>
@@ -2313,8 +2480,8 @@
       </c>
     </row>
     <row r="60" spans="1:5" ht="30">
-      <c r="A60" s="27"/>
-      <c r="B60" s="37" t="s">
+      <c r="A60" s="34"/>
+      <c r="B60" s="39" t="s">
         <v>162</v>
       </c>
       <c r="C60" s="18" t="s">
@@ -2328,8 +2495,8 @@
       </c>
     </row>
     <row r="61" spans="1:5" ht="33">
-      <c r="A61" s="27"/>
-      <c r="B61" s="38"/>
+      <c r="A61" s="34"/>
+      <c r="B61" s="40"/>
       <c r="C61" s="18" t="s">
         <v>165</v>
       </c>
@@ -2341,8 +2508,8 @@
       </c>
     </row>
     <row r="62" spans="1:5" ht="30">
-      <c r="A62" s="27"/>
-      <c r="B62" s="37" t="s">
+      <c r="A62" s="34"/>
+      <c r="B62" s="39" t="s">
         <v>167</v>
       </c>
       <c r="C62" s="18" t="s">
@@ -2356,8 +2523,8 @@
       </c>
     </row>
     <row r="63" spans="1:5" ht="49.5">
-      <c r="A63" s="27"/>
-      <c r="B63" s="39"/>
+      <c r="A63" s="34"/>
+      <c r="B63" s="41"/>
       <c r="C63" s="18" t="s">
         <v>170</v>
       </c>
@@ -2369,8 +2536,8 @@
       </c>
     </row>
     <row r="64" spans="1:5" ht="30">
-      <c r="A64" s="27"/>
-      <c r="B64" s="39"/>
+      <c r="A64" s="34"/>
+      <c r="B64" s="41"/>
       <c r="C64" s="18" t="s">
         <v>171</v>
       </c>
@@ -2382,8 +2549,8 @@
       </c>
     </row>
     <row r="65" spans="1:5" ht="33">
-      <c r="A65" s="27"/>
-      <c r="B65" s="38"/>
+      <c r="A65" s="34"/>
+      <c r="B65" s="40"/>
       <c r="C65" s="18" t="s">
         <v>172</v>
       </c>
@@ -2395,8 +2562,8 @@
       </c>
     </row>
     <row r="66" spans="1:5" ht="30">
-      <c r="A66" s="27"/>
-      <c r="B66" s="37" t="s">
+      <c r="A66" s="34"/>
+      <c r="B66" s="39" t="s">
         <v>174</v>
       </c>
       <c r="C66" s="18" t="s">
@@ -2410,8 +2577,8 @@
       </c>
     </row>
     <row r="67" spans="1:5" ht="49.5">
-      <c r="A67" s="27"/>
-      <c r="B67" s="38"/>
+      <c r="A67" s="34"/>
+      <c r="B67" s="40"/>
       <c r="C67" s="18" t="s">
         <v>177</v>
       </c>
@@ -2423,10 +2590,10 @@
       </c>
     </row>
     <row r="68" spans="1:5" ht="30">
-      <c r="A68" s="41" t="s">
+      <c r="A68" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="B68" s="28" t="s">
+      <c r="B68" s="24" t="s">
         <v>125</v>
       </c>
       <c r="C68" s="16" t="s">
@@ -2440,8 +2607,8 @@
       </c>
     </row>
     <row r="69" spans="1:5" ht="30">
-      <c r="A69" s="41"/>
-      <c r="B69" s="29"/>
+      <c r="A69" s="27"/>
+      <c r="B69" s="25"/>
       <c r="C69" s="16" t="s">
         <v>130</v>
       </c>
@@ -2453,8 +2620,8 @@
       </c>
     </row>
     <row r="70" spans="1:5" ht="30">
-      <c r="A70" s="41"/>
-      <c r="B70" s="29"/>
+      <c r="A70" s="27"/>
+      <c r="B70" s="25"/>
       <c r="C70" s="16" t="s">
         <v>131</v>
       </c>
@@ -2466,8 +2633,8 @@
       </c>
     </row>
     <row r="71" spans="1:5" ht="30">
-      <c r="A71" s="41"/>
-      <c r="B71" s="29"/>
+      <c r="A71" s="27"/>
+      <c r="B71" s="25"/>
       <c r="C71" s="16" t="s">
         <v>133</v>
       </c>
@@ -2479,8 +2646,8 @@
       </c>
     </row>
     <row r="72" spans="1:5" ht="45">
-      <c r="A72" s="41"/>
-      <c r="B72" s="29"/>
+      <c r="A72" s="27"/>
+      <c r="B72" s="25"/>
       <c r="C72" s="16" t="s">
         <v>135</v>
       </c>
@@ -2492,7 +2659,7 @@
       </c>
     </row>
     <row r="73" spans="1:5" ht="45">
-      <c r="A73" s="41"/>
+      <c r="A73" s="27"/>
       <c r="B73" s="10" t="s">
         <v>126</v>
       </c>
@@ -2507,8 +2674,8 @@
       </c>
     </row>
     <row r="74" spans="1:5" ht="45">
-      <c r="A74" s="41"/>
-      <c r="B74" s="28" t="s">
+      <c r="A74" s="27"/>
+      <c r="B74" s="24" t="s">
         <v>127</v>
       </c>
       <c r="C74" s="16" t="s">
@@ -2522,8 +2689,8 @@
       </c>
     </row>
     <row r="75" spans="1:5" ht="45">
-      <c r="A75" s="41"/>
-      <c r="B75" s="30"/>
+      <c r="A75" s="27"/>
+      <c r="B75" s="26"/>
       <c r="C75" s="16" t="s">
         <v>138</v>
       </c>
@@ -2535,8 +2702,8 @@
       </c>
     </row>
     <row r="76" spans="1:5" ht="45">
-      <c r="A76" s="41"/>
-      <c r="B76" s="28" t="s">
+      <c r="A76" s="27"/>
+      <c r="B76" s="24" t="s">
         <v>132</v>
       </c>
       <c r="C76" s="16" t="s">
@@ -2550,8 +2717,8 @@
       </c>
     </row>
     <row r="77" spans="1:5" ht="30">
-      <c r="A77" s="41"/>
-      <c r="B77" s="29"/>
+      <c r="A77" s="27"/>
+      <c r="B77" s="25"/>
       <c r="C77" s="16" t="s">
         <v>140</v>
       </c>
@@ -2563,8 +2730,8 @@
       </c>
     </row>
     <row r="78" spans="1:5" ht="30">
-      <c r="A78" s="41"/>
-      <c r="B78" s="30"/>
+      <c r="A78" s="27"/>
+      <c r="B78" s="26"/>
       <c r="C78" s="16" t="s">
         <v>141</v>
       </c>
@@ -2576,8 +2743,8 @@
       </c>
     </row>
     <row r="79" spans="1:5" ht="30">
-      <c r="A79" s="41"/>
-      <c r="B79" s="34" t="s">
+      <c r="A79" s="27"/>
+      <c r="B79" s="28" t="s">
         <v>134</v>
       </c>
       <c r="C79" s="16" t="s">
@@ -2591,8 +2758,8 @@
       </c>
     </row>
     <row r="80" spans="1:5" ht="30">
-      <c r="A80" s="41"/>
-      <c r="B80" s="35"/>
+      <c r="A80" s="27"/>
+      <c r="B80" s="29"/>
       <c r="C80" s="16" t="s">
         <v>149</v>
       </c>
@@ -2603,13 +2770,129 @@
         <v>128</v>
       </c>
     </row>
+    <row r="81" spans="1:5" ht="90">
+      <c r="A81" s="42" t="s">
+        <v>252</v>
+      </c>
+      <c r="B81" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="C81" s="43" t="s">
+        <v>256</v>
+      </c>
+      <c r="D81" s="44" t="s">
+        <v>259</v>
+      </c>
+      <c r="E81" s="43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="45">
+      <c r="A82" s="42"/>
+      <c r="B82" s="42"/>
+      <c r="C82" s="43" t="s">
+        <v>257</v>
+      </c>
+      <c r="D82" s="45" t="s">
+        <v>260</v>
+      </c>
+      <c r="E82" s="43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="45">
+      <c r="A83" s="42"/>
+      <c r="B83" s="42"/>
+      <c r="C83" s="43" t="s">
+        <v>258</v>
+      </c>
+      <c r="D83" s="45" t="s">
+        <v>261</v>
+      </c>
+      <c r="E83" s="43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="30">
+      <c r="A84" s="42"/>
+      <c r="B84" s="42"/>
+      <c r="C84" s="43" t="s">
+        <v>263</v>
+      </c>
+      <c r="D84" s="45" t="s">
+        <v>262</v>
+      </c>
+      <c r="E84" s="43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="75">
+      <c r="A85" s="42"/>
+      <c r="B85" s="42" t="s">
+        <v>254</v>
+      </c>
+      <c r="C85" s="43" t="s">
+        <v>264</v>
+      </c>
+      <c r="D85" s="44" t="s">
+        <v>266</v>
+      </c>
+      <c r="E85" s="43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="30">
+      <c r="A86" s="42"/>
+      <c r="B86" s="42"/>
+      <c r="C86" s="43" t="s">
+        <v>265</v>
+      </c>
+      <c r="D86" s="45" t="s">
+        <v>267</v>
+      </c>
+      <c r="E86" s="43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="75">
+      <c r="A87" s="42"/>
+      <c r="B87" s="42" t="s">
+        <v>255</v>
+      </c>
+      <c r="C87" s="43" t="s">
+        <v>269</v>
+      </c>
+      <c r="D87" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="E87" s="43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="45">
+      <c r="A88" s="42"/>
+      <c r="B88" s="42"/>
+      <c r="C88" s="43" t="s">
+        <v>270</v>
+      </c>
+      <c r="D88" s="45" t="s">
+        <v>268</v>
+      </c>
+      <c r="E88" s="43" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B68:B72"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="B76:B78"/>
+  <mergeCells count="30">
+    <mergeCell ref="B81:B84"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="B87:B88"/>
+    <mergeCell ref="A81:A88"/>
+    <mergeCell ref="A25:A34"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B15:B19"/>
     <mergeCell ref="A68:A80"/>
     <mergeCell ref="B79:B80"/>
     <mergeCell ref="B20:B21"/>
@@ -2626,11 +2909,11 @@
     <mergeCell ref="B60:B61"/>
     <mergeCell ref="B62:B65"/>
     <mergeCell ref="B66:B67"/>
-    <mergeCell ref="A25:A34"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B68:B72"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="B76:B78"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <dataValidations count="1">
@@ -2643,10 +2926,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2825,6 +3108,20 @@
         <v>45786</v>
       </c>
     </row>
+    <row r="13" spans="1:4" ht="18.75">
+      <c r="A13" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="D13" s="5">
+        <v>45786</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
v2.9 updated Login and Delete user due to review
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_SRS.xlsx
+++ b/LH_REQUIREMENTS/LH_SRS.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\testing\iti\6_QA\workshop\new_repo\Group-3-Learning-hub-dev\LH_REQUIREMENTS\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="LH_SRS" sheetId="1" r:id="rId1"/>
     <sheet name="LH_SRS_VERSION_HISTORY" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="307">
   <si>
     <t>Feature</t>
   </si>
@@ -137,9 +132,6 @@
     <t>Ensure all errors are visible and consistent in placement.</t>
   </si>
   <si>
-    <t>Ahmed Abuzaid</t>
-  </si>
-  <si>
     <t>Login</t>
   </si>
   <si>
@@ -158,22 +150,28 @@
     <t>LH-SRS-LOGIN-002</t>
   </si>
   <si>
-    <t>The system shall verify user registration status before allowing login; The email address must follow the format username@domain.com.</t>
+    <t>The system shall verify user registration status before allowing login.</t>
   </si>
   <si>
     <t>LH-SRS-LOGIN-003</t>
   </si>
   <si>
+    <t>The email address must follow the format username@domain.com.</t>
+  </si>
+  <si>
+    <t>LH-SRS-LOGIN-004</t>
+  </si>
+  <si>
     <t>The password must match the one provided during user registration.</t>
   </si>
   <si>
-    <t>LH-SRS-LOGIN-004</t>
+    <t>LH-SRS-LOGIN-005</t>
   </si>
   <si>
     <t>The system shall verify that login credentials match a registered user present in the user database.</t>
   </si>
   <si>
-    <t>LH-SRS-LOGIN-005</t>
+    <t>LH-SRS-LOGIN-006</t>
   </si>
   <si>
     <t>Only users with an active registration are permitted to access the system.</t>
@@ -182,13 +180,13 @@
     <t>LH-CRS-LOGIN-002</t>
   </si>
   <si>
-    <t>LH-SRS-LOGIN-006</t>
+    <t>LH-SRS-LOGIN-007</t>
   </si>
   <si>
     <t>In case of a failed login attempt, the system shall display a generic error message : "Invalid credentials" for all login failures (no specifics).</t>
   </si>
   <si>
-    <t>LH-SRS-LOGIN-007</t>
+    <t>LH-SRS-LOGIN-008</t>
   </si>
   <si>
     <t>The system shall not disclose whether the error is due to an incorrect email, incorrect password, or missing inputs.</t>
@@ -197,22 +195,22 @@
     <t>LH-CRS-LOGIN-003</t>
   </si>
   <si>
-    <t>LH-SRS-LOGIN-008</t>
+    <t>LH-SRS-LOGIN-009</t>
   </si>
   <si>
     <t>The system shall store user passwords in a hashed format to prevent plain-text storage.</t>
   </si>
   <si>
-    <t>LH-SRS-LOGIN-009</t>
-  </si>
-  <si>
-    <t>A simple salting mechanism shall be applied to each password before hashing to increase uniqueness.</t>
-  </si>
-  <si>
     <t>LH-SRS-LOGIN-010</t>
   </si>
   <si>
-    <t>The system shall not store raw (plain-text) passwords at any stage.</t>
+    <t>A random-generated salting shall be applied to each password before hashing to increase uniqueness.</t>
+  </si>
+  <si>
+    <t>LH-SRS-LOGIN-011</t>
+  </si>
+  <si>
+    <t>The system shall not store raw (plain-text) passwords in database, logs, or transmitted over the network.</t>
   </si>
   <si>
     <t>Categories</t>
@@ -234,6 +232,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF404040"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">	Render a dropdown list of available categories (e.g., </t>
     </r>
     <r>
@@ -241,7 +246,7 @@
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>“Category 1”, “Category 2”</t>
@@ -251,7 +256,7 @@
         <sz val="11"/>
         <color rgb="FF404040"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>).</t>
@@ -342,6 +347,9 @@
     <t>The system shall be deployable as a web-based application designed to run on PC platforms</t>
   </si>
   <si>
+    <t>Ahmed Abuzaid</t>
+  </si>
+  <si>
     <t>ADMIN Constraints</t>
   </si>
   <si>
@@ -447,7 +455,7 @@
     <t>LH-SRS-DELETEUSER-006</t>
   </si>
   <si>
-    <t>If no user matches the entered username, the system shall display an inline message indicating the user was not found.</t>
+    <t>If no user matches the entered username, the system shall display an inline message: "User was not found".</t>
   </si>
   <si>
     <t>LH-CRS-DELETEUSER-005</t>
@@ -670,6 +678,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF404040"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>The system enable the "Publish" button </t>
     </r>
     <r>
@@ -678,7 +693,7 @@
         <sz val="11"/>
         <color rgb="FF404040"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>only</t>
@@ -688,7 +703,7 @@
         <sz val="11"/>
         <color rgb="FF404040"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t> when: (1) A recording exists (≤5 mins), and (2) The title field is non-empty.</t>
@@ -815,6 +830,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">The Admin Home Page shall include a dropdown menu 
 labeled </t>
     </r>
@@ -824,7 +846,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>"Admin Tools"</t>
@@ -834,7 +856,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>, containing various 
@@ -846,6 +868,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">The Admin Home Page shall display a personalized 
 welcome message for the logged-in administrator in
  the </t>
@@ -856,7 +885,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>top-right corner</t>
@@ -866,7 +895,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>.</t>
@@ -877,6 +906,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">The Admin Home Page shall display the application </t>
     </r>
     <r>
@@ -885,7 +921,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>logo
@@ -896,7 +932,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>.</t>
@@ -939,6 +975,45 @@
 confirmation before execution).</t>
   </si>
   <si>
+    <t>Notifications</t>
+  </si>
+  <si>
+    <t>LH-CRS-NOTIFICATIONS-001</t>
+  </si>
+  <si>
+    <t>LH-SRS-NOTIFICATIONS-001</t>
+  </si>
+  <si>
+    <t>The system allow users to follow specific categories (e.g., Economy, Sports) from the categories section.</t>
+  </si>
+  <si>
+    <t>LH-SRS-NOTIFICATIONS-002</t>
+  </si>
+  <si>
+    <t>The system store followed categories in the user's profile for future reference.</t>
+  </si>
+  <si>
+    <t>LH-CRS-NOTIFICATIONS-002</t>
+  </si>
+  <si>
+    <t>LH-SRS-NOTIFICATIONS-003</t>
+  </si>
+  <si>
+    <t>The system display an "Updates from Followed Categories" section on the home page.</t>
+  </si>
+  <si>
+    <t>LH-SRS-NOTIFICATIONS-004</t>
+  </si>
+  <si>
+    <t>The system shall automatically update this section when new content is added to followed categories.</t>
+  </si>
+  <si>
+    <t>LH-SRS-NOTIFICATIONS-005</t>
+  </si>
+  <si>
+    <t>there is a bell icon that show the number of new notifications</t>
+  </si>
+  <si>
     <t>Version number</t>
   </si>
   <si>
@@ -1030,56 +1105,29 @@
     <t>Update Delete User feature</t>
   </si>
   <si>
-    <t>LH-CRS-NOTIFICATIONS-001</t>
-  </si>
-  <si>
-    <t>LH-CRS-NOTIFICATIONS-002</t>
-  </si>
-  <si>
-    <t>Notifications</t>
-  </si>
-  <si>
-    <t>LH-SRS-NOTIFICATIONS-001</t>
-  </si>
-  <si>
-    <t>LH-SRS-NOTIFICATIONS-002</t>
-  </si>
-  <si>
-    <t>LH-SRS-NOTIFICATIONS-003</t>
-  </si>
-  <si>
-    <t>LH-SRS-NOTIFICATIONS-004</t>
-  </si>
-  <si>
-    <t>The system allow users to follow specific categories (e.g., Economy, Sports) from the categories section.</t>
-  </si>
-  <si>
-    <t>The system store followed categories in the user's profile for future reference.</t>
-  </si>
-  <si>
-    <t>The system display an "Updates from Followed Categories" section on the home page.</t>
-  </si>
-  <si>
-    <t>The system shall automatically update this section when new content is added to followed categories.</t>
-  </si>
-  <si>
-    <t>there is a bell icon that show the number of new notifications</t>
-  </si>
-  <si>
-    <t>LH-SRS-NOTIFICATIONS-005</t>
-  </si>
-  <si>
     <t>v2.8</t>
   </si>
   <si>
     <t>Update system constraints and notifications feature</t>
+  </si>
+  <si>
+    <t>v2.9</t>
+  </si>
+  <si>
+    <t>Update Login and Delete user feature due to the review</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="16">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="33">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1088,18 +1136,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="16"/>
       <color theme="0"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -1112,36 +1153,28 @@
       <sz val="15"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="15"/>
       <color theme="0"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="15"/>
       <color theme="0"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1156,34 +1189,128 @@
       <sz val="11"/>
       <color rgb="FF404040"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF404040"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF404040"/>
       <name val="Segoe UI"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF404040"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1191,11 +1318,61 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1222,7 +1399,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79995117038483843"/>
+        <fgColor theme="4" tint="0.799951170384838"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1232,8 +1409,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1293,28 +1656,270 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1326,153 +1931,185 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1730,29 +2367,29 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G98"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="D98" sqref="D98"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85714285714286" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="53.42578125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" style="7" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="7"/>
+    <col min="1" max="1" width="19.8571428571429" style="7" customWidth="1"/>
+    <col min="2" max="2" width="32.7142857142857" style="7" customWidth="1"/>
+    <col min="3" max="3" width="29.5714285714286" style="8" customWidth="1"/>
+    <col min="4" max="4" width="53.4285714285714" style="9" customWidth="1"/>
+    <col min="5" max="5" width="23.1428571428571" style="7" customWidth="1"/>
+    <col min="6" max="16384" width="8.85714285714286" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5">
+    <row r="1" ht="19.5" spans="1:5">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1769,1676 +2406,1706 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30">
-      <c r="A2" s="28" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30">
-      <c r="A3" s="29"/>
-      <c r="B3" s="15" t="s">
+    <row r="3" spans="1:5">
+      <c r="A3" s="18"/>
+      <c r="B3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30">
-      <c r="A4" s="29"/>
-      <c r="B4" s="15" t="s">
+    <row r="4" ht="30" spans="1:5">
+      <c r="A4" s="18"/>
+      <c r="B4" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="29"/>
-      <c r="B5" s="15" t="s">
+      <c r="A5" s="18"/>
+      <c r="B5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30">
-      <c r="A6" s="29"/>
-      <c r="B6" s="15" t="s">
+    <row r="6" spans="1:5">
+      <c r="A6" s="18"/>
+      <c r="B6" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="29"/>
-      <c r="B7" s="17" t="s">
+      <c r="A7" s="18"/>
+      <c r="B7" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="29"/>
-      <c r="B8" s="17" t="s">
+      <c r="A8" s="18"/>
+      <c r="B8" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30">
-      <c r="A9" s="29"/>
-      <c r="B9" s="15" t="s">
+    <row r="9" ht="30" spans="1:5">
+      <c r="A9" s="18"/>
+      <c r="B9" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="29"/>
-      <c r="B10" s="17" t="s">
+      <c r="A10" s="18"/>
+      <c r="B10" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30">
-      <c r="A11" s="28" t="s">
+    <row r="11" ht="30" spans="1:5">
+      <c r="A11" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="C11" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="D11" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="E11" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="15" t="s">
+    </row>
+    <row r="12" ht="30" spans="1:5">
+      <c r="A12" s="18"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="16" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="45">
-      <c r="A12" s="29"/>
-      <c r="B12" s="40"/>
-      <c r="C12" s="15" t="s">
+      <c r="D12" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="E12" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" ht="28.5" customHeight="1" spans="1:5">
+      <c r="A13" s="18"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="28.5" customHeight="1">
-      <c r="A13" s="29"/>
-      <c r="B13" s="40"/>
-      <c r="C13" s="15" t="s">
+      <c r="D13" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="E13" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" ht="28.5" customHeight="1" spans="1:5">
+      <c r="A14" s="18"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="30">
-      <c r="A14" s="29"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="15" t="s">
+      <c r="D14" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="E14" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" ht="30" spans="1:5">
+      <c r="A15" s="18"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30">
-      <c r="A15" s="29"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="15" t="s">
+      <c r="D15" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="E15" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" ht="30" spans="1:5">
+      <c r="A16" s="18"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="45">
-      <c r="A16" s="29"/>
-      <c r="B16" s="39" t="s">
+      <c r="D16" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="E16" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" ht="45" spans="1:5">
+      <c r="A17" s="18"/>
+      <c r="B17" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="C17" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="30">
-      <c r="A17" s="29"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="15" t="s">
+      <c r="D17" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="E17" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" ht="30" spans="1:5">
+      <c r="A18" s="18"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="30">
-      <c r="A18" s="29"/>
-      <c r="B18" s="39" t="s">
+      <c r="D18" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="E18" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" ht="30" spans="1:5">
+      <c r="A19" s="18"/>
+      <c r="B19" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="C19" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="E18" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="30">
-      <c r="A19" s="29"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="15" t="s">
+      <c r="D19" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="E19" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" ht="30" spans="1:5">
+      <c r="A20" s="18"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="30">
-      <c r="A20" s="33"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="15" t="s">
+      <c r="D20" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="E20" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" ht="30" spans="1:5">
+      <c r="A21" s="22"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="E20" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="30">
-      <c r="A21" s="30" t="s">
+      <c r="D21" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="E21" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" ht="30" spans="1:5">
+      <c r="A22" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="B22" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="C22" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="E21" s="18" t="s">
+      <c r="D22" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="30">
-      <c r="A22" s="31"/>
-      <c r="B22" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="18" t="s">
+    <row r="23" ht="30" spans="1:5">
+      <c r="A23" s="26"/>
+      <c r="B23" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="C23" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="D23" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" s="24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="31"/>
-      <c r="B23" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="18" t="s">
+    <row r="24" spans="1:5">
+      <c r="A24" s="26"/>
+      <c r="B24" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="C24" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="E23" s="18" t="s">
+      <c r="D24" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" s="24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="30">
-      <c r="A24" s="31"/>
-      <c r="B24" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" s="18" t="s">
+    <row r="25" ht="30" spans="1:5">
+      <c r="A25" s="26"/>
+      <c r="B25" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="C25" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="E24" s="18" t="s">
+      <c r="D25" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="30">
-      <c r="A25" s="31"/>
-      <c r="B25" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="C25" s="18" t="s">
+    <row r="26" ht="30" spans="1:5">
+      <c r="A26" s="26"/>
+      <c r="B26" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="C26" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="E25" s="18" t="s">
+      <c r="D26" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" s="24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="30">
-      <c r="A26" s="31"/>
-      <c r="B26" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="C26" s="18" t="s">
+    <row r="27" ht="30" spans="1:5">
+      <c r="A27" s="26"/>
+      <c r="B27" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="C27" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="E26" s="18" t="s">
+      <c r="D27" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" s="24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="30">
-      <c r="A27" s="31"/>
-      <c r="B27" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C27" s="18" t="s">
+    <row r="28" ht="30" spans="1:5">
+      <c r="A28" s="26"/>
+      <c r="B28" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="C28" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="D28" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" s="24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="30">
-      <c r="A28" s="31"/>
-      <c r="B28" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="C28" s="18" t="s">
+    <row r="29" ht="30" spans="1:5">
+      <c r="A29" s="26"/>
+      <c r="B29" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="C29" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="E28" s="18" t="s">
+      <c r="D29" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29" s="24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="30">
-      <c r="A29" s="31"/>
-      <c r="B29" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="C29" s="18" t="s">
+    <row r="30" ht="30" spans="1:5">
+      <c r="A30" s="26"/>
+      <c r="B30" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="C30" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="E29" s="18" t="s">
+      <c r="D30" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="E30" s="24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="30">
-      <c r="A30" s="32"/>
-      <c r="B30" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="C30" s="18" t="s">
+    <row r="31" ht="30" spans="1:5">
+      <c r="A31" s="27"/>
+      <c r="B31" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="D30" s="19" t="s">
+      <c r="C31" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="E30" s="18" t="s">
+      <c r="D31" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E31" s="24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="30">
-      <c r="A31" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="B31" s="15" t="s">
+    <row r="32" ht="30" spans="1:7">
+      <c r="A32" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="B32" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="C32" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E31" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-    </row>
-    <row r="32" spans="1:7" ht="30" customHeight="1">
-      <c r="A32" s="30" t="s">
+      <c r="D32" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B32" s="42" t="s">
+      <c r="E32" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+    </row>
+    <row r="33" ht="30" customHeight="1" spans="1:5">
+      <c r="A33" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="D32" s="24" t="s">
+      <c r="B33" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="E32" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="30" customHeight="1">
-      <c r="A33" s="31"/>
-      <c r="B33" s="42"/>
-      <c r="C33" s="24" t="s">
+      <c r="C33" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="D33" s="24" t="s">
+      <c r="D33" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E33" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="30" customHeight="1">
-      <c r="A34" s="31"/>
-      <c r="B34" s="42" t="s">
+      <c r="E33" s="24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" ht="30" customHeight="1" spans="1:5">
+      <c r="A34" s="26"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="C34" s="24" t="s">
+      <c r="D34" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="D34" s="24" t="s">
+      <c r="E34" s="24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" ht="30" customHeight="1" spans="1:5">
+      <c r="A35" s="26"/>
+      <c r="B35" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="E34" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="30" customHeight="1">
-      <c r="A35" s="31"/>
-      <c r="B35" s="42"/>
-      <c r="C35" s="24" t="s">
+      <c r="C35" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="D35" s="24" t="s">
+      <c r="D35" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="E35" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="30" customHeight="1">
-      <c r="A36" s="31"/>
-      <c r="B36" s="23" t="s">
+      <c r="E35" s="24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" ht="30" customHeight="1" spans="1:5">
+      <c r="A36" s="26"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="C36" s="24" t="s">
+      <c r="D36" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="D36" s="24" t="s">
+      <c r="E36" s="24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" ht="30" customHeight="1" spans="1:5">
+      <c r="A37" s="26"/>
+      <c r="B37" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="E36" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="30" customHeight="1">
-      <c r="A37" s="31"/>
-      <c r="B37" s="23" t="s">
+      <c r="C37" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="C37" s="24" t="s">
+      <c r="D37" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="D37" s="24" t="s">
+      <c r="E37" s="24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" ht="30" customHeight="1" spans="1:5">
+      <c r="A38" s="26"/>
+      <c r="B38" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="E37" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="30">
-      <c r="A38" s="31"/>
-      <c r="B38" s="23" t="s">
+      <c r="C38" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="C38" s="24" t="s">
+      <c r="D38" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="D38" s="24" t="s">
+      <c r="E38" s="24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" ht="30" spans="1:5">
+      <c r="A39" s="26"/>
+      <c r="B39" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="E38" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="30">
-      <c r="A39" s="34"/>
-      <c r="B39" s="43" t="s">
+      <c r="C39" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="C39" s="24" t="s">
+      <c r="D39" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="D39" s="24" t="s">
+      <c r="E39" s="24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" ht="30" spans="1:5">
+      <c r="A40" s="32"/>
+      <c r="B40" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="E39" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="45">
-      <c r="A40" s="34"/>
-      <c r="B40" s="44"/>
-      <c r="C40" s="24" t="s">
+      <c r="C40" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="D40" s="24" t="s">
+      <c r="D40" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="E40" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="30">
-      <c r="A41" s="34"/>
-      <c r="B41" s="43" t="s">
+      <c r="E40" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" ht="30" spans="1:5">
+      <c r="A41" s="32"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="C41" s="24" t="s">
+      <c r="D41" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="D41" s="24" t="s">
+      <c r="E41" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" ht="30" spans="1:5">
+      <c r="A42" s="32"/>
+      <c r="B42" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="E41" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="30">
-      <c r="A42" s="34"/>
-      <c r="B42" s="44"/>
-      <c r="C42" s="24" t="s">
+      <c r="C42" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="D42" s="24" t="s">
+      <c r="D42" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="E42" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="30">
-      <c r="A43" s="34"/>
-      <c r="B43" s="23" t="s">
+      <c r="E42" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" ht="30" spans="1:5">
+      <c r="A43" s="32"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="C43" s="24" t="s">
+      <c r="D43" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="D43" s="24" t="s">
+      <c r="E43" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" ht="30" spans="1:5">
+      <c r="A44" s="32"/>
+      <c r="B44" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="E43" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="45">
-      <c r="A44" s="34"/>
-      <c r="B44" s="23" t="s">
+      <c r="C44" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="C44" s="24" t="s">
+      <c r="D44" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="D44" s="24" t="s">
+      <c r="E44" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" ht="30" spans="1:5">
+      <c r="A45" s="32"/>
+      <c r="B45" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="E44" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="30">
-      <c r="A45" s="34"/>
-      <c r="B45" s="23" t="s">
+      <c r="C45" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="C45" s="24" t="s">
+      <c r="D45" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="D45" s="24" t="s">
+      <c r="E45" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" ht="30" spans="1:5">
+      <c r="A46" s="32"/>
+      <c r="B46" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="E45" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="30">
-      <c r="A46" s="34"/>
-      <c r="B46" s="23" t="s">
+      <c r="C46" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="C46" s="24" t="s">
+      <c r="D46" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="D46" s="24" t="s">
+      <c r="E46" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" ht="30" spans="1:5">
+      <c r="A47" s="32"/>
+      <c r="B47" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="E46" s="23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="45">
-      <c r="A47" s="34"/>
-      <c r="B47" s="43" t="s">
+      <c r="C47" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="C47" s="24" t="s">
+      <c r="D47" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="D47" s="24" t="s">
+      <c r="E47" s="30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" ht="45" spans="1:5">
+      <c r="A48" s="32"/>
+      <c r="B48" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="E47" s="23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="60">
-      <c r="A48" s="34"/>
-      <c r="B48" s="44"/>
-      <c r="C48" s="24" t="s">
+      <c r="C48" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="D48" s="24" t="s">
+      <c r="D48" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="E48" s="23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="45">
-      <c r="A49" s="28" t="s">
+      <c r="E48" s="30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="49" ht="60" spans="1:5">
+      <c r="A49" s="32"/>
+      <c r="B49" s="34"/>
+      <c r="C49" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="B49" s="15" t="s">
+      <c r="D49" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="C49" s="15" t="s">
+      <c r="E49" s="30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50" ht="45" spans="1:5">
+      <c r="A50" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="D49" s="16" t="s">
+      <c r="B50" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="E49" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="30">
-      <c r="A50" s="29"/>
-      <c r="B50" s="15" t="s">
+      <c r="C50" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="C50" s="15" t="s">
+      <c r="D50" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="D50" s="16" t="s">
+      <c r="E50" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" ht="30" spans="1:5">
+      <c r="A51" s="18"/>
+      <c r="B51" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="E50" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="30">
-      <c r="A51" s="29"/>
-      <c r="B51" s="15" t="s">
+      <c r="C51" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="C51" s="15" t="s">
+      <c r="D51" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="D51" s="16" t="s">
+      <c r="E51" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="52" ht="30" spans="1:5">
+      <c r="A52" s="18"/>
+      <c r="B52" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="E51" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="30">
-      <c r="A52" s="30" t="s">
+      <c r="C52" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="B52" s="36" t="s">
+      <c r="D52" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="C52" s="18" t="s">
+      <c r="E52" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53" ht="30" spans="1:5">
+      <c r="A53" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="D52" s="19" t="s">
+      <c r="B53" s="35" t="s">
         <v>155</v>
       </c>
-      <c r="E52" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="30">
-      <c r="A53" s="31"/>
-      <c r="B53" s="37"/>
-      <c r="C53" s="18" t="s">
+      <c r="C53" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="D53" s="19" t="s">
+      <c r="D53" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="E53" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="30">
-      <c r="A54" s="31"/>
-      <c r="B54" s="37"/>
-      <c r="C54" s="18" t="s">
+      <c r="E53" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" ht="30" spans="1:5">
+      <c r="A54" s="26"/>
+      <c r="B54" s="36"/>
+      <c r="C54" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="D54" s="19" t="s">
+      <c r="D54" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="E54" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="30">
-      <c r="A55" s="31"/>
-      <c r="B55" s="38"/>
-      <c r="C55" s="18" t="s">
+      <c r="E54" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="55" ht="30" spans="1:5">
+      <c r="A55" s="26"/>
+      <c r="B55" s="36"/>
+      <c r="C55" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="D55" s="19" t="s">
+      <c r="D55" s="25" t="s">
         <v>161</v>
       </c>
-      <c r="E55" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="30">
-      <c r="A56" s="31"/>
-      <c r="B56" s="36" t="s">
+      <c r="E55" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="56" ht="30" spans="1:5">
+      <c r="A56" s="26"/>
+      <c r="B56" s="37"/>
+      <c r="C56" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="C56" s="18" t="s">
+      <c r="D56" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="D56" s="19" t="s">
+      <c r="E56" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="57" ht="30" spans="1:5">
+      <c r="A57" s="26"/>
+      <c r="B57" s="35" t="s">
         <v>164</v>
       </c>
-      <c r="E56" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="30">
-      <c r="A57" s="31"/>
-      <c r="B57" s="37"/>
-      <c r="C57" s="18" t="s">
+      <c r="C57" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="D57" s="19" t="s">
+      <c r="D57" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="E57" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="45">
-      <c r="A58" s="31"/>
-      <c r="B58" s="37"/>
-      <c r="C58" s="18" t="s">
+      <c r="E57" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="58" ht="30" spans="1:5">
+      <c r="A58" s="26"/>
+      <c r="B58" s="36"/>
+      <c r="C58" s="24" t="s">
         <v>167</v>
       </c>
-      <c r="D58" s="19" t="s">
+      <c r="D58" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="E58" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="45">
-      <c r="A59" s="31"/>
-      <c r="B59" s="38"/>
-      <c r="C59" s="18" t="s">
+      <c r="E58" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" ht="45" spans="1:5">
+      <c r="A59" s="26"/>
+      <c r="B59" s="36"/>
+      <c r="C59" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="D59" s="19" t="s">
+      <c r="D59" s="25" t="s">
         <v>170</v>
       </c>
-      <c r="E59" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="45">
-      <c r="A60" s="31"/>
-      <c r="B60" s="20" t="s">
+      <c r="E59" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="60" ht="30" spans="1:5">
+      <c r="A60" s="26"/>
+      <c r="B60" s="37"/>
+      <c r="C60" s="24" t="s">
         <v>171</v>
       </c>
-      <c r="C60" s="18" t="s">
+      <c r="D60" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="D60" s="19" t="s">
+      <c r="E60" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="61" ht="45" spans="1:5">
+      <c r="A61" s="26"/>
+      <c r="B61" s="37" t="s">
         <v>173</v>
       </c>
-      <c r="E60" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="45">
-      <c r="A61" s="31"/>
-      <c r="B61" s="20" t="s">
+      <c r="C61" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="C61" s="18" t="s">
+      <c r="D61" s="25" t="s">
         <v>175</v>
       </c>
-      <c r="D61" s="19" t="s">
+      <c r="E61" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="62" ht="45" spans="1:5">
+      <c r="A62" s="26"/>
+      <c r="B62" s="37" t="s">
         <v>176</v>
       </c>
-      <c r="E61" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="30">
-      <c r="A62" s="31"/>
-      <c r="B62" s="36" t="s">
+      <c r="C62" s="24" t="s">
         <v>177</v>
       </c>
-      <c r="C62" s="18" t="s">
+      <c r="D62" s="25" t="s">
         <v>178</v>
       </c>
-      <c r="D62" s="19" t="s">
+      <c r="E62" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="63" ht="30" spans="1:5">
+      <c r="A63" s="26"/>
+      <c r="B63" s="35" t="s">
         <v>179</v>
       </c>
-      <c r="E62" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="45">
-      <c r="A63" s="32"/>
-      <c r="B63" s="38"/>
-      <c r="C63" s="18" t="s">
+      <c r="C63" s="24" t="s">
         <v>180</v>
       </c>
-      <c r="D63" s="19" t="s">
+      <c r="D63" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="E63" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="30">
-      <c r="A64" s="28" t="s">
+      <c r="E63" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="64" ht="45" spans="1:5">
+      <c r="A64" s="27"/>
+      <c r="B64" s="37"/>
+      <c r="C64" s="24" t="s">
         <v>182</v>
       </c>
-      <c r="B64" s="45" t="s">
+      <c r="D64" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="C64" s="25" t="s">
+      <c r="E64" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="65" ht="30" spans="1:5">
+      <c r="A65" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="D64" s="25" t="s">
+      <c r="B65" s="38" t="s">
         <v>185</v>
       </c>
-      <c r="E64" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="30">
-      <c r="A65" s="29"/>
-      <c r="B65" s="46"/>
-      <c r="C65" s="25" t="s">
+      <c r="C65" s="39" t="s">
         <v>186</v>
       </c>
-      <c r="D65" s="25" t="s">
+      <c r="D65" s="39" t="s">
         <v>187</v>
       </c>
-      <c r="E65" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="30">
-      <c r="A66" s="29"/>
-      <c r="B66" s="45" t="s">
+      <c r="E65" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="66" ht="30" spans="1:5">
+      <c r="A66" s="18"/>
+      <c r="B66" s="40"/>
+      <c r="C66" s="39" t="s">
         <v>188</v>
       </c>
-      <c r="C66" s="25" t="s">
+      <c r="D66" s="39" t="s">
         <v>189</v>
       </c>
-      <c r="D66" s="25" t="s">
+      <c r="E66" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="67" ht="30" spans="1:5">
+      <c r="A67" s="18"/>
+      <c r="B67" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="E66" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="30">
-      <c r="A67" s="29"/>
-      <c r="B67" s="46"/>
-      <c r="C67" s="25" t="s">
+      <c r="C67" s="39" t="s">
         <v>191</v>
       </c>
-      <c r="D67" s="25" t="s">
+      <c r="D67" s="39" t="s">
         <v>192</v>
       </c>
-      <c r="E67" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="30">
-      <c r="A68" s="29"/>
-      <c r="B68" s="45" t="s">
+      <c r="E67" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="68" ht="30" spans="1:5">
+      <c r="A68" s="18"/>
+      <c r="B68" s="40"/>
+      <c r="C68" s="39" t="s">
         <v>193</v>
       </c>
-      <c r="C68" s="25" t="s">
+      <c r="D68" s="39" t="s">
         <v>194</v>
       </c>
-      <c r="D68" s="25" t="s">
+      <c r="E68" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="69" ht="30" spans="1:5">
+      <c r="A69" s="18"/>
+      <c r="B69" s="38" t="s">
         <v>195</v>
       </c>
-      <c r="E68" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="30">
-      <c r="A69" s="29"/>
-      <c r="B69" s="47"/>
-      <c r="C69" s="25" t="s">
+      <c r="C69" s="39" t="s">
         <v>196</v>
       </c>
-      <c r="D69" s="25" t="s">
+      <c r="D69" s="39" t="s">
         <v>197</v>
       </c>
-      <c r="E69" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="30">
-      <c r="A70" s="29"/>
-      <c r="B70" s="47"/>
-      <c r="C70" s="25" t="s">
+      <c r="E69" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="70" ht="30" spans="1:5">
+      <c r="A70" s="18"/>
+      <c r="B70" s="41"/>
+      <c r="C70" s="39" t="s">
         <v>198</v>
       </c>
-      <c r="D70" s="25" t="s">
+      <c r="D70" s="39" t="s">
         <v>199</v>
       </c>
-      <c r="E70" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="30">
-      <c r="A71" s="29"/>
-      <c r="B71" s="45" t="s">
+      <c r="E70" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="71" ht="30" spans="1:5">
+      <c r="A71" s="18"/>
+      <c r="B71" s="41"/>
+      <c r="C71" s="39" t="s">
         <v>200</v>
       </c>
-      <c r="C71" s="25" t="s">
+      <c r="D71" s="39" t="s">
         <v>201</v>
       </c>
-      <c r="D71" s="25" t="s">
+      <c r="E71" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="72" ht="30" spans="1:5">
+      <c r="A72" s="18"/>
+      <c r="B72" s="38" t="s">
         <v>202</v>
       </c>
-      <c r="E71" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="45">
-      <c r="A72" s="29"/>
-      <c r="B72" s="46"/>
-      <c r="C72" s="25" t="s">
+      <c r="C72" s="39" t="s">
         <v>203</v>
       </c>
-      <c r="D72" s="25" t="s">
+      <c r="D72" s="39" t="s">
         <v>204</v>
       </c>
-      <c r="E72" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="30">
-      <c r="A73" s="35" t="s">
+      <c r="E72" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="73" ht="45" spans="1:5">
+      <c r="A73" s="18"/>
+      <c r="B73" s="40"/>
+      <c r="C73" s="39" t="s">
         <v>205</v>
       </c>
-      <c r="B73" s="36" t="s">
+      <c r="D73" s="39" t="s">
         <v>206</v>
       </c>
-      <c r="C73" s="26" t="s">
+      <c r="E73" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="74" ht="30" spans="1:5">
+      <c r="A74" s="42" t="s">
         <v>207</v>
       </c>
-      <c r="D73" s="19" t="s">
+      <c r="B74" s="35" t="s">
         <v>208</v>
       </c>
-      <c r="E73" s="18" t="s">
+      <c r="C74" s="43" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" ht="30">
-      <c r="A74" s="35"/>
-      <c r="B74" s="37"/>
-      <c r="C74" s="26" t="s">
+      <c r="D74" s="25" t="s">
         <v>210</v>
       </c>
-      <c r="D74" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="E74" s="18" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="30">
-      <c r="A75" s="35"/>
-      <c r="B75" s="37"/>
-      <c r="C75" s="26" t="s">
+      <c r="E74" s="24" t="s">
         <v>211</v>
       </c>
-      <c r="D75" s="19" t="s">
+    </row>
+    <row r="75" ht="30" spans="1:5">
+      <c r="A75" s="42"/>
+      <c r="B75" s="36"/>
+      <c r="C75" s="43" t="s">
         <v>212</v>
       </c>
-      <c r="E75" s="18" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="30">
-      <c r="A76" s="35"/>
-      <c r="B76" s="37"/>
-      <c r="C76" s="26" t="s">
+      <c r="D75" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="E75" s="24" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="76" ht="30" spans="1:5">
+      <c r="A76" s="42"/>
+      <c r="B76" s="36"/>
+      <c r="C76" s="43" t="s">
         <v>213</v>
       </c>
-      <c r="D76" s="19" t="s">
+      <c r="D76" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="E76" s="18" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="45">
-      <c r="A77" s="35"/>
-      <c r="B77" s="37"/>
-      <c r="C77" s="26" t="s">
+      <c r="E76" s="24" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="77" ht="30" spans="1:5">
+      <c r="A77" s="42"/>
+      <c r="B77" s="36"/>
+      <c r="C77" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="D77" s="19" t="s">
+      <c r="D77" s="25" t="s">
         <v>216</v>
       </c>
-      <c r="E77" s="18" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="45">
-      <c r="A78" s="35"/>
-      <c r="B78" s="18" t="s">
+      <c r="E77" s="24" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="78" ht="45" spans="1:5">
+      <c r="A78" s="42"/>
+      <c r="B78" s="36"/>
+      <c r="C78" s="43" t="s">
         <v>217</v>
       </c>
-      <c r="C78" s="26" t="s">
+      <c r="D78" s="25" t="s">
         <v>218</v>
       </c>
-      <c r="D78" s="19" t="s">
+      <c r="E78" s="24" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="79" ht="45" spans="1:5">
+      <c r="A79" s="42"/>
+      <c r="B79" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="E78" s="18" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="45">
-      <c r="A79" s="35"/>
-      <c r="B79" s="36" t="s">
+      <c r="C79" s="43" t="s">
         <v>220</v>
       </c>
-      <c r="C79" s="26" t="s">
+      <c r="D79" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="D79" s="19" t="s">
+      <c r="E79" s="24" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="80" ht="45" spans="1:5">
+      <c r="A80" s="42"/>
+      <c r="B80" s="35" t="s">
         <v>222</v>
       </c>
-      <c r="E79" s="18" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="45">
-      <c r="A80" s="35"/>
-      <c r="B80" s="38"/>
-      <c r="C80" s="26" t="s">
+      <c r="C80" s="43" t="s">
         <v>223</v>
       </c>
-      <c r="D80" s="19" t="s">
+      <c r="D80" s="25" t="s">
         <v>224</v>
       </c>
-      <c r="E80" s="18" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="45">
-      <c r="A81" s="35"/>
-      <c r="B81" s="36" t="s">
+      <c r="E80" s="24" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="81" ht="45" spans="1:5">
+      <c r="A81" s="42"/>
+      <c r="B81" s="37"/>
+      <c r="C81" s="43" t="s">
         <v>225</v>
       </c>
-      <c r="C81" s="26" t="s">
+      <c r="D81" s="25" t="s">
         <v>226</v>
       </c>
-      <c r="D81" s="19" t="s">
+      <c r="E81" s="24" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="82" ht="45" spans="1:5">
+      <c r="A82" s="42"/>
+      <c r="B82" s="35" t="s">
         <v>227</v>
       </c>
-      <c r="E81" s="18" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="30">
-      <c r="A82" s="35"/>
-      <c r="B82" s="37"/>
-      <c r="C82" s="26" t="s">
+      <c r="C82" s="43" t="s">
         <v>228</v>
       </c>
-      <c r="D82" s="19" t="s">
+      <c r="D82" s="25" t="s">
         <v>229</v>
       </c>
-      <c r="E82" s="18" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="30">
-      <c r="A83" s="35"/>
-      <c r="B83" s="38"/>
-      <c r="C83" s="26" t="s">
+      <c r="E82" s="24" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="83" ht="30" spans="1:5">
+      <c r="A83" s="42"/>
+      <c r="B83" s="36"/>
+      <c r="C83" s="43" t="s">
         <v>230</v>
       </c>
-      <c r="D83" s="19" t="s">
+      <c r="D83" s="25" t="s">
         <v>231</v>
       </c>
-      <c r="E83" s="18" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="30">
-      <c r="A84" s="35"/>
-      <c r="B84" s="48" t="s">
+      <c r="E83" s="24" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="84" ht="30" spans="1:5">
+      <c r="A84" s="42"/>
+      <c r="B84" s="37"/>
+      <c r="C84" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="C84" s="26" t="s">
+      <c r="D84" s="25" t="s">
         <v>233</v>
       </c>
-      <c r="D84" s="19" t="s">
+      <c r="E84" s="24" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="85" ht="30" spans="1:5">
+      <c r="A85" s="42"/>
+      <c r="B85" s="44" t="s">
         <v>234</v>
       </c>
-      <c r="E84" s="18" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="30">
-      <c r="A85" s="35"/>
-      <c r="B85" s="49"/>
-      <c r="C85" s="26" t="s">
+      <c r="C85" s="43" t="s">
         <v>235</v>
       </c>
-      <c r="D85" s="19" t="s">
+      <c r="D85" s="25" t="s">
         <v>236</v>
       </c>
-      <c r="E85" s="18" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="69.95" customHeight="1">
-      <c r="A86" s="28" t="s">
+      <c r="E85" s="24" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="86" ht="30" spans="1:5">
+      <c r="A86" s="42"/>
+      <c r="B86" s="45"/>
+      <c r="C86" s="43" t="s">
         <v>237</v>
       </c>
-      <c r="B86" s="45" t="s">
+      <c r="D86" s="25" t="s">
         <v>238</v>
       </c>
-      <c r="C86" s="25" t="s">
+      <c r="E86" s="24" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="87" ht="69.95" customHeight="1" spans="1:5">
+      <c r="A87" s="15" t="s">
         <v>239</v>
       </c>
-      <c r="D86" s="25" t="s">
+      <c r="B87" s="38" t="s">
         <v>240</v>
       </c>
-      <c r="E86" s="15" t="s">
+      <c r="C87" s="39" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" ht="45">
-      <c r="A87" s="29"/>
-      <c r="B87" s="47"/>
-      <c r="C87" s="25" t="s">
+      <c r="D87" s="39" t="s">
         <v>242</v>
       </c>
-      <c r="D87" s="27" t="s">
+      <c r="E87" s="16" t="s">
         <v>243</v>
       </c>
-      <c r="E87" s="15" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="45">
-      <c r="A88" s="29"/>
-      <c r="B88" s="47"/>
-      <c r="C88" s="25" t="s">
+    </row>
+    <row r="88" ht="45" spans="1:5">
+      <c r="A88" s="18"/>
+      <c r="B88" s="41"/>
+      <c r="C88" s="39" t="s">
         <v>244</v>
       </c>
-      <c r="D88" s="27" t="s">
+      <c r="D88" s="46" t="s">
         <v>245</v>
       </c>
-      <c r="E88" s="15" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="30">
-      <c r="A89" s="29"/>
-      <c r="B89" s="46"/>
-      <c r="C89" s="25" t="s">
+      <c r="E88" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="89" ht="45" spans="1:5">
+      <c r="A89" s="18"/>
+      <c r="B89" s="41"/>
+      <c r="C89" s="39" t="s">
         <v>246</v>
       </c>
-      <c r="D89" s="27" t="s">
+      <c r="D89" s="46" t="s">
         <v>247</v>
       </c>
-      <c r="E89" s="15" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="50.1" customHeight="1">
-      <c r="A90" s="29"/>
-      <c r="B90" s="45" t="s">
+      <c r="E89" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="90" ht="30" spans="1:5">
+      <c r="A90" s="18"/>
+      <c r="B90" s="40"/>
+      <c r="C90" s="39" t="s">
         <v>248</v>
       </c>
-      <c r="C90" s="25" t="s">
+      <c r="D90" s="46" t="s">
         <v>249</v>
       </c>
-      <c r="D90" s="25" t="s">
+      <c r="E90" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="91" ht="50.1" customHeight="1" spans="1:5">
+      <c r="A91" s="18"/>
+      <c r="B91" s="38" t="s">
         <v>250</v>
       </c>
-      <c r="E90" s="15" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="30">
-      <c r="A91" s="29"/>
-      <c r="B91" s="47"/>
-      <c r="C91" s="25" t="s">
+      <c r="C91" s="39" t="s">
         <v>251</v>
       </c>
-      <c r="D91" s="25" t="s">
+      <c r="D91" s="39" t="s">
         <v>252</v>
       </c>
-      <c r="E91" s="15" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="63.95" customHeight="1">
-      <c r="A92" s="29"/>
-      <c r="B92" s="47" t="s">
+      <c r="E91" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="92" ht="30" spans="1:5">
+      <c r="A92" s="18"/>
+      <c r="B92" s="41"/>
+      <c r="C92" s="39" t="s">
         <v>253</v>
       </c>
-      <c r="C92" s="25" t="s">
+      <c r="D92" s="39" t="s">
         <v>254</v>
       </c>
-      <c r="D92" s="25" t="s">
+      <c r="E92" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="93" ht="63.95" customHeight="1" spans="1:5">
+      <c r="A93" s="18"/>
+      <c r="B93" s="41" t="s">
         <v>255</v>
       </c>
-      <c r="E92" s="15" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="45">
-      <c r="A93" s="29"/>
-      <c r="B93" s="47"/>
-      <c r="C93" s="50" t="s">
+      <c r="C93" s="39" t="s">
         <v>256</v>
       </c>
-      <c r="D93" s="50" t="s">
+      <c r="D93" s="39" t="s">
         <v>257</v>
       </c>
-      <c r="E93" s="17" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="33">
-      <c r="A94" s="51" t="s">
-        <v>290</v>
-      </c>
-      <c r="B94" s="53" t="s">
-        <v>288</v>
-      </c>
-      <c r="C94" s="26" t="s">
-        <v>291</v>
-      </c>
-      <c r="D94" s="52" t="s">
-        <v>295</v>
-      </c>
-      <c r="E94" s="54" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" ht="33">
-      <c r="A95" s="51"/>
-      <c r="B95" s="53"/>
-      <c r="C95" s="26" t="s">
-        <v>292</v>
-      </c>
-      <c r="D95" s="52" t="s">
-        <v>296</v>
-      </c>
-      <c r="E95" s="54" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="33">
-      <c r="A96" s="51"/>
-      <c r="B96" s="53" t="s">
-        <v>289</v>
-      </c>
-      <c r="C96" s="26" t="s">
-        <v>293</v>
-      </c>
-      <c r="D96" s="52" t="s">
-        <v>297</v>
-      </c>
-      <c r="E96" s="54" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="33">
-      <c r="A97" s="51"/>
-      <c r="B97" s="53"/>
-      <c r="C97" s="26" t="s">
-        <v>294</v>
-      </c>
-      <c r="D97" s="52" t="s">
-        <v>298</v>
-      </c>
-      <c r="E97" s="54" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" ht="30">
-      <c r="A98" s="51"/>
-      <c r="B98" s="53"/>
-      <c r="C98" s="26" t="s">
-        <v>300</v>
-      </c>
-      <c r="D98" s="24" t="s">
-        <v>299</v>
-      </c>
-      <c r="E98" s="54" t="s">
-        <v>34</v>
+      <c r="E93" s="16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="94" ht="45" spans="1:5">
+      <c r="A94" s="18"/>
+      <c r="B94" s="41"/>
+      <c r="C94" s="47" t="s">
+        <v>258</v>
+      </c>
+      <c r="D94" s="47" t="s">
+        <v>259</v>
+      </c>
+      <c r="E94" s="19" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="95" ht="33" spans="1:5">
+      <c r="A95" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="B95" s="49" t="s">
+        <v>261</v>
+      </c>
+      <c r="C95" s="43" t="s">
+        <v>262</v>
+      </c>
+      <c r="D95" s="50" t="s">
+        <v>263</v>
+      </c>
+      <c r="E95" s="48" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="96" ht="33" spans="1:5">
+      <c r="A96" s="48"/>
+      <c r="B96" s="49"/>
+      <c r="C96" s="43" t="s">
+        <v>264</v>
+      </c>
+      <c r="D96" s="50" t="s">
+        <v>265</v>
+      </c>
+      <c r="E96" s="48" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="97" ht="33" spans="1:5">
+      <c r="A97" s="48"/>
+      <c r="B97" s="49" t="s">
+        <v>266</v>
+      </c>
+      <c r="C97" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="D97" s="50" t="s">
+        <v>268</v>
+      </c>
+      <c r="E97" s="48" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" ht="33" spans="1:5">
+      <c r="A98" s="48"/>
+      <c r="B98" s="49"/>
+      <c r="C98" s="43" t="s">
+        <v>269</v>
+      </c>
+      <c r="D98" s="50" t="s">
+        <v>270</v>
+      </c>
+      <c r="E98" s="48" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="99" ht="30" spans="1:5">
+      <c r="A99" s="48"/>
+      <c r="B99" s="49"/>
+      <c r="C99" s="43" t="s">
+        <v>271</v>
+      </c>
+      <c r="D99" s="31" t="s">
+        <v>272</v>
+      </c>
+      <c r="E99" s="48" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B86:B89"/>
-    <mergeCell ref="B90:B93"/>
-    <mergeCell ref="B94:B95"/>
-    <mergeCell ref="B96:B98"/>
-    <mergeCell ref="A94:A98"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="B73:B77"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="B81:B83"/>
-    <mergeCell ref="B84:B85"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="B68:B70"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B52:B55"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A52:A63"/>
-    <mergeCell ref="A64:A72"/>
-    <mergeCell ref="A73:A85"/>
-    <mergeCell ref="A86:A93"/>
     <mergeCell ref="A2:A10"/>
-    <mergeCell ref="A11:A20"/>
-    <mergeCell ref="A21:A30"/>
-    <mergeCell ref="A32:A48"/>
+    <mergeCell ref="A11:A21"/>
+    <mergeCell ref="A22:A31"/>
+    <mergeCell ref="A33:A49"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="A53:A64"/>
+    <mergeCell ref="A65:A73"/>
+    <mergeCell ref="A74:A86"/>
+    <mergeCell ref="A87:A94"/>
+    <mergeCell ref="A95:A99"/>
+    <mergeCell ref="B11:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B53:B56"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="B69:B71"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="B74:B78"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="B82:B84"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="B87:B90"/>
+    <mergeCell ref="B91:B94"/>
+    <mergeCell ref="B95:B96"/>
+    <mergeCell ref="B97:B99"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" sqref="A32:A37"/>
+    <dataValidation allowBlank="1" sqref="A33:A38"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="20.7142857142857" customWidth="1"/>
     <col min="3" max="3" width="45" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="40.5">
+    <row r="1" ht="40.5" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>259</v>
+        <v>274</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>260</v>
+        <v>275</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="56.25">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="2" ht="37.5" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>263</v>
+        <v>278</v>
       </c>
       <c r="D2" s="5">
         <v>45760</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="56.25">
+    <row r="3" ht="56.25" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>264</v>
+        <v>279</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>265</v>
+        <v>280</v>
       </c>
       <c r="D3" s="5">
         <v>45765</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="37.5">
+    <row r="4" ht="37.5" spans="1:4">
       <c r="A4" s="3" t="s">
-        <v>266</v>
+        <v>281</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>267</v>
+        <v>282</v>
       </c>
       <c r="D4" s="5">
         <v>45766</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="75">
+    <row r="5" ht="75" spans="1:4">
       <c r="A5" s="3" t="s">
-        <v>268</v>
+        <v>283</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>269</v>
+        <v>284</v>
       </c>
       <c r="D5" s="5">
         <v>45773</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="37.5">
+    <row r="6" ht="37.5" spans="1:4">
       <c r="A6" s="3" t="s">
-        <v>270</v>
+        <v>285</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="D6" s="5">
         <v>45773</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="37.5">
+    <row r="7" ht="37.5" spans="1:4">
       <c r="A7" s="3" t="s">
-        <v>272</v>
+        <v>287</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>273</v>
+        <v>288</v>
       </c>
       <c r="D7" s="5">
         <v>45780</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="37.5">
+    <row r="8" ht="37.5" spans="1:4">
       <c r="A8" s="3" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>275</v>
+        <v>290</v>
       </c>
       <c r="D8" s="5">
         <v>45781</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="37.5">
+    <row r="9" ht="37.5" spans="1:4">
       <c r="A9" s="3" t="s">
-        <v>276</v>
+        <v>291</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>277</v>
+        <v>292</v>
       </c>
       <c r="D9" s="5">
         <v>45784</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="37.5">
+    <row r="10" ht="37.5" spans="1:4">
       <c r="A10" s="3" t="s">
-        <v>278</v>
+        <v>293</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>279</v>
+        <v>294</v>
       </c>
       <c r="D10" s="5">
         <v>45785</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="37.5">
+    <row r="11" ht="37.5" spans="1:4">
       <c r="A11" s="3" t="s">
-        <v>280</v>
+        <v>295</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>281</v>
+        <v>296</v>
       </c>
       <c r="D11" s="5">
         <v>45786</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="37.5">
+    <row r="12" ht="37.5" spans="1:4">
       <c r="A12" s="3" t="s">
-        <v>282</v>
+        <v>297</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>283</v>
+        <v>298</v>
       </c>
       <c r="D12" s="5">
         <v>45786</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="18.75">
+    <row r="13" ht="18.75" spans="1:4">
       <c r="A13" s="3" t="s">
-        <v>284</v>
+        <v>299</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>285</v>
+        <v>300</v>
       </c>
       <c r="D13" s="5">
         <v>45786</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="18.75">
+    <row r="14" ht="18.75" spans="1:4">
       <c r="A14" s="3" t="s">
-        <v>286</v>
+        <v>301</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>287</v>
+        <v>302</v>
       </c>
       <c r="D14" s="5">
         <v>45786</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="37.5">
+    <row r="15" ht="37.5" spans="1:4">
       <c r="A15" s="3" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="D15" s="5">
         <v>45787</v>
       </c>
     </row>
+    <row r="16" ht="37.5" spans="1:4">
+      <c r="A16" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="D16" s="5">
+        <v>45787</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
v3.1 Update [system constraints ID] and [USERHOME] SRS Features
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_SRS.xlsx
+++ b/LH_REQUIREMENTS/LH_SRS.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omars\Documents\GitHub\Group-3-Learning-hub\LH_REQUIREMENTS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halae\OneDrive\Desktop\Group-3-Learning-hub-dev\LH_REQUIREMENTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2F6BEE-2055-4C16-84E7-DD4D9A0D8A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="LH_SRS" sheetId="1" r:id="rId1"/>
     <sheet name="LH_SRS_VERSION_HISTORY" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="330">
   <si>
     <t>Feature</t>
   </si>
@@ -1121,16 +1120,84 @@
     <t>Send notifications to the user’s Home Page at notification section about new posts in followed categories.</t>
   </si>
   <si>
-    <t>v2.10</t>
-  </si>
-  <si>
     <t xml:space="preserve">Update on review on Registration and CATEGORIES SRS </t>
+  </si>
+  <si>
+    <t>LH-SRS-SYS-002</t>
+  </si>
+  <si>
+    <t>LH-CRS-ID-CONSTRAINS-001</t>
+  </si>
+  <si>
+    <t>LH-CRS-ID-CONSTRAINS-002</t>
+  </si>
+  <si>
+    <t>The system shall automatically assign a unique and simple user ID to each newly registered user in a consistent format (e.g., U001, U002, U003).</t>
+  </si>
+  <si>
+    <t>v3.0</t>
+  </si>
+  <si>
+    <t>v3.1</t>
+  </si>
+  <si>
+    <t>Update [system constraints ID] and [USERHOME] SRS Features</t>
+  </si>
+  <si>
+    <t>User Home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LH-CRS-USERHOME-001 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LH-SRS-USERHOME-001 </t>
+  </si>
+  <si>
+    <t>LH-SRS-USERHOME-002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system shall provide a personalized home page for each user, displaying a welcome message and the user’s username clearly at the top.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The home page shall include a “Go to Categories” button that allows users to navigate to the categories page directly.
+</t>
+  </si>
+  <si>
+    <t>LH-SRS-USERHOME-003</t>
+  </si>
+  <si>
+    <t>LH-CRS-USERHOME-002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The home page shall list posts from the categories followed by the user.
+</t>
+  </si>
+  <si>
+    <t>LH-SRS-USERHOME-004</t>
+  </si>
+  <si>
+    <t>LH-CRS-USERHOME-003</t>
+  </si>
+  <si>
+    <t>LH-SRS-USERHOME-005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system shall display a notification bell icon on the user home page, showing the current count of new notifications.
+</t>
+  </si>
+  <si>
+    <t>LH-CRS-USERHOME-004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system shall dynamically retrieve and display notifications for new posts in categories the user follows in notification section
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="15">
     <font>
       <sz val="11"/>
@@ -1238,7 +1305,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1275,8 +1342,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1336,11 +1409,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1382,121 +1490,136 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1772,24 +1895,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G99"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G108"/>
   <sheetViews>
-    <sheetView zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="91" zoomScaleNormal="111" workbookViewId="0">
+      <selection activeCell="G103" sqref="G103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="29.5546875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="53.44140625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="23.109375" style="7" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="7"/>
+    <col min="1" max="1" width="19.85546875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="53.42578125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" style="7" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.8">
+    <row r="1" spans="1:5" ht="19.5">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1806,8 +1929,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="57.6">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:5" ht="60">
+      <c r="A2" s="23" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="14" t="s">
@@ -1816,37 +1939,37 @@
       <c r="C2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>305</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="31"/>
+    <row r="3" spans="1:5" ht="30">
+      <c r="A3" s="24"/>
       <c r="B3" s="14" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.8">
-      <c r="A4" s="31"/>
+    <row r="4" spans="1:5" ht="30">
+      <c r="A4" s="24"/>
       <c r="B4" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="14" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="14" t="s">
@@ -1854,44 +1977,44 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="31"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="14" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="28.8">
-      <c r="A6" s="31"/>
+    <row r="6" spans="1:5" ht="30">
+      <c r="A6" s="24"/>
       <c r="B6" s="14" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="14" t="s">
         <v>303</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="28.8">
-      <c r="A7" s="31"/>
-      <c r="B7" s="16" t="s">
+    <row r="7" spans="1:5" ht="30">
+      <c r="A7" s="24"/>
+      <c r="B7" s="26" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="14" t="s">
         <v>304</v>
       </c>
       <c r="E7" s="14" t="s">
@@ -1899,14 +2022,14 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="31"/>
-      <c r="B8" s="16" t="s">
+      <c r="A8" s="24"/>
+      <c r="B8" s="26" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="14" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="14" t="s">
@@ -1914,14 +2037,14 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="31"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="14" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="14" t="s">
         <v>302</v>
       </c>
       <c r="E9" s="14" t="s">
@@ -1929,44 +2052,44 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="31"/>
-      <c r="B10" s="16" t="s">
+      <c r="A10" s="24"/>
+      <c r="B10" s="26" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="14" t="s">
         <v>29</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28.8">
-      <c r="A11" s="30" t="s">
+    <row r="11" spans="1:5" ht="30">
+      <c r="A11" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="27" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="14" t="s">
         <v>33</v>
       </c>
       <c r="E11" s="14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="28.8">
-      <c r="A12" s="31"/>
-      <c r="B12" s="39"/>
+    <row r="12" spans="1:5" ht="30">
+      <c r="A12" s="24"/>
+      <c r="B12" s="28"/>
       <c r="C12" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="14" t="s">
         <v>36</v>
       </c>
       <c r="E12" s="14" t="s">
@@ -1974,12 +2097,12 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="28.5" customHeight="1">
-      <c r="A13" s="31"/>
-      <c r="B13" s="39"/>
+      <c r="A13" s="24"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="14" t="s">
         <v>38</v>
       </c>
       <c r="E13" s="14" t="s">
@@ -1987,267 +2110,267 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="28.5" customHeight="1">
-      <c r="A14" s="31"/>
-      <c r="B14" s="39"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="14" t="s">
         <v>40</v>
       </c>
       <c r="E14" s="14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="28.8">
-      <c r="A15" s="31"/>
-      <c r="B15" s="39"/>
+    <row r="15" spans="1:5" ht="30">
+      <c r="A15" s="24"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="14" t="s">
         <v>42</v>
       </c>
       <c r="E15" s="14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="28.8">
-      <c r="A16" s="31"/>
-      <c r="B16" s="40"/>
+    <row r="16" spans="1:5" ht="30">
+      <c r="A16" s="24"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="14" t="s">
         <v>44</v>
       </c>
       <c r="E16" s="14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="43.2">
-      <c r="A17" s="31"/>
-      <c r="B17" s="38" t="s">
+    <row r="17" spans="1:7" ht="45">
+      <c r="A17" s="24"/>
+      <c r="B17" s="27" t="s">
         <v>45</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="14" t="s">
         <v>47</v>
       </c>
       <c r="E17" s="14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="28.8">
-      <c r="A18" s="31"/>
-      <c r="B18" s="40"/>
+    <row r="18" spans="1:7" ht="30">
+      <c r="A18" s="24"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="14" t="s">
         <v>49</v>
       </c>
       <c r="E18" s="14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="28.8">
-      <c r="A19" s="31"/>
-      <c r="B19" s="38" t="s">
+    <row r="19" spans="1:7" ht="30">
+      <c r="A19" s="24"/>
+      <c r="B19" s="27" t="s">
         <v>50</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="14" t="s">
         <v>52</v>
       </c>
       <c r="E19" s="14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="28.8">
-      <c r="A20" s="31"/>
-      <c r="B20" s="39"/>
+    <row r="20" spans="1:7" ht="30">
+      <c r="A20" s="24"/>
+      <c r="B20" s="28"/>
       <c r="C20" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="14" t="s">
         <v>54</v>
       </c>
       <c r="E20" s="14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="28.8">
-      <c r="A21" s="32"/>
-      <c r="B21" s="40"/>
+    <row r="21" spans="1:7" ht="30">
+      <c r="A21" s="25"/>
+      <c r="B21" s="29"/>
       <c r="C21" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E21" s="14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="28.8">
-      <c r="A22" s="33" t="s">
+    <row r="22" spans="1:7" ht="30">
+      <c r="A22" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="E22" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="28.8">
-      <c r="A23" s="34"/>
-      <c r="B23" s="17" t="s">
+    <row r="23" spans="1:7" ht="30">
+      <c r="A23" s="31"/>
+      <c r="B23" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="E23" s="15" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="34"/>
-      <c r="B24" s="17" t="s">
+      <c r="A24" s="31"/>
+      <c r="B24" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="E24" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="28.8">
-      <c r="A25" s="34"/>
-      <c r="B25" s="17" t="s">
+    <row r="25" spans="1:7" ht="30">
+      <c r="A25" s="31"/>
+      <c r="B25" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="D25" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="E25" s="17" t="s">
+      <c r="E25" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="28.8">
-      <c r="A26" s="34"/>
-      <c r="B26" s="17" t="s">
+    <row r="26" spans="1:7" ht="30">
+      <c r="A26" s="31"/>
+      <c r="B26" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="D26" s="18" t="s">
+      <c r="D26" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="E26" s="17" t="s">
+      <c r="E26" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="28.8">
-      <c r="A27" s="34"/>
-      <c r="B27" s="17" t="s">
+    <row r="27" spans="1:7" ht="30">
+      <c r="A27" s="31"/>
+      <c r="B27" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="E27" s="17" t="s">
+      <c r="E27" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="28.8">
-      <c r="A28" s="34"/>
-      <c r="B28" s="17" t="s">
+    <row r="28" spans="1:7" ht="45">
+      <c r="A28" s="31"/>
+      <c r="B28" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="D28" s="18" t="s">
+      <c r="D28" s="15" t="s">
         <v>306</v>
       </c>
-      <c r="E28" s="17" t="s">
+      <c r="E28" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="28.8">
-      <c r="A29" s="34"/>
-      <c r="B29" s="17" t="s">
+    <row r="29" spans="1:7" ht="30">
+      <c r="A29" s="31"/>
+      <c r="B29" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="D29" s="18" t="s">
+      <c r="D29" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="E29" s="17" t="s">
+      <c r="E29" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="28.8">
-      <c r="A30" s="34"/>
-      <c r="B30" s="17" t="s">
+    <row r="30" spans="1:7" ht="30">
+      <c r="A30" s="31"/>
+      <c r="B30" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="D30" s="18" t="s">
+      <c r="D30" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="E30" s="17" t="s">
+      <c r="E30" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="28.8">
-      <c r="A31" s="35"/>
-      <c r="B31" s="17" t="s">
+    <row r="31" spans="1:7" ht="30">
+      <c r="A31" s="32"/>
+      <c r="B31" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="D31" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="28.8">
-      <c r="A32" s="19" t="s">
+    <row r="32" spans="1:7" ht="30">
+      <c r="A32" s="23" t="s">
         <v>87</v>
       </c>
       <c r="B32" s="14" t="s">
@@ -2256,1006 +2379,1125 @@
       <c r="C32" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="14" t="s">
         <v>90</v>
       </c>
       <c r="E32" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-    </row>
-    <row r="33" spans="1:5" ht="30" customHeight="1">
-      <c r="A33" s="33" t="s">
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+    </row>
+    <row r="33" spans="1:7" ht="30" customHeight="1">
+      <c r="A33" s="24"/>
+      <c r="B33" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C33" s="27" t="s">
+        <v>308</v>
+      </c>
+      <c r="D33" s="27" t="s">
+        <v>311</v>
+      </c>
+      <c r="E33" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+    </row>
+    <row r="34" spans="1:7" ht="75" customHeight="1">
+      <c r="A34" s="25"/>
+      <c r="B34" s="14" t="s">
+        <v>310</v>
+      </c>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+    </row>
+    <row r="35" spans="1:7" ht="30" customHeight="1">
+      <c r="A35" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="B33" s="41" t="s">
+      <c r="B35" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="C33" s="22" t="s">
+      <c r="C35" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="D33" s="22" t="s">
+      <c r="D35" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="E33" s="17" t="s">
+      <c r="E35" s="15" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="30" customHeight="1">
-      <c r="A34" s="34"/>
-      <c r="B34" s="41"/>
-      <c r="C34" s="22" t="s">
+    <row r="36" spans="1:7" ht="30" customHeight="1">
+      <c r="A36" s="31"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="D34" s="22" t="s">
+      <c r="D36" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="E34" s="17" t="s">
+      <c r="E36" s="15" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="30" customHeight="1">
-      <c r="A35" s="34"/>
-      <c r="B35" s="41" t="s">
+    <row r="37" spans="1:7" ht="30" customHeight="1">
+      <c r="A37" s="31"/>
+      <c r="B37" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="C35" s="22" t="s">
+      <c r="C37" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="D35" s="22" t="s">
+      <c r="D37" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="E35" s="17" t="s">
+      <c r="E37" s="15" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="30" customHeight="1">
-      <c r="A36" s="34"/>
-      <c r="B36" s="41"/>
-      <c r="C36" s="22" t="s">
+    <row r="38" spans="1:7" ht="30" customHeight="1">
+      <c r="A38" s="31"/>
+      <c r="B38" s="33"/>
+      <c r="C38" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="D36" s="22" t="s">
+      <c r="D38" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="E36" s="17" t="s">
+      <c r="E38" s="15" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="30" customHeight="1">
-      <c r="A37" s="34"/>
-      <c r="B37" s="21" t="s">
+    <row r="39" spans="1:7" ht="30" customHeight="1">
+      <c r="A39" s="31"/>
+      <c r="B39" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="C37" s="22" t="s">
+      <c r="C39" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="D37" s="22" t="s">
+      <c r="D39" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="E37" s="17" t="s">
+      <c r="E39" s="15" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="30" customHeight="1">
-      <c r="A38" s="34"/>
-      <c r="B38" s="21" t="s">
+    <row r="40" spans="1:7" ht="30" customHeight="1">
+      <c r="A40" s="31"/>
+      <c r="B40" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="C38" s="22" t="s">
+      <c r="C40" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="D38" s="22" t="s">
+      <c r="D40" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="E38" s="17" t="s">
+      <c r="E40" s="15" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="28.8">
-      <c r="A39" s="34"/>
-      <c r="B39" s="21" t="s">
+    <row r="41" spans="1:7" ht="30">
+      <c r="A41" s="31"/>
+      <c r="B41" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="C39" s="22" t="s">
+      <c r="C41" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="D39" s="22" t="s">
+      <c r="D41" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="E39" s="17" t="s">
+      <c r="E41" s="15" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="28.8">
-      <c r="A40" s="34"/>
-      <c r="B40" s="42" t="s">
+    <row r="42" spans="1:7" ht="30">
+      <c r="A42" s="31"/>
+      <c r="B42" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="C40" s="22" t="s">
+      <c r="C42" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="D40" s="22" t="s">
+      <c r="D42" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="E40" s="17" t="s">
+      <c r="E42" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="28.8">
-      <c r="A41" s="34"/>
-      <c r="B41" s="43"/>
-      <c r="C41" s="22" t="s">
+    <row r="43" spans="1:7" ht="45">
+      <c r="A43" s="31"/>
+      <c r="B43" s="36"/>
+      <c r="C43" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="D41" s="22" t="s">
+      <c r="D43" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="E41" s="17" t="s">
+      <c r="E43" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="28.8">
-      <c r="A42" s="34"/>
-      <c r="B42" s="42" t="s">
+    <row r="44" spans="1:7" ht="30">
+      <c r="A44" s="31"/>
+      <c r="B44" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="C42" s="22" t="s">
+      <c r="C44" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="D42" s="22" t="s">
+      <c r="D44" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="E42" s="17" t="s">
+      <c r="E44" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="28.8">
-      <c r="A43" s="34"/>
-      <c r="B43" s="43"/>
-      <c r="C43" s="22" t="s">
+    <row r="45" spans="1:7" ht="30">
+      <c r="A45" s="31"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="D43" s="22" t="s">
+      <c r="D45" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="E43" s="17" t="s">
+      <c r="E45" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="28.8">
-      <c r="A44" s="34"/>
-      <c r="B44" s="21" t="s">
+    <row r="46" spans="1:7" ht="30">
+      <c r="A46" s="31"/>
+      <c r="B46" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="C44" s="22" t="s">
+      <c r="C46" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="D44" s="22" t="s">
+      <c r="D46" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="E44" s="17" t="s">
+      <c r="E46" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="28.8">
-      <c r="A45" s="34"/>
-      <c r="B45" s="21" t="s">
+    <row r="47" spans="1:7" ht="30">
+      <c r="A47" s="31"/>
+      <c r="B47" s="34" t="s">
         <v>125</v>
       </c>
-      <c r="C45" s="22" t="s">
+      <c r="C47" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="D45" s="22" t="s">
+      <c r="D47" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="E45" s="17" t="s">
+      <c r="E47" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="28.8">
-      <c r="A46" s="34"/>
-      <c r="B46" s="21" t="s">
+    <row r="48" spans="1:7" ht="30">
+      <c r="A48" s="31"/>
+      <c r="B48" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="C46" s="22" t="s">
+      <c r="C48" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="D46" s="22" t="s">
+      <c r="D48" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="E46" s="17" t="s">
+      <c r="E48" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="28.8">
-      <c r="A47" s="34"/>
-      <c r="B47" s="21" t="s">
+    <row r="49" spans="1:5" ht="30">
+      <c r="A49" s="31"/>
+      <c r="B49" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="C47" s="22" t="s">
+      <c r="C49" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="D47" s="22" t="s">
+      <c r="D49" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="E47" s="21" t="s">
+      <c r="E49" s="34" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="28.8">
-      <c r="A48" s="34"/>
-      <c r="B48" s="42" t="s">
+    <row r="50" spans="1:5" ht="45">
+      <c r="A50" s="31"/>
+      <c r="B50" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="C48" s="22" t="s">
+      <c r="C50" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="D48" s="22" t="s">
+      <c r="D50" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="E48" s="21" t="s">
+      <c r="E50" s="34" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="57.6">
-      <c r="A49" s="34"/>
-      <c r="B49" s="43"/>
-      <c r="C49" s="22" t="s">
+    <row r="51" spans="1:5" ht="60">
+      <c r="A51" s="31"/>
+      <c r="B51" s="36"/>
+      <c r="C51" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="D49" s="22" t="s">
+      <c r="D51" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="E49" s="21" t="s">
+      <c r="E51" s="34" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="28.8">
-      <c r="A50" s="30" t="s">
+    <row r="52" spans="1:5" ht="45">
+      <c r="A52" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="B50" s="14" t="s">
+      <c r="B52" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="C50" s="14" t="s">
+      <c r="C52" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="D50" s="15" t="s">
+      <c r="D52" s="14" t="s">
         <v>142</v>
-      </c>
-      <c r="E50" s="14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="28.8">
-      <c r="A51" s="31"/>
-      <c r="B51" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="C51" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="D51" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="E51" s="14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="28.8">
-      <c r="A52" s="31"/>
-      <c r="B52" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="C52" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="D52" s="15" t="s">
-        <v>148</v>
       </c>
       <c r="E52" s="14" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="28.8">
-      <c r="A53" s="33" t="s">
+    <row r="53" spans="1:5" ht="30">
+      <c r="A53" s="24"/>
+      <c r="B53" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="30">
+      <c r="A54" s="24"/>
+      <c r="B54" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="E54" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="30">
+      <c r="A55" s="30" t="s">
         <v>149</v>
       </c>
-      <c r="B53" s="44" t="s">
+      <c r="B55" s="37" t="s">
         <v>150</v>
       </c>
-      <c r="C53" s="17" t="s">
+      <c r="C55" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="D53" s="18" t="s">
+      <c r="D55" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="E53" s="17" t="s">
+      <c r="E55" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="28.8">
-      <c r="A54" s="34"/>
-      <c r="B54" s="45"/>
-      <c r="C54" s="17" t="s">
+    <row r="56" spans="1:5" ht="30">
+      <c r="A56" s="31"/>
+      <c r="B56" s="38"/>
+      <c r="C56" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="D54" s="18" t="s">
+      <c r="D56" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="E54" s="17" t="s">
+      <c r="E56" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="28.8">
-      <c r="A55" s="34"/>
-      <c r="B55" s="45"/>
-      <c r="C55" s="17" t="s">
+    <row r="57" spans="1:5" ht="30">
+      <c r="A57" s="31"/>
+      <c r="B57" s="38"/>
+      <c r="C57" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="D55" s="18" t="s">
+      <c r="D57" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="E55" s="17" t="s">
+      <c r="E57" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="28.8">
-      <c r="A56" s="34"/>
-      <c r="B56" s="46"/>
-      <c r="C56" s="17" t="s">
+    <row r="58" spans="1:5" ht="30">
+      <c r="A58" s="31"/>
+      <c r="B58" s="39"/>
+      <c r="C58" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="D56" s="18" t="s">
+      <c r="D58" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="E56" s="17" t="s">
+      <c r="E58" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="28.8">
-      <c r="A57" s="34"/>
-      <c r="B57" s="44" t="s">
+    <row r="59" spans="1:5" ht="30">
+      <c r="A59" s="31"/>
+      <c r="B59" s="37" t="s">
         <v>159</v>
       </c>
-      <c r="C57" s="17" t="s">
+      <c r="C59" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="D57" s="18" t="s">
+      <c r="D59" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="E57" s="17" t="s">
+      <c r="E59" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="28.8">
-      <c r="A58" s="34"/>
-      <c r="B58" s="45"/>
-      <c r="C58" s="17" t="s">
+    <row r="60" spans="1:5" ht="45">
+      <c r="A60" s="31"/>
+      <c r="B60" s="38"/>
+      <c r="C60" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="D58" s="18" t="s">
+      <c r="D60" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="E58" s="17" t="s">
+      <c r="E60" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="43.2">
-      <c r="A59" s="34"/>
-      <c r="B59" s="45"/>
-      <c r="C59" s="17" t="s">
+    <row r="61" spans="1:5" ht="45">
+      <c r="A61" s="31"/>
+      <c r="B61" s="38"/>
+      <c r="C61" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="D59" s="18" t="s">
+      <c r="D61" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="E59" s="17" t="s">
+      <c r="E61" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="28.8">
-      <c r="A60" s="34"/>
-      <c r="B60" s="46"/>
-      <c r="C60" s="17" t="s">
+    <row r="62" spans="1:5" ht="45">
+      <c r="A62" s="31"/>
+      <c r="B62" s="39"/>
+      <c r="C62" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="D60" s="18" t="s">
+      <c r="D62" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="E60" s="17" t="s">
+      <c r="E62" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="28.8">
-      <c r="A61" s="34"/>
-      <c r="B61" s="23" t="s">
+    <row r="63" spans="1:5" ht="45">
+      <c r="A63" s="31"/>
+      <c r="B63" s="40" t="s">
         <v>168</v>
       </c>
-      <c r="C61" s="17" t="s">
+      <c r="C63" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="D61" s="18" t="s">
+      <c r="D63" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="E61" s="17" t="s">
+      <c r="E63" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="43.2">
-      <c r="A62" s="34"/>
-      <c r="B62" s="23" t="s">
+    <row r="64" spans="1:5" ht="45">
+      <c r="A64" s="31"/>
+      <c r="B64" s="40" t="s">
         <v>171</v>
       </c>
-      <c r="C62" s="17" t="s">
+      <c r="C64" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="D62" s="18" t="s">
+      <c r="D64" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="E62" s="17" t="s">
+      <c r="E64" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="28.8">
-      <c r="A63" s="34"/>
-      <c r="B63" s="44" t="s">
+    <row r="65" spans="1:5" ht="30">
+      <c r="A65" s="31"/>
+      <c r="B65" s="37" t="s">
         <v>174</v>
       </c>
-      <c r="C63" s="17" t="s">
+      <c r="C65" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="D63" s="18" t="s">
+      <c r="D65" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="E63" s="17" t="s">
+      <c r="E65" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="43.2">
-      <c r="A64" s="35"/>
-      <c r="B64" s="46"/>
-      <c r="C64" s="17" t="s">
+    <row r="66" spans="1:5" ht="45">
+      <c r="A66" s="32"/>
+      <c r="B66" s="39"/>
+      <c r="C66" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="D64" s="18" t="s">
+      <c r="D66" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="E64" s="17" t="s">
+      <c r="E66" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="28.8">
-      <c r="A65" s="30" t="s">
+    <row r="67" spans="1:5" ht="30">
+      <c r="A67" s="23" t="s">
         <v>179</v>
       </c>
-      <c r="B65" s="47" t="s">
+      <c r="B67" s="41" t="s">
         <v>180</v>
       </c>
-      <c r="C65" s="24" t="s">
+      <c r="C67" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="D65" s="24" t="s">
+      <c r="D67" s="14" t="s">
         <v>182</v>
-      </c>
-      <c r="E65" s="14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="28.8">
-      <c r="A66" s="31"/>
-      <c r="B66" s="48"/>
-      <c r="C66" s="24" t="s">
-        <v>183</v>
-      </c>
-      <c r="D66" s="24" t="s">
-        <v>184</v>
-      </c>
-      <c r="E66" s="14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="28.8">
-      <c r="A67" s="31"/>
-      <c r="B67" s="47" t="s">
-        <v>185</v>
-      </c>
-      <c r="C67" s="24" t="s">
-        <v>186</v>
-      </c>
-      <c r="D67" s="24" t="s">
-        <v>187</v>
       </c>
       <c r="E67" s="14" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="28.8">
-      <c r="A68" s="31"/>
-      <c r="B68" s="48"/>
-      <c r="C68" s="24" t="s">
-        <v>188</v>
-      </c>
-      <c r="D68" s="24" t="s">
-        <v>189</v>
+    <row r="68" spans="1:5" ht="30">
+      <c r="A68" s="24"/>
+      <c r="B68" s="42"/>
+      <c r="C68" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="D68" s="14" t="s">
+        <v>184</v>
       </c>
       <c r="E68" s="14" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="28.8">
-      <c r="A69" s="31"/>
-      <c r="B69" s="47" t="s">
-        <v>190</v>
-      </c>
-      <c r="C69" s="24" t="s">
-        <v>191</v>
-      </c>
-      <c r="D69" s="24" t="s">
-        <v>192</v>
+    <row r="69" spans="1:5" ht="30">
+      <c r="A69" s="24"/>
+      <c r="B69" s="41" t="s">
+        <v>185</v>
+      </c>
+      <c r="C69" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="D69" s="14" t="s">
+        <v>187</v>
       </c>
       <c r="E69" s="14" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="28.8">
-      <c r="A70" s="31"/>
-      <c r="B70" s="49"/>
-      <c r="C70" s="24" t="s">
-        <v>193</v>
-      </c>
-      <c r="D70" s="24" t="s">
-        <v>194</v>
+    <row r="70" spans="1:5" ht="30">
+      <c r="A70" s="24"/>
+      <c r="B70" s="42"/>
+      <c r="C70" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="D70" s="14" t="s">
+        <v>189</v>
       </c>
       <c r="E70" s="14" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="28.8">
-      <c r="A71" s="31"/>
-      <c r="B71" s="49"/>
-      <c r="C71" s="24" t="s">
-        <v>195</v>
-      </c>
-      <c r="D71" s="24" t="s">
-        <v>196</v>
+    <row r="71" spans="1:5" ht="30">
+      <c r="A71" s="24"/>
+      <c r="B71" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="C71" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D71" s="14" t="s">
+        <v>192</v>
       </c>
       <c r="E71" s="14" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="28.8">
-      <c r="A72" s="31"/>
-      <c r="B72" s="47" t="s">
-        <v>197</v>
-      </c>
-      <c r="C72" s="24" t="s">
-        <v>198</v>
-      </c>
-      <c r="D72" s="24" t="s">
-        <v>199</v>
+    <row r="72" spans="1:5" ht="30">
+      <c r="A72" s="24"/>
+      <c r="B72" s="43"/>
+      <c r="C72" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="D72" s="14" t="s">
+        <v>194</v>
       </c>
       <c r="E72" s="14" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="28.8">
-      <c r="A73" s="31"/>
-      <c r="B73" s="48"/>
-      <c r="C73" s="24" t="s">
-        <v>200</v>
-      </c>
-      <c r="D73" s="24" t="s">
-        <v>201</v>
+    <row r="73" spans="1:5" ht="30">
+      <c r="A73" s="24"/>
+      <c r="B73" s="43"/>
+      <c r="C73" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="D73" s="14" t="s">
+        <v>196</v>
       </c>
       <c r="E73" s="14" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="28.8">
-      <c r="A74" s="36" t="s">
+    <row r="74" spans="1:5" ht="30">
+      <c r="A74" s="24"/>
+      <c r="B74" s="41" t="s">
+        <v>197</v>
+      </c>
+      <c r="C74" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="D74" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="E74" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="45">
+      <c r="A75" s="24"/>
+      <c r="B75" s="42"/>
+      <c r="C75" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="D75" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="E75" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="30">
+      <c r="A76" s="44" t="s">
         <v>202</v>
       </c>
-      <c r="B74" s="44" t="s">
+      <c r="B76" s="37" t="s">
         <v>203</v>
       </c>
-      <c r="C74" s="25" t="s">
+      <c r="C76" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="D74" s="18" t="s">
+      <c r="D76" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="E74" s="17" t="s">
+      <c r="E76" s="15" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="28.8">
-      <c r="A75" s="36"/>
-      <c r="B75" s="45"/>
-      <c r="C75" s="25" t="s">
+    <row r="77" spans="1:5" ht="30">
+      <c r="A77" s="44"/>
+      <c r="B77" s="38"/>
+      <c r="C77" s="22" t="s">
         <v>207</v>
       </c>
-      <c r="D75" s="18" t="s">
+      <c r="D77" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="E75" s="17" t="s">
+      <c r="E77" s="15" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="28.8">
-      <c r="A76" s="36"/>
-      <c r="B76" s="45"/>
-      <c r="C76" s="25" t="s">
+    <row r="78" spans="1:5" ht="30">
+      <c r="A78" s="44"/>
+      <c r="B78" s="38"/>
+      <c r="C78" s="22" t="s">
         <v>208</v>
       </c>
-      <c r="D76" s="18" t="s">
+      <c r="D78" s="15" t="s">
         <v>209</v>
       </c>
-      <c r="E76" s="17" t="s">
+      <c r="E78" s="15" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="28.8">
-      <c r="A77" s="36"/>
-      <c r="B77" s="45"/>
-      <c r="C77" s="25" t="s">
+    <row r="79" spans="1:5" ht="30">
+      <c r="A79" s="44"/>
+      <c r="B79" s="38"/>
+      <c r="C79" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="D77" s="18" t="s">
+      <c r="D79" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="E77" s="17" t="s">
+      <c r="E79" s="15" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="43.2">
-      <c r="A78" s="36"/>
-      <c r="B78" s="45"/>
-      <c r="C78" s="25" t="s">
+    <row r="80" spans="1:5" ht="45">
+      <c r="A80" s="44"/>
+      <c r="B80" s="38"/>
+      <c r="C80" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="D78" s="18" t="s">
+      <c r="D80" s="15" t="s">
         <v>213</v>
       </c>
-      <c r="E78" s="17" t="s">
+      <c r="E80" s="15" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="43.2">
-      <c r="A79" s="36"/>
-      <c r="B79" s="17" t="s">
+    <row r="81" spans="1:5" ht="45">
+      <c r="A81" s="44"/>
+      <c r="B81" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="C79" s="25" t="s">
+      <c r="C81" s="22" t="s">
         <v>215</v>
       </c>
-      <c r="D79" s="18" t="s">
+      <c r="D81" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="E79" s="17" t="s">
+      <c r="E81" s="15" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="43.2">
-      <c r="A80" s="36"/>
-      <c r="B80" s="44" t="s">
+    <row r="82" spans="1:5" ht="45">
+      <c r="A82" s="44"/>
+      <c r="B82" s="37" t="s">
         <v>217</v>
       </c>
-      <c r="C80" s="25" t="s">
+      <c r="C82" s="22" t="s">
         <v>218</v>
       </c>
-      <c r="D80" s="18" t="s">
+      <c r="D82" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="E80" s="17" t="s">
+      <c r="E82" s="15" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="43.2">
-      <c r="A81" s="36"/>
-      <c r="B81" s="46"/>
-      <c r="C81" s="25" t="s">
+    <row r="83" spans="1:5" ht="45">
+      <c r="A83" s="44"/>
+      <c r="B83" s="39"/>
+      <c r="C83" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="D81" s="18" t="s">
+      <c r="D83" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="E81" s="17" t="s">
+      <c r="E83" s="15" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="43.2">
-      <c r="A82" s="36"/>
-      <c r="B82" s="44" t="s">
+    <row r="84" spans="1:5" ht="45">
+      <c r="A84" s="44"/>
+      <c r="B84" s="37" t="s">
         <v>222</v>
       </c>
-      <c r="C82" s="25" t="s">
+      <c r="C84" s="22" t="s">
         <v>223</v>
       </c>
-      <c r="D82" s="18" t="s">
+      <c r="D84" s="15" t="s">
         <v>224</v>
       </c>
-      <c r="E82" s="17" t="s">
+      <c r="E84" s="15" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
-      <c r="A83" s="36"/>
-      <c r="B83" s="45"/>
-      <c r="C83" s="25" t="s">
+    <row r="85" spans="1:5" ht="30">
+      <c r="A85" s="44"/>
+      <c r="B85" s="38"/>
+      <c r="C85" s="22" t="s">
         <v>225</v>
       </c>
-      <c r="D83" s="18" t="s">
+      <c r="D85" s="15" t="s">
         <v>226</v>
       </c>
-      <c r="E83" s="17" t="s">
+      <c r="E85" s="15" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="28.8">
-      <c r="A84" s="36"/>
-      <c r="B84" s="46"/>
-      <c r="C84" s="25" t="s">
+    <row r="86" spans="1:5" ht="30">
+      <c r="A86" s="44"/>
+      <c r="B86" s="39"/>
+      <c r="C86" s="22" t="s">
         <v>227</v>
       </c>
-      <c r="D84" s="18" t="s">
+      <c r="D86" s="15" t="s">
         <v>228</v>
       </c>
-      <c r="E84" s="17" t="s">
+      <c r="E86" s="15" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="28.8">
-      <c r="A85" s="36"/>
-      <c r="B85" s="50" t="s">
+    <row r="87" spans="1:5" ht="30">
+      <c r="A87" s="44"/>
+      <c r="B87" s="45" t="s">
         <v>229</v>
       </c>
-      <c r="C85" s="25" t="s">
+      <c r="C87" s="22" t="s">
         <v>230</v>
       </c>
-      <c r="D85" s="18" t="s">
+      <c r="D87" s="15" t="s">
         <v>231</v>
       </c>
-      <c r="E85" s="17" t="s">
+      <c r="E87" s="15" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="28.8">
-      <c r="A86" s="36"/>
-      <c r="B86" s="51"/>
-      <c r="C86" s="25" t="s">
+    <row r="88" spans="1:5" ht="30">
+      <c r="A88" s="44"/>
+      <c r="B88" s="46"/>
+      <c r="C88" s="22" t="s">
         <v>232</v>
       </c>
-      <c r="D86" s="18" t="s">
+      <c r="D88" s="15" t="s">
         <v>233</v>
       </c>
-      <c r="E86" s="17" t="s">
+      <c r="E88" s="15" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="69.900000000000006" customHeight="1">
-      <c r="A87" s="30" t="s">
+    <row r="89" spans="1:5" ht="69.95" customHeight="1">
+      <c r="A89" s="23" t="s">
         <v>234</v>
       </c>
-      <c r="B87" s="47" t="s">
+      <c r="B89" s="41" t="s">
         <v>235</v>
       </c>
-      <c r="C87" s="24" t="s">
+      <c r="C89" s="14" t="s">
         <v>236</v>
       </c>
-      <c r="D87" s="24" t="s">
+      <c r="D89" s="14" t="s">
         <v>237</v>
-      </c>
-      <c r="E87" s="14" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="43.2">
-      <c r="A88" s="31"/>
-      <c r="B88" s="49"/>
-      <c r="C88" s="24" t="s">
-        <v>239</v>
-      </c>
-      <c r="D88" s="26" t="s">
-        <v>240</v>
-      </c>
-      <c r="E88" s="14" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="43.2">
-      <c r="A89" s="31"/>
-      <c r="B89" s="49"/>
-      <c r="C89" s="24" t="s">
-        <v>241</v>
-      </c>
-      <c r="D89" s="26" t="s">
-        <v>242</v>
       </c>
       <c r="E89" s="14" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="28.8">
-      <c r="A90" s="31"/>
-      <c r="B90" s="48"/>
-      <c r="C90" s="24" t="s">
-        <v>243</v>
-      </c>
-      <c r="D90" s="26" t="s">
-        <v>244</v>
+    <row r="90" spans="1:5" ht="45">
+      <c r="A90" s="24"/>
+      <c r="B90" s="43"/>
+      <c r="C90" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="D90" s="21" t="s">
+        <v>240</v>
       </c>
       <c r="E90" s="14" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="50.1" customHeight="1">
-      <c r="A91" s="31"/>
-      <c r="B91" s="47" t="s">
-        <v>245</v>
-      </c>
-      <c r="C91" s="24" t="s">
-        <v>246</v>
-      </c>
-      <c r="D91" s="24" t="s">
-        <v>247</v>
+    <row r="91" spans="1:5" ht="45">
+      <c r="A91" s="24"/>
+      <c r="B91" s="43"/>
+      <c r="C91" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="D91" s="21" t="s">
+        <v>242</v>
       </c>
       <c r="E91" s="14" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="28.8">
-      <c r="A92" s="31"/>
-      <c r="B92" s="49"/>
-      <c r="C92" s="24" t="s">
-        <v>248</v>
-      </c>
-      <c r="D92" s="24" t="s">
-        <v>249</v>
+    <row r="92" spans="1:5" ht="30">
+      <c r="A92" s="24"/>
+      <c r="B92" s="42"/>
+      <c r="C92" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="D92" s="21" t="s">
+        <v>244</v>
       </c>
       <c r="E92" s="14" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="63.9" customHeight="1">
-      <c r="A93" s="31"/>
-      <c r="B93" s="49" t="s">
-        <v>250</v>
-      </c>
-      <c r="C93" s="24" t="s">
-        <v>251</v>
-      </c>
-      <c r="D93" s="24" t="s">
-        <v>252</v>
+    <row r="93" spans="1:5" ht="50.1" customHeight="1">
+      <c r="A93" s="24"/>
+      <c r="B93" s="41" t="s">
+        <v>245</v>
+      </c>
+      <c r="C93" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="D93" s="14" t="s">
+        <v>247</v>
       </c>
       <c r="E93" s="14" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="43.2">
-      <c r="A94" s="31"/>
-      <c r="B94" s="49"/>
-      <c r="C94" s="27" t="s">
+    <row r="94" spans="1:5" ht="30">
+      <c r="A94" s="24"/>
+      <c r="B94" s="43"/>
+      <c r="C94" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="D94" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="E94" s="14" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="63.95" customHeight="1">
+      <c r="A95" s="24"/>
+      <c r="B95" s="43" t="s">
+        <v>250</v>
+      </c>
+      <c r="C95" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="D95" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="E95" s="14" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="45">
+      <c r="A96" s="24"/>
+      <c r="B96" s="43"/>
+      <c r="C96" s="26" t="s">
         <v>253</v>
       </c>
-      <c r="D94" s="27" t="s">
+      <c r="D96" s="26" t="s">
         <v>254</v>
       </c>
-      <c r="E94" s="16" t="s">
+      <c r="E96" s="26" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="33.6">
-      <c r="A95" s="37" t="s">
+    <row r="97" spans="1:5" ht="33">
+      <c r="A97" s="47" t="s">
         <v>255</v>
       </c>
-      <c r="B95" s="52" t="s">
+      <c r="B97" s="48" t="s">
         <v>256</v>
       </c>
-      <c r="C95" s="25" t="s">
+      <c r="C97" s="22" t="s">
         <v>257</v>
       </c>
-      <c r="D95" s="29" t="s">
+      <c r="D97" s="49" t="s">
         <v>258</v>
       </c>
-      <c r="E95" s="28" t="s">
+      <c r="E97" s="17" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="33.6">
-      <c r="A96" s="37"/>
-      <c r="B96" s="52"/>
-      <c r="C96" s="25" t="s">
+    <row r="98" spans="1:5" ht="33">
+      <c r="A98" s="47"/>
+      <c r="B98" s="48"/>
+      <c r="C98" s="22" t="s">
         <v>259</v>
       </c>
-      <c r="D96" s="29" t="s">
+      <c r="D98" s="49" t="s">
         <v>260</v>
       </c>
-      <c r="E96" s="28" t="s">
+      <c r="E98" s="17" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="33.6">
-      <c r="A97" s="37"/>
-      <c r="B97" s="52" t="s">
+    <row r="99" spans="1:5" ht="33">
+      <c r="A99" s="47"/>
+      <c r="B99" s="48" t="s">
         <v>261</v>
       </c>
-      <c r="C97" s="25" t="s">
+      <c r="C99" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="D97" s="29" t="s">
+      <c r="D99" s="49" t="s">
         <v>263</v>
       </c>
-      <c r="E97" s="28" t="s">
+      <c r="E99" s="17" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="33.6">
-      <c r="A98" s="37"/>
-      <c r="B98" s="52"/>
-      <c r="C98" s="25" t="s">
+    <row r="100" spans="1:5" ht="33">
+      <c r="A100" s="47"/>
+      <c r="B100" s="48"/>
+      <c r="C100" s="22" t="s">
         <v>264</v>
       </c>
-      <c r="D98" s="29" t="s">
+      <c r="D100" s="49" t="s">
         <v>265</v>
       </c>
-      <c r="E98" s="28" t="s">
+      <c r="E100" s="17" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="99" spans="1:5">
-      <c r="A99" s="37"/>
-      <c r="B99" s="52"/>
-      <c r="C99" s="25" t="s">
+    <row r="101" spans="1:5" ht="30">
+      <c r="A101" s="47"/>
+      <c r="B101" s="48"/>
+      <c r="C101" s="22" t="s">
         <v>266</v>
       </c>
-      <c r="D99" s="22" t="s">
+      <c r="D101" s="15" t="s">
         <v>267</v>
       </c>
-      <c r="E99" s="28" t="s">
+      <c r="E101" s="17" t="s">
         <v>91</v>
       </c>
     </row>
+    <row r="102" spans="1:5" ht="60">
+      <c r="A102" s="50" t="s">
+        <v>315</v>
+      </c>
+      <c r="B102" s="51" t="s">
+        <v>316</v>
+      </c>
+      <c r="C102" s="52" t="s">
+        <v>317</v>
+      </c>
+      <c r="D102" s="52" t="s">
+        <v>319</v>
+      </c>
+      <c r="E102" s="52" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="60">
+      <c r="A103" s="53"/>
+      <c r="B103" s="54"/>
+      <c r="C103" s="52" t="s">
+        <v>318</v>
+      </c>
+      <c r="D103" s="55" t="s">
+        <v>320</v>
+      </c>
+      <c r="E103" s="52" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="60">
+      <c r="A104" s="53"/>
+      <c r="B104" s="56" t="s">
+        <v>322</v>
+      </c>
+      <c r="C104" s="52" t="s">
+        <v>321</v>
+      </c>
+      <c r="D104" s="52" t="s">
+        <v>329</v>
+      </c>
+      <c r="E104" s="52" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="45">
+      <c r="A105" s="53"/>
+      <c r="B105" s="56" t="s">
+        <v>325</v>
+      </c>
+      <c r="C105" s="52" t="s">
+        <v>324</v>
+      </c>
+      <c r="D105" s="52" t="s">
+        <v>323</v>
+      </c>
+      <c r="E105" s="52" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="15" customHeight="1">
+      <c r="A106" s="57"/>
+      <c r="B106" s="56" t="s">
+        <v>328</v>
+      </c>
+      <c r="C106" s="52" t="s">
+        <v>326</v>
+      </c>
+      <c r="D106" s="52" t="s">
+        <v>327</v>
+      </c>
+      <c r="E106" s="52" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="15" customHeight="1">
+      <c r="A107" s="18"/>
+      <c r="B107" s="19"/>
+      <c r="C107" s="19"/>
+      <c r="D107" s="20"/>
+      <c r="E107" s="19"/>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" s="19"/>
+    </row>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="B91:B94"/>
-    <mergeCell ref="B95:B96"/>
-    <mergeCell ref="B97:B99"/>
-    <mergeCell ref="B74:B78"/>
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="B82:B84"/>
-    <mergeCell ref="B85:B86"/>
-    <mergeCell ref="B87:B90"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="B69:B71"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B53:B56"/>
-    <mergeCell ref="B57:B60"/>
+  <mergeCells count="39">
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="B102:B103"/>
+    <mergeCell ref="A102:A106"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A11:A21"/>
+    <mergeCell ref="A22:A31"/>
+    <mergeCell ref="A35:A51"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="A55:A66"/>
+    <mergeCell ref="A67:A75"/>
+    <mergeCell ref="A76:A88"/>
+    <mergeCell ref="A89:A96"/>
+    <mergeCell ref="A97:A101"/>
     <mergeCell ref="B11:B16"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B33:B34"/>
     <mergeCell ref="B35:B36"/>
-    <mergeCell ref="A53:A64"/>
-    <mergeCell ref="A65:A73"/>
-    <mergeCell ref="A74:A86"/>
-    <mergeCell ref="A87:A94"/>
-    <mergeCell ref="A95:A99"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="A11:A21"/>
-    <mergeCell ref="A22:A31"/>
-    <mergeCell ref="A33:A49"/>
-    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="B59:B62"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="B71:B73"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="B93:B96"/>
+    <mergeCell ref="B97:B98"/>
+    <mergeCell ref="B99:B101"/>
+    <mergeCell ref="B76:B80"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="B84:B86"/>
+    <mergeCell ref="B87:B88"/>
+    <mergeCell ref="B89:B92"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" sqref="A33:A38" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" sqref="A35:A40"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -3263,22 +3505,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="45" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="42">
+    <row r="1" spans="1:4" ht="40.5">
       <c r="A1" s="1" t="s">
         <v>268</v>
       </c>
@@ -3292,7 +3534,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="55.8">
+    <row r="2" spans="1:4" ht="56.25">
       <c r="A2" s="3" t="s">
         <v>272</v>
       </c>
@@ -3306,7 +3548,7 @@
         <v>45760</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="55.8">
+    <row r="3" spans="1:4" ht="56.25">
       <c r="A3" s="3" t="s">
         <v>274</v>
       </c>
@@ -3320,7 +3562,7 @@
         <v>45765</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="37.200000000000003">
+    <row r="4" spans="1:4" ht="37.5">
       <c r="A4" s="3" t="s">
         <v>276</v>
       </c>
@@ -3334,7 +3576,7 @@
         <v>45766</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="74.400000000000006">
+    <row r="5" spans="1:4" ht="75">
       <c r="A5" s="3" t="s">
         <v>278</v>
       </c>
@@ -3348,7 +3590,7 @@
         <v>45773</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="37.200000000000003">
+    <row r="6" spans="1:4" ht="37.5">
       <c r="A6" s="3" t="s">
         <v>280</v>
       </c>
@@ -3362,7 +3604,7 @@
         <v>45773</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="37.200000000000003">
+    <row r="7" spans="1:4" ht="37.5">
       <c r="A7" s="3" t="s">
         <v>282</v>
       </c>
@@ -3376,7 +3618,7 @@
         <v>45780</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="37.200000000000003">
+    <row r="8" spans="1:4" ht="37.5">
       <c r="A8" s="3" t="s">
         <v>284</v>
       </c>
@@ -3390,7 +3632,7 @@
         <v>45781</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="37.200000000000003">
+    <row r="9" spans="1:4" ht="37.5">
       <c r="A9" s="3" t="s">
         <v>286</v>
       </c>
@@ -3404,7 +3646,7 @@
         <v>45784</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="37.200000000000003">
+    <row r="10" spans="1:4" ht="37.5">
       <c r="A10" s="3" t="s">
         <v>288</v>
       </c>
@@ -3418,7 +3660,7 @@
         <v>45785</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="37.200000000000003">
+    <row r="11" spans="1:4" ht="37.5">
       <c r="A11" s="3" t="s">
         <v>290</v>
       </c>
@@ -3432,7 +3674,7 @@
         <v>45786</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="37.200000000000003">
+    <row r="12" spans="1:4" ht="37.5">
       <c r="A12" s="3" t="s">
         <v>292</v>
       </c>
@@ -3446,7 +3688,7 @@
         <v>45786</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="18.600000000000001">
+    <row r="13" spans="1:4" ht="18.75">
       <c r="A13" s="3" t="s">
         <v>294</v>
       </c>
@@ -3460,7 +3702,7 @@
         <v>45786</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="18.600000000000001">
+    <row r="14" spans="1:4" ht="18.75">
       <c r="A14" s="3" t="s">
         <v>296</v>
       </c>
@@ -3474,7 +3716,7 @@
         <v>45786</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="37.200000000000003">
+    <row r="15" spans="1:4" ht="37.5">
       <c r="A15" s="3" t="s">
         <v>298</v>
       </c>
@@ -3488,7 +3730,7 @@
         <v>45787</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="37.200000000000003">
+    <row r="16" spans="1:4" ht="37.5">
       <c r="A16" s="3" t="s">
         <v>300</v>
       </c>
@@ -3502,17 +3744,31 @@
         <v>45787</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="37.200000000000003">
+    <row r="17" spans="1:4" ht="37.5">
       <c r="A17" s="3" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D17" s="5">
+        <v>45787</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="37.5">
+      <c r="A18" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="D18" s="5">
         <v>45787</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v3.2 Adjusted the [Publish video] after get comments
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_SRS.xlsx
+++ b/LH_REQUIREMENTS/LH_SRS.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halae\OneDrive\Desktop\Group-3-Learning-hub-dev\LH_REQUIREMENTS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halae\OneDrive\Desktop\Group-3-Learning-hub-dev\Group-3-Learning-hub-dev\LH_REQUIREMENTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="LH_SRS" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="332">
   <si>
     <t>Feature</t>
   </si>
@@ -704,31 +704,16 @@
     <t>LH-CRS-PUBLISHVIDEO-001</t>
   </si>
   <si>
-    <t>LH-SRS-PUBVID-001</t>
-  </si>
-  <si>
     <t>The system shall restrict access to the publish video interface to registered users only.</t>
   </si>
   <si>
     <t>Mahmoud Abdelmageed</t>
   </si>
   <si>
-    <t>LH-SRS-PUBVID-002</t>
-  </si>
-  <si>
-    <t>LH-SRS-PUBVID-003</t>
-  </si>
-  <si>
     <t>The "Categories" page shall contain a dropdown menu that includes an option labeled "Publish video".</t>
   </si>
   <si>
-    <t>LH-SRS-PUBVID-004</t>
-  </si>
-  <si>
     <t>Selecting "Publish Video" shall navigate the user to the video publish page.</t>
-  </si>
-  <si>
-    <t>LH-SRS-PUBVID-005</t>
   </si>
   <si>
     <t>The system shall provide a size indicator showing the video size like this : 
@@ -738,16 +723,10 @@
     <t>LH-CRS-PUBLISHVIDEO-002</t>
   </si>
   <si>
-    <t>LH-SRS-PUBVID-007</t>
-  </si>
-  <si>
     <t>The system shall validate video file size before upload and reject files exceeding 100MB, with the message: "Max size: 100MB."</t>
   </si>
   <si>
     <t>LH-CRS-PUBLISHVIDEO-003</t>
-  </si>
-  <si>
-    <t>LH-SRS-PUBVID-008</t>
   </si>
   <si>
     <t xml:space="preserve">The system shall display the message :
@@ -755,44 +734,26 @@
 </t>
   </si>
   <si>
-    <t>LH-SRS-PUBVID-009</t>
-  </si>
-  <si>
     <t>Upon clicking Upload the system shall open a window to browse files on the user pc with restricted rule of viewing MP4 files only</t>
   </si>
   <si>
     <t>LH-CRS-PUBLISHVIDEO-004</t>
-  </si>
-  <si>
-    <t>LH-SRS-PUBVID-010</t>
   </si>
   <si>
     <t xml:space="preserve">The publish button will be inactive if the video size is above 100 MB
 </t>
   </si>
   <si>
-    <t>LH-SRS-PUBVID-011</t>
-  </si>
-  <si>
     <t>The publish button will be inactive if the video title is empty</t>
   </si>
   <si>
-    <t>LH-SRS-PUBVID-012</t>
-  </si>
-  <si>
     <t>Clicking the publish button will store the video in the database to the designated category</t>
   </si>
   <si>
     <t>LH-CRS-PUBLISHVIDEO-005</t>
   </si>
   <si>
-    <t>LH-SRS-PUBVID-013</t>
-  </si>
-  <si>
     <t>Clicking the publish button without uploading a video will display error message : Please Upload a valid video</t>
-  </si>
-  <si>
-    <t>LH-SRS-PUBVID-014</t>
   </si>
   <si>
     <t>Clicking the publish button without adding a title will display error message : Please add a title</t>
@@ -1192,6 +1153,51 @@
   <si>
     <t xml:space="preserve">The system shall dynamically retrieve and display notifications for new posts in categories the user follows in notification section
 </t>
+  </si>
+  <si>
+    <t>LH-SRS-PUBLISHVIDEO-001</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUBLISHVIDEO-002</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUBLISHVIDEO-003</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUBLISHVIDEO-004</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUBLISHVIDEO-005</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUBLISHVIDEO-006</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUBLISHVIDEO-007</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUBLISHVIDEO-008</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUBLISHVIDEO-009</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUBLISHVIDEO-010</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUBLISHVIDEO-011</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUBLISHVIDEO-012</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUBLISHVIDEO-013</t>
+  </si>
+  <si>
+    <t>v3.2</t>
+  </si>
+  <si>
+    <t>Adjusted the [Publish video] after get comments</t>
   </si>
 </sst>
 </file>
@@ -1516,6 +1522,33 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1525,33 +1558,42 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1567,9 +1609,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1579,46 +1618,13 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1898,8 +1904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="91" zoomScaleNormal="111" workbookViewId="0">
-      <selection activeCell="G103" sqref="G103"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="79" zoomScaleNormal="111" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1930,7 +1936,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="60">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="32" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="14" t="s">
@@ -1940,14 +1946,14 @@
         <v>7</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30">
-      <c r="A3" s="24"/>
+      <c r="A3" s="33"/>
       <c r="B3" s="14" t="s">
         <v>9</v>
       </c>
@@ -1962,7 +1968,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="30">
-      <c r="A4" s="24"/>
+      <c r="A4" s="33"/>
       <c r="B4" s="14" t="s">
         <v>12</v>
       </c>
@@ -1977,7 +1983,7 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="24"/>
+      <c r="A5" s="33"/>
       <c r="B5" s="14" t="s">
         <v>15</v>
       </c>
@@ -1992,7 +1998,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="30">
-      <c r="A6" s="24"/>
+      <c r="A6" s="33"/>
       <c r="B6" s="14" t="s">
         <v>18</v>
       </c>
@@ -2000,30 +2006,30 @@
         <v>19</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30">
-      <c r="A7" s="24"/>
-      <c r="B7" s="26" t="s">
+      <c r="A7" s="33"/>
+      <c r="B7" s="23" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="24"/>
-      <c r="B8" s="26" t="s">
+      <c r="A8" s="33"/>
+      <c r="B8" s="23" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="14" t="s">
@@ -2037,7 +2043,7 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="24"/>
+      <c r="A9" s="33"/>
       <c r="B9" s="14" t="s">
         <v>25</v>
       </c>
@@ -2045,15 +2051,15 @@
         <v>26</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="24"/>
-      <c r="B10" s="26" t="s">
+      <c r="A10" s="33"/>
+      <c r="B10" s="23" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="14" t="s">
@@ -2067,10 +2073,10 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="30">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="30" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="14" t="s">
@@ -2084,8 +2090,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="30">
-      <c r="A12" s="24"/>
-      <c r="B12" s="28"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="45"/>
       <c r="C12" s="14" t="s">
         <v>35</v>
       </c>
@@ -2097,8 +2103,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="28.5" customHeight="1">
-      <c r="A13" s="24"/>
-      <c r="B13" s="28"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="45"/>
       <c r="C13" s="14" t="s">
         <v>37</v>
       </c>
@@ -2110,8 +2116,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="28.5" customHeight="1">
-      <c r="A14" s="24"/>
-      <c r="B14" s="28"/>
+      <c r="A14" s="33"/>
+      <c r="B14" s="45"/>
       <c r="C14" s="14" t="s">
         <v>39</v>
       </c>
@@ -2123,8 +2129,8 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="30">
-      <c r="A15" s="24"/>
-      <c r="B15" s="28"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="45"/>
       <c r="C15" s="14" t="s">
         <v>41</v>
       </c>
@@ -2136,8 +2142,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="30">
-      <c r="A16" s="24"/>
-      <c r="B16" s="29"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="31"/>
       <c r="C16" s="14" t="s">
         <v>43</v>
       </c>
@@ -2149,8 +2155,8 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="45">
-      <c r="A17" s="24"/>
-      <c r="B17" s="27" t="s">
+      <c r="A17" s="33"/>
+      <c r="B17" s="30" t="s">
         <v>45</v>
       </c>
       <c r="C17" s="14" t="s">
@@ -2164,8 +2170,8 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="30">
-      <c r="A18" s="24"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="31"/>
       <c r="C18" s="14" t="s">
         <v>48</v>
       </c>
@@ -2177,8 +2183,8 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="30">
-      <c r="A19" s="24"/>
-      <c r="B19" s="27" t="s">
+      <c r="A19" s="33"/>
+      <c r="B19" s="30" t="s">
         <v>50</v>
       </c>
       <c r="C19" s="14" t="s">
@@ -2192,8 +2198,8 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="30">
-      <c r="A20" s="24"/>
-      <c r="B20" s="28"/>
+      <c r="A20" s="33"/>
+      <c r="B20" s="45"/>
       <c r="C20" s="14" t="s">
         <v>53</v>
       </c>
@@ -2205,8 +2211,8 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="30">
-      <c r="A21" s="25"/>
-      <c r="B21" s="29"/>
+      <c r="A21" s="34"/>
+      <c r="B21" s="31"/>
       <c r="C21" s="14" t="s">
         <v>55</v>
       </c>
@@ -2218,7 +2224,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="30">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="40" t="s">
         <v>57</v>
       </c>
       <c r="B22" s="15" t="s">
@@ -2235,7 +2241,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="30">
-      <c r="A23" s="31"/>
+      <c r="A23" s="41"/>
       <c r="B23" s="15" t="s">
         <v>61</v>
       </c>
@@ -2250,7 +2256,7 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="31"/>
+      <c r="A24" s="41"/>
       <c r="B24" s="15" t="s">
         <v>64</v>
       </c>
@@ -2265,7 +2271,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="30">
-      <c r="A25" s="31"/>
+      <c r="A25" s="41"/>
       <c r="B25" s="15" t="s">
         <v>67</v>
       </c>
@@ -2280,7 +2286,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="30">
-      <c r="A26" s="31"/>
+      <c r="A26" s="41"/>
       <c r="B26" s="15" t="s">
         <v>70</v>
       </c>
@@ -2295,7 +2301,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="30">
-      <c r="A27" s="31"/>
+      <c r="A27" s="41"/>
       <c r="B27" s="15" t="s">
         <v>73</v>
       </c>
@@ -2309,8 +2315,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="45">
-      <c r="A28" s="31"/>
+    <row r="28" spans="1:7" ht="30">
+      <c r="A28" s="41"/>
       <c r="B28" s="15" t="s">
         <v>76</v>
       </c>
@@ -2318,14 +2324,14 @@
         <v>77</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="E28" s="15" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30">
-      <c r="A29" s="31"/>
+      <c r="A29" s="41"/>
       <c r="B29" s="15" t="s">
         <v>78</v>
       </c>
@@ -2340,7 +2346,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="30">
-      <c r="A30" s="31"/>
+      <c r="A30" s="41"/>
       <c r="B30" s="15" t="s">
         <v>81</v>
       </c>
@@ -2355,7 +2361,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="30">
-      <c r="A31" s="32"/>
+      <c r="A31" s="42"/>
       <c r="B31" s="15" t="s">
         <v>84</v>
       </c>
@@ -2370,7 +2376,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="30">
-      <c r="A32" s="23" t="s">
+      <c r="A32" s="32" t="s">
         <v>87</v>
       </c>
       <c r="B32" s="14" t="s">
@@ -2389,38 +2395,38 @@
       <c r="G32" s="16"/>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1">
-      <c r="A33" s="24"/>
+      <c r="A33" s="33"/>
       <c r="B33" s="14" t="s">
-        <v>309</v>
-      </c>
-      <c r="C33" s="27" t="s">
-        <v>308</v>
-      </c>
-      <c r="D33" s="27" t="s">
-        <v>311</v>
-      </c>
-      <c r="E33" s="27" t="s">
-        <v>238</v>
+        <v>296</v>
+      </c>
+      <c r="C33" s="30" t="s">
+        <v>295</v>
+      </c>
+      <c r="D33" s="30" t="s">
+        <v>298</v>
+      </c>
+      <c r="E33" s="30" t="s">
+        <v>225</v>
       </c>
       <c r="F33" s="16"/>
       <c r="G33" s="16"/>
     </row>
     <row r="34" spans="1:7" ht="75" customHeight="1">
-      <c r="A34" s="25"/>
+      <c r="A34" s="34"/>
       <c r="B34" s="14" t="s">
-        <v>310</v>
-      </c>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="29"/>
+        <v>297</v>
+      </c>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
       <c r="F34" s="16"/>
       <c r="G34" s="16"/>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1">
-      <c r="A35" s="30" t="s">
+      <c r="A35" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="B35" s="33" t="s">
+      <c r="B35" s="46" t="s">
         <v>93</v>
       </c>
       <c r="C35" s="15" t="s">
@@ -2434,8 +2440,8 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1">
-      <c r="A36" s="31"/>
-      <c r="B36" s="33"/>
+      <c r="A36" s="41"/>
+      <c r="B36" s="46"/>
       <c r="C36" s="15" t="s">
         <v>96</v>
       </c>
@@ -2447,8 +2453,8 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1">
-      <c r="A37" s="31"/>
-      <c r="B37" s="33" t="s">
+      <c r="A37" s="41"/>
+      <c r="B37" s="46" t="s">
         <v>98</v>
       </c>
       <c r="C37" s="15" t="s">
@@ -2462,8 +2468,8 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1">
-      <c r="A38" s="31"/>
-      <c r="B38" s="33"/>
+      <c r="A38" s="41"/>
+      <c r="B38" s="46"/>
       <c r="C38" s="15" t="s">
         <v>101</v>
       </c>
@@ -2475,8 +2481,8 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1">
-      <c r="A39" s="31"/>
-      <c r="B39" s="34" t="s">
+      <c r="A39" s="41"/>
+      <c r="B39" s="24" t="s">
         <v>103</v>
       </c>
       <c r="C39" s="15" t="s">
@@ -2490,8 +2496,8 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1">
-      <c r="A40" s="31"/>
-      <c r="B40" s="34" t="s">
+      <c r="A40" s="41"/>
+      <c r="B40" s="24" t="s">
         <v>106</v>
       </c>
       <c r="C40" s="15" t="s">
@@ -2505,8 +2511,8 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="30">
-      <c r="A41" s="31"/>
-      <c r="B41" s="34" t="s">
+      <c r="A41" s="41"/>
+      <c r="B41" s="24" t="s">
         <v>109</v>
       </c>
       <c r="C41" s="15" t="s">
@@ -2520,8 +2526,8 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="30">
-      <c r="A42" s="31"/>
-      <c r="B42" s="35" t="s">
+      <c r="A42" s="41"/>
+      <c r="B42" s="47" t="s">
         <v>112</v>
       </c>
       <c r="C42" s="15" t="s">
@@ -2535,8 +2541,8 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="45">
-      <c r="A43" s="31"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="48"/>
       <c r="C43" s="15" t="s">
         <v>115</v>
       </c>
@@ -2548,8 +2554,8 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="30">
-      <c r="A44" s="31"/>
-      <c r="B44" s="35" t="s">
+      <c r="A44" s="41"/>
+      <c r="B44" s="47" t="s">
         <v>117</v>
       </c>
       <c r="C44" s="15" t="s">
@@ -2563,8 +2569,8 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="30">
-      <c r="A45" s="31"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="48"/>
       <c r="C45" s="15" t="s">
         <v>120</v>
       </c>
@@ -2576,8 +2582,8 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="30">
-      <c r="A46" s="31"/>
-      <c r="B46" s="34" t="s">
+      <c r="A46" s="41"/>
+      <c r="B46" s="24" t="s">
         <v>122</v>
       </c>
       <c r="C46" s="15" t="s">
@@ -2591,8 +2597,8 @@
       </c>
     </row>
     <row r="47" spans="1:7" ht="30">
-      <c r="A47" s="31"/>
-      <c r="B47" s="34" t="s">
+      <c r="A47" s="41"/>
+      <c r="B47" s="24" t="s">
         <v>125</v>
       </c>
       <c r="C47" s="15" t="s">
@@ -2606,8 +2612,8 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="30">
-      <c r="A48" s="31"/>
-      <c r="B48" s="34" t="s">
+      <c r="A48" s="41"/>
+      <c r="B48" s="24" t="s">
         <v>128</v>
       </c>
       <c r="C48" s="15" t="s">
@@ -2621,8 +2627,8 @@
       </c>
     </row>
     <row r="49" spans="1:5" ht="30">
-      <c r="A49" s="31"/>
-      <c r="B49" s="34" t="s">
+      <c r="A49" s="41"/>
+      <c r="B49" s="24" t="s">
         <v>131</v>
       </c>
       <c r="C49" s="15" t="s">
@@ -2631,13 +2637,13 @@
       <c r="D49" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="E49" s="34" t="s">
+      <c r="E49" s="24" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="45">
-      <c r="A50" s="31"/>
-      <c r="B50" s="35" t="s">
+      <c r="A50" s="41"/>
+      <c r="B50" s="47" t="s">
         <v>134</v>
       </c>
       <c r="C50" s="15" t="s">
@@ -2646,25 +2652,25 @@
       <c r="D50" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="E50" s="34" t="s">
+      <c r="E50" s="24" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="60">
-      <c r="A51" s="31"/>
-      <c r="B51" s="36"/>
+      <c r="A51" s="41"/>
+      <c r="B51" s="48"/>
       <c r="C51" s="15" t="s">
         <v>137</v>
       </c>
       <c r="D51" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="E51" s="34" t="s">
+      <c r="E51" s="24" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="45">
-      <c r="A52" s="23" t="s">
+      <c r="A52" s="32" t="s">
         <v>139</v>
       </c>
       <c r="B52" s="14" t="s">
@@ -2681,7 +2687,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" ht="30">
-      <c r="A53" s="24"/>
+      <c r="A53" s="33"/>
       <c r="B53" s="14" t="s">
         <v>143</v>
       </c>
@@ -2696,7 +2702,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" ht="30">
-      <c r="A54" s="24"/>
+      <c r="A54" s="33"/>
       <c r="B54" s="14" t="s">
         <v>146</v>
       </c>
@@ -2711,10 +2717,10 @@
       </c>
     </row>
     <row r="55" spans="1:5" ht="30">
-      <c r="A55" s="30" t="s">
+      <c r="A55" s="40" t="s">
         <v>149</v>
       </c>
-      <c r="B55" s="37" t="s">
+      <c r="B55" s="49" t="s">
         <v>150</v>
       </c>
       <c r="C55" s="15" t="s">
@@ -2728,8 +2734,8 @@
       </c>
     </row>
     <row r="56" spans="1:5" ht="30">
-      <c r="A56" s="31"/>
-      <c r="B56" s="38"/>
+      <c r="A56" s="41"/>
+      <c r="B56" s="50"/>
       <c r="C56" s="15" t="s">
         <v>153</v>
       </c>
@@ -2741,8 +2747,8 @@
       </c>
     </row>
     <row r="57" spans="1:5" ht="30">
-      <c r="A57" s="31"/>
-      <c r="B57" s="38"/>
+      <c r="A57" s="41"/>
+      <c r="B57" s="50"/>
       <c r="C57" s="15" t="s">
         <v>155</v>
       </c>
@@ -2754,8 +2760,8 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="30">
-      <c r="A58" s="31"/>
-      <c r="B58" s="39"/>
+      <c r="A58" s="41"/>
+      <c r="B58" s="51"/>
       <c r="C58" s="15" t="s">
         <v>157</v>
       </c>
@@ -2767,8 +2773,8 @@
       </c>
     </row>
     <row r="59" spans="1:5" ht="30">
-      <c r="A59" s="31"/>
-      <c r="B59" s="37" t="s">
+      <c r="A59" s="41"/>
+      <c r="B59" s="49" t="s">
         <v>159</v>
       </c>
       <c r="C59" s="15" t="s">
@@ -2781,9 +2787,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="45">
-      <c r="A60" s="31"/>
-      <c r="B60" s="38"/>
+    <row r="60" spans="1:5" ht="30">
+      <c r="A60" s="41"/>
+      <c r="B60" s="50"/>
       <c r="C60" s="15" t="s">
         <v>162</v>
       </c>
@@ -2795,8 +2801,8 @@
       </c>
     </row>
     <row r="61" spans="1:5" ht="45">
-      <c r="A61" s="31"/>
-      <c r="B61" s="38"/>
+      <c r="A61" s="41"/>
+      <c r="B61" s="50"/>
       <c r="C61" s="15" t="s">
         <v>164</v>
       </c>
@@ -2808,8 +2814,8 @@
       </c>
     </row>
     <row r="62" spans="1:5" ht="45">
-      <c r="A62" s="31"/>
-      <c r="B62" s="39"/>
+      <c r="A62" s="41"/>
+      <c r="B62" s="51"/>
       <c r="C62" s="15" t="s">
         <v>166</v>
       </c>
@@ -2821,8 +2827,8 @@
       </c>
     </row>
     <row r="63" spans="1:5" ht="45">
-      <c r="A63" s="31"/>
-      <c r="B63" s="40" t="s">
+      <c r="A63" s="41"/>
+      <c r="B63" s="25" t="s">
         <v>168</v>
       </c>
       <c r="C63" s="15" t="s">
@@ -2836,8 +2842,8 @@
       </c>
     </row>
     <row r="64" spans="1:5" ht="45">
-      <c r="A64" s="31"/>
-      <c r="B64" s="40" t="s">
+      <c r="A64" s="41"/>
+      <c r="B64" s="25" t="s">
         <v>171</v>
       </c>
       <c r="C64" s="15" t="s">
@@ -2851,8 +2857,8 @@
       </c>
     </row>
     <row r="65" spans="1:5" ht="30">
-      <c r="A65" s="31"/>
-      <c r="B65" s="37" t="s">
+      <c r="A65" s="41"/>
+      <c r="B65" s="49" t="s">
         <v>174</v>
       </c>
       <c r="C65" s="15" t="s">
@@ -2866,8 +2872,8 @@
       </c>
     </row>
     <row r="66" spans="1:5" ht="45">
-      <c r="A66" s="32"/>
-      <c r="B66" s="39"/>
+      <c r="A66" s="42"/>
+      <c r="B66" s="51"/>
       <c r="C66" s="15" t="s">
         <v>177</v>
       </c>
@@ -2879,10 +2885,10 @@
       </c>
     </row>
     <row r="67" spans="1:5" ht="30">
-      <c r="A67" s="23" t="s">
+      <c r="A67" s="32" t="s">
         <v>179</v>
       </c>
-      <c r="B67" s="41" t="s">
+      <c r="B67" s="52" t="s">
         <v>180</v>
       </c>
       <c r="C67" s="14" t="s">
@@ -2896,8 +2902,8 @@
       </c>
     </row>
     <row r="68" spans="1:5" ht="30">
-      <c r="A68" s="24"/>
-      <c r="B68" s="42"/>
+      <c r="A68" s="33"/>
+      <c r="B68" s="53"/>
       <c r="C68" s="14" t="s">
         <v>183</v>
       </c>
@@ -2909,8 +2915,8 @@
       </c>
     </row>
     <row r="69" spans="1:5" ht="30">
-      <c r="A69" s="24"/>
-      <c r="B69" s="41" t="s">
+      <c r="A69" s="33"/>
+      <c r="B69" s="52" t="s">
         <v>185</v>
       </c>
       <c r="C69" s="14" t="s">
@@ -2924,8 +2930,8 @@
       </c>
     </row>
     <row r="70" spans="1:5" ht="30">
-      <c r="A70" s="24"/>
-      <c r="B70" s="42"/>
+      <c r="A70" s="33"/>
+      <c r="B70" s="53"/>
       <c r="C70" s="14" t="s">
         <v>188</v>
       </c>
@@ -2937,8 +2943,8 @@
       </c>
     </row>
     <row r="71" spans="1:5" ht="30">
-      <c r="A71" s="24"/>
-      <c r="B71" s="41" t="s">
+      <c r="A71" s="33"/>
+      <c r="B71" s="52" t="s">
         <v>190</v>
       </c>
       <c r="C71" s="14" t="s">
@@ -2952,8 +2958,8 @@
       </c>
     </row>
     <row r="72" spans="1:5" ht="30">
-      <c r="A72" s="24"/>
-      <c r="B72" s="43"/>
+      <c r="A72" s="33"/>
+      <c r="B72" s="54"/>
       <c r="C72" s="14" t="s">
         <v>193</v>
       </c>
@@ -2965,8 +2971,8 @@
       </c>
     </row>
     <row r="73" spans="1:5" ht="30">
-      <c r="A73" s="24"/>
-      <c r="B73" s="43"/>
+      <c r="A73" s="33"/>
+      <c r="B73" s="54"/>
       <c r="C73" s="14" t="s">
         <v>195</v>
       </c>
@@ -2978,8 +2984,8 @@
       </c>
     </row>
     <row r="74" spans="1:5" ht="30">
-      <c r="A74" s="24"/>
-      <c r="B74" s="41" t="s">
+      <c r="A74" s="33"/>
+      <c r="B74" s="52" t="s">
         <v>197</v>
       </c>
       <c r="C74" s="14" t="s">
@@ -2993,8 +2999,8 @@
       </c>
     </row>
     <row r="75" spans="1:5" ht="45">
-      <c r="A75" s="24"/>
-      <c r="B75" s="42"/>
+      <c r="A75" s="33"/>
+      <c r="B75" s="53"/>
       <c r="C75" s="14" t="s">
         <v>200</v>
       </c>
@@ -3006,442 +3012,442 @@
       </c>
     </row>
     <row r="76" spans="1:5" ht="30">
-      <c r="A76" s="44" t="s">
+      <c r="A76" s="43" t="s">
         <v>202</v>
       </c>
-      <c r="B76" s="37" t="s">
+      <c r="B76" s="49" t="s">
         <v>203</v>
       </c>
       <c r="C76" s="22" t="s">
+        <v>317</v>
+      </c>
+      <c r="D76" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="D76" s="15" t="s">
+      <c r="E76" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="E76" s="15" t="s">
-        <v>206</v>
-      </c>
     </row>
     <row r="77" spans="1:5" ht="30">
-      <c r="A77" s="44"/>
-      <c r="B77" s="38"/>
+      <c r="A77" s="43"/>
+      <c r="B77" s="50"/>
       <c r="C77" s="22" t="s">
-        <v>207</v>
+        <v>318</v>
       </c>
       <c r="D77" s="15" t="s">
         <v>154</v>
       </c>
       <c r="E77" s="15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="30">
+      <c r="A78" s="43"/>
+      <c r="B78" s="50"/>
+      <c r="C78" s="22" t="s">
+        <v>319</v>
+      </c>
+      <c r="D78" s="15" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" ht="30">
-      <c r="A78" s="44"/>
-      <c r="B78" s="38"/>
-      <c r="C78" s="22" t="s">
+      <c r="E78" s="15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="30">
+      <c r="A79" s="43"/>
+      <c r="B79" s="50"/>
+      <c r="C79" s="22" t="s">
+        <v>320</v>
+      </c>
+      <c r="D79" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="E79" s="15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="45">
+      <c r="A80" s="43"/>
+      <c r="B80" s="50"/>
+      <c r="C80" s="22" t="s">
+        <v>321</v>
+      </c>
+      <c r="D80" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="D78" s="15" t="s">
+      <c r="E80" s="15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="45">
+      <c r="A81" s="43"/>
+      <c r="B81" s="15" t="s">
         <v>209</v>
       </c>
-      <c r="E78" s="15" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="30">
-      <c r="A79" s="44"/>
-      <c r="B79" s="38"/>
-      <c r="C79" s="22" t="s">
+      <c r="C81" s="22" t="s">
+        <v>322</v>
+      </c>
+      <c r="D81" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="D79" s="15" t="s">
+      <c r="E81" s="15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="45">
+      <c r="A82" s="43"/>
+      <c r="B82" s="49" t="s">
         <v>211</v>
       </c>
-      <c r="E79" s="15" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="45">
-      <c r="A80" s="44"/>
-      <c r="B80" s="38"/>
-      <c r="C80" s="22" t="s">
+      <c r="C82" s="22" t="s">
+        <v>323</v>
+      </c>
+      <c r="D82" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="D80" s="15" t="s">
+      <c r="E82" s="15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="45">
+      <c r="A83" s="43"/>
+      <c r="B83" s="51"/>
+      <c r="C83" s="22" t="s">
+        <v>324</v>
+      </c>
+      <c r="D83" s="15" t="s">
         <v>213</v>
       </c>
-      <c r="E80" s="15" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="45">
-      <c r="A81" s="44"/>
-      <c r="B81" s="15" t="s">
+      <c r="E83" s="15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="45">
+      <c r="A84" s="43"/>
+      <c r="B84" s="49" t="s">
         <v>214</v>
       </c>
-      <c r="C81" s="22" t="s">
+      <c r="C84" s="22" t="s">
+        <v>325</v>
+      </c>
+      <c r="D84" s="15" t="s">
         <v>215</v>
       </c>
-      <c r="D81" s="15" t="s">
+      <c r="E84" s="15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="30">
+      <c r="A85" s="43"/>
+      <c r="B85" s="50"/>
+      <c r="C85" s="22" t="s">
+        <v>326</v>
+      </c>
+      <c r="D85" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="E81" s="15" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="45">
-      <c r="A82" s="44"/>
-      <c r="B82" s="37" t="s">
+      <c r="E85" s="15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="30">
+      <c r="A86" s="43"/>
+      <c r="B86" s="51"/>
+      <c r="C86" s="22" t="s">
+        <v>327</v>
+      </c>
+      <c r="D86" s="15" t="s">
         <v>217</v>
       </c>
-      <c r="C82" s="22" t="s">
+      <c r="E86" s="15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="30">
+      <c r="A87" s="43"/>
+      <c r="B87" s="56" t="s">
         <v>218</v>
       </c>
-      <c r="D82" s="15" t="s">
+      <c r="C87" s="22" t="s">
+        <v>328</v>
+      </c>
+      <c r="D87" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="E82" s="15" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="45">
-      <c r="A83" s="44"/>
-      <c r="B83" s="39"/>
-      <c r="C83" s="22" t="s">
+      <c r="E87" s="15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="30">
+      <c r="A88" s="43"/>
+      <c r="B88" s="57"/>
+      <c r="C88" s="22" t="s">
+        <v>329</v>
+      </c>
+      <c r="D88" s="15" t="s">
         <v>220</v>
       </c>
-      <c r="D83" s="15" t="s">
+      <c r="E88" s="15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="69.95" customHeight="1">
+      <c r="A89" s="32" t="s">
         <v>221</v>
       </c>
-      <c r="E83" s="15" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="45">
-      <c r="A84" s="44"/>
-      <c r="B84" s="37" t="s">
+      <c r="B89" s="52" t="s">
         <v>222</v>
       </c>
-      <c r="C84" s="22" t="s">
+      <c r="C89" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="D84" s="15" t="s">
+      <c r="D89" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="E84" s="15" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="30">
-      <c r="A85" s="44"/>
-      <c r="B85" s="38"/>
-      <c r="C85" s="22" t="s">
+      <c r="E89" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="D85" s="15" t="s">
+    </row>
+    <row r="90" spans="1:5" ht="45">
+      <c r="A90" s="33"/>
+      <c r="B90" s="54"/>
+      <c r="C90" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="E85" s="15" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="30">
-      <c r="A86" s="44"/>
-      <c r="B86" s="39"/>
-      <c r="C86" s="22" t="s">
+      <c r="D90" s="21" t="s">
         <v>227</v>
       </c>
-      <c r="D86" s="15" t="s">
+      <c r="E90" s="14" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="45">
+      <c r="A91" s="33"/>
+      <c r="B91" s="54"/>
+      <c r="C91" s="14" t="s">
         <v>228</v>
       </c>
-      <c r="E86" s="15" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="30">
-      <c r="A87" s="44"/>
-      <c r="B87" s="45" t="s">
+      <c r="D91" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="C87" s="22" t="s">
+      <c r="E91" s="14" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="30">
+      <c r="A92" s="33"/>
+      <c r="B92" s="53"/>
+      <c r="C92" s="14" t="s">
         <v>230</v>
       </c>
-      <c r="D87" s="15" t="s">
+      <c r="D92" s="21" t="s">
         <v>231</v>
       </c>
-      <c r="E87" s="15" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="30">
-      <c r="A88" s="44"/>
-      <c r="B88" s="46"/>
-      <c r="C88" s="22" t="s">
+      <c r="E92" s="14" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="50.1" customHeight="1">
+      <c r="A93" s="33"/>
+      <c r="B93" s="52" t="s">
         <v>232</v>
       </c>
-      <c r="D88" s="15" t="s">
+      <c r="C93" s="14" t="s">
         <v>233</v>
       </c>
-      <c r="E88" s="15" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="69.95" customHeight="1">
-      <c r="A89" s="23" t="s">
+      <c r="D93" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="B89" s="41" t="s">
+      <c r="E93" s="14" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="30">
+      <c r="A94" s="33"/>
+      <c r="B94" s="54"/>
+      <c r="C94" s="14" t="s">
         <v>235</v>
       </c>
-      <c r="C89" s="14" t="s">
+      <c r="D94" s="14" t="s">
         <v>236</v>
       </c>
-      <c r="D89" s="14" t="s">
+      <c r="E94" s="14" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="63.95" customHeight="1">
+      <c r="A95" s="33"/>
+      <c r="B95" s="54" t="s">
         <v>237</v>
       </c>
-      <c r="E89" s="14" t="s">
+      <c r="C95" s="14" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" ht="45">
-      <c r="A90" s="24"/>
-      <c r="B90" s="43"/>
-      <c r="C90" s="14" t="s">
+      <c r="D95" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="D90" s="21" t="s">
+      <c r="E95" s="14" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="45">
+      <c r="A96" s="33"/>
+      <c r="B96" s="54"/>
+      <c r="C96" s="23" t="s">
         <v>240</v>
       </c>
-      <c r="E90" s="14" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="45">
-      <c r="A91" s="24"/>
-      <c r="B91" s="43"/>
-      <c r="C91" s="14" t="s">
+      <c r="D96" s="23" t="s">
         <v>241</v>
       </c>
-      <c r="D91" s="21" t="s">
+      <c r="E96" s="23" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="33">
+      <c r="A97" s="44" t="s">
         <v>242</v>
       </c>
-      <c r="E91" s="14" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="30">
-      <c r="A92" s="24"/>
-      <c r="B92" s="42"/>
-      <c r="C92" s="14" t="s">
+      <c r="B97" s="55" t="s">
         <v>243</v>
       </c>
-      <c r="D92" s="21" t="s">
+      <c r="C97" s="22" t="s">
         <v>244</v>
       </c>
-      <c r="E92" s="14" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="50.1" customHeight="1">
-      <c r="A93" s="24"/>
-      <c r="B93" s="41" t="s">
+      <c r="D97" s="26" t="s">
         <v>245</v>
-      </c>
-      <c r="C93" s="14" t="s">
-        <v>246</v>
-      </c>
-      <c r="D93" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="E93" s="14" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="30">
-      <c r="A94" s="24"/>
-      <c r="B94" s="43"/>
-      <c r="C94" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="D94" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="E94" s="14" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" ht="63.95" customHeight="1">
-      <c r="A95" s="24"/>
-      <c r="B95" s="43" t="s">
-        <v>250</v>
-      </c>
-      <c r="C95" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="D95" s="14" t="s">
-        <v>252</v>
-      </c>
-      <c r="E95" s="14" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="45">
-      <c r="A96" s="24"/>
-      <c r="B96" s="43"/>
-      <c r="C96" s="26" t="s">
-        <v>253</v>
-      </c>
-      <c r="D96" s="26" t="s">
-        <v>254</v>
-      </c>
-      <c r="E96" s="26" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="33">
-      <c r="A97" s="47" t="s">
-        <v>255</v>
-      </c>
-      <c r="B97" s="48" t="s">
-        <v>256</v>
-      </c>
-      <c r="C97" s="22" t="s">
-        <v>257</v>
-      </c>
-      <c r="D97" s="49" t="s">
-        <v>258</v>
       </c>
       <c r="E97" s="17" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="33">
-      <c r="A98" s="47"/>
-      <c r="B98" s="48"/>
+      <c r="A98" s="44"/>
+      <c r="B98" s="55"/>
       <c r="C98" s="22" t="s">
-        <v>259</v>
-      </c>
-      <c r="D98" s="49" t="s">
-        <v>260</v>
+        <v>246</v>
+      </c>
+      <c r="D98" s="26" t="s">
+        <v>247</v>
       </c>
       <c r="E98" s="17" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="33">
-      <c r="A99" s="47"/>
-      <c r="B99" s="48" t="s">
-        <v>261</v>
+      <c r="A99" s="44"/>
+      <c r="B99" s="55" t="s">
+        <v>248</v>
       </c>
       <c r="C99" s="22" t="s">
-        <v>262</v>
-      </c>
-      <c r="D99" s="49" t="s">
-        <v>263</v>
+        <v>249</v>
+      </c>
+      <c r="D99" s="26" t="s">
+        <v>250</v>
       </c>
       <c r="E99" s="17" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="33">
-      <c r="A100" s="47"/>
-      <c r="B100" s="48"/>
+      <c r="A100" s="44"/>
+      <c r="B100" s="55"/>
       <c r="C100" s="22" t="s">
-        <v>264</v>
-      </c>
-      <c r="D100" s="49" t="s">
-        <v>265</v>
+        <v>251</v>
+      </c>
+      <c r="D100" s="26" t="s">
+        <v>252</v>
       </c>
       <c r="E100" s="17" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="30">
-      <c r="A101" s="47"/>
-      <c r="B101" s="48"/>
+      <c r="A101" s="44"/>
+      <c r="B101" s="55"/>
       <c r="C101" s="22" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="D101" s="15" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="E101" s="17" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="60">
-      <c r="A102" s="50" t="s">
+      <c r="A102" s="37" t="s">
+        <v>302</v>
+      </c>
+      <c r="B102" s="35" t="s">
+        <v>303</v>
+      </c>
+      <c r="C102" s="27" t="s">
+        <v>304</v>
+      </c>
+      <c r="D102" s="27" t="s">
+        <v>306</v>
+      </c>
+      <c r="E102" s="27" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="60">
+      <c r="A103" s="38"/>
+      <c r="B103" s="36"/>
+      <c r="C103" s="27" t="s">
+        <v>305</v>
+      </c>
+      <c r="D103" s="28" t="s">
+        <v>307</v>
+      </c>
+      <c r="E103" s="27" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="60">
+      <c r="A104" s="38"/>
+      <c r="B104" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="C104" s="27" t="s">
+        <v>308</v>
+      </c>
+      <c r="D104" s="27" t="s">
+        <v>316</v>
+      </c>
+      <c r="E104" s="27" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="45">
+      <c r="A105" s="38"/>
+      <c r="B105" s="29" t="s">
+        <v>312</v>
+      </c>
+      <c r="C105" s="27" t="s">
+        <v>311</v>
+      </c>
+      <c r="D105" s="27" t="s">
+        <v>310</v>
+      </c>
+      <c r="E105" s="27" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="15" customHeight="1">
+      <c r="A106" s="39"/>
+      <c r="B106" s="29" t="s">
         <v>315</v>
       </c>
-      <c r="B102" s="51" t="s">
-        <v>316</v>
-      </c>
-      <c r="C102" s="52" t="s">
-        <v>317</v>
-      </c>
-      <c r="D102" s="52" t="s">
-        <v>319</v>
-      </c>
-      <c r="E102" s="52" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" ht="60">
-      <c r="A103" s="53"/>
-      <c r="B103" s="54"/>
-      <c r="C103" s="52" t="s">
-        <v>318</v>
-      </c>
-      <c r="D103" s="55" t="s">
-        <v>320</v>
-      </c>
-      <c r="E103" s="52" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" ht="60">
-      <c r="A104" s="53"/>
-      <c r="B104" s="56" t="s">
-        <v>322</v>
-      </c>
-      <c r="C104" s="52" t="s">
-        <v>321</v>
-      </c>
-      <c r="D104" s="52" t="s">
-        <v>329</v>
-      </c>
-      <c r="E104" s="52" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" ht="45">
-      <c r="A105" s="53"/>
-      <c r="B105" s="56" t="s">
-        <v>325</v>
-      </c>
-      <c r="C105" s="52" t="s">
-        <v>324</v>
-      </c>
-      <c r="D105" s="52" t="s">
-        <v>323</v>
-      </c>
-      <c r="E105" s="52" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" ht="15" customHeight="1">
-      <c r="A106" s="57"/>
-      <c r="B106" s="56" t="s">
-        <v>328</v>
-      </c>
-      <c r="C106" s="52" t="s">
-        <v>326</v>
-      </c>
-      <c r="D106" s="52" t="s">
-        <v>327</v>
-      </c>
-      <c r="E106" s="52" t="s">
-        <v>238</v>
+      <c r="C106" s="27" t="s">
+        <v>313</v>
+      </c>
+      <c r="D106" s="27" t="s">
+        <v>314</v>
+      </c>
+      <c r="E106" s="27" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="15" customHeight="1">
@@ -3456,37 +3462,6 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="B102:B103"/>
-    <mergeCell ref="A102:A106"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="A11:A21"/>
-    <mergeCell ref="A22:A31"/>
-    <mergeCell ref="A35:A51"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="A55:A66"/>
-    <mergeCell ref="A67:A75"/>
-    <mergeCell ref="A76:A88"/>
-    <mergeCell ref="A89:A96"/>
-    <mergeCell ref="A97:A101"/>
-    <mergeCell ref="B11:B16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="B59:B62"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="B71:B73"/>
-    <mergeCell ref="B74:B75"/>
     <mergeCell ref="B93:B96"/>
     <mergeCell ref="B97:B98"/>
     <mergeCell ref="B99:B101"/>
@@ -3495,6 +3470,37 @@
     <mergeCell ref="B84:B86"/>
     <mergeCell ref="B87:B88"/>
     <mergeCell ref="B89:B92"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="B71:B73"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="B11:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A11:A21"/>
+    <mergeCell ref="A22:A31"/>
+    <mergeCell ref="A35:A51"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="B102:B103"/>
+    <mergeCell ref="A102:A106"/>
+    <mergeCell ref="A55:A66"/>
+    <mergeCell ref="A67:A75"/>
+    <mergeCell ref="A76:A88"/>
+    <mergeCell ref="A89:A96"/>
+    <mergeCell ref="A97:A101"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="B59:B62"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" sqref="A35:A40"/>
@@ -3506,10 +3512,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3522,27 +3528,27 @@
   <sheetData>
     <row r="1" spans="1:4" ht="40.5">
       <c r="A1" s="1" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="56.25">
       <c r="A2" s="3" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="D2" s="5">
         <v>45760</v>
@@ -3550,13 +3556,13 @@
     </row>
     <row r="3" spans="1:4" ht="56.25">
       <c r="A3" s="3" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c r="D3" s="5">
         <v>45765</v>
@@ -3564,13 +3570,13 @@
     </row>
     <row r="4" spans="1:4" ht="37.5">
       <c r="A4" s="3" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c r="D4" s="5">
         <v>45766</v>
@@ -3578,13 +3584,13 @@
     </row>
     <row r="5" spans="1:4" ht="75">
       <c r="A5" s="3" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="D5" s="5">
         <v>45773</v>
@@ -3592,13 +3598,13 @@
     </row>
     <row r="6" spans="1:4" ht="37.5">
       <c r="A6" s="3" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="D6" s="5">
         <v>45773</v>
@@ -3606,13 +3612,13 @@
     </row>
     <row r="7" spans="1:4" ht="37.5">
       <c r="A7" s="3" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="D7" s="5">
         <v>45780</v>
@@ -3620,13 +3626,13 @@
     </row>
     <row r="8" spans="1:4" ht="37.5">
       <c r="A8" s="3" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="D8" s="5">
         <v>45781</v>
@@ -3634,13 +3640,13 @@
     </row>
     <row r="9" spans="1:4" ht="37.5">
       <c r="A9" s="3" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="D9" s="5">
         <v>45784</v>
@@ -3648,13 +3654,13 @@
     </row>
     <row r="10" spans="1:4" ht="37.5">
       <c r="A10" s="3" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
       <c r="D10" s="5">
         <v>45785</v>
@@ -3662,13 +3668,13 @@
     </row>
     <row r="11" spans="1:4" ht="37.5">
       <c r="A11" s="3" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="D11" s="5">
         <v>45786</v>
@@ -3676,13 +3682,13 @@
     </row>
     <row r="12" spans="1:4" ht="37.5">
       <c r="A12" s="3" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="D12" s="5">
         <v>45786</v>
@@ -3690,13 +3696,13 @@
     </row>
     <row r="13" spans="1:4" ht="18.75">
       <c r="A13" s="3" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="D13" s="5">
         <v>45786</v>
@@ -3704,13 +3710,13 @@
     </row>
     <row r="14" spans="1:4" ht="18.75">
       <c r="A14" s="3" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="D14" s="5">
         <v>45786</v>
@@ -3718,13 +3724,13 @@
     </row>
     <row r="15" spans="1:4" ht="37.5">
       <c r="A15" s="3" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="D15" s="5">
         <v>45787</v>
@@ -3732,13 +3738,13 @@
     </row>
     <row r="16" spans="1:4" ht="37.5">
       <c r="A16" s="3" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
       <c r="D16" s="5">
         <v>45787</v>
@@ -3746,13 +3752,13 @@
     </row>
     <row r="17" spans="1:4" ht="37.5">
       <c r="A17" s="3" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="D17" s="5">
         <v>45787</v>
@@ -3760,15 +3766,29 @@
     </row>
     <row r="18" spans="1:4" ht="37.5">
       <c r="A18" s="3" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
       <c r="D18" s="5">
+        <v>45787</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="37.5">
+      <c r="A19" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="D19" s="5">
         <v>45787</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v3.3 Removed out of scope features
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_SRS.xlsx
+++ b/LH_REQUIREMENTS/LH_SRS.xlsx
@@ -1,37 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halae\OneDrive\Desktop\Group-3-Learning-hub-dev\Group-3-Learning-hub-dev\LH_REQUIREMENTS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mego\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E903EB5-4F3B-4E91-902B-CC4643F3DA11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LH_SRS" sheetId="1" r:id="rId1"/>
     <sheet name="LH_SRS_VERSION_HISTORY" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="324">
   <si>
     <t>Feature</t>
   </si>
@@ -477,36 +467,6 @@
   </si>
   <si>
     <t>The system shall ensure that refreshing the "Delete User" page does not disrupt its functionality and shall continue to allow the admin to perform a new user search immediately after the page reloads.</t>
-  </si>
-  <si>
-    <t>Navigation</t>
-  </si>
-  <si>
-    <t>LH-CRS-NAVIGATION-001</t>
-  </si>
-  <si>
-    <t>LH-SRS-NAV-001</t>
-  </si>
-  <si>
-    <t>The system allow users to navigate between four predefined content categories  ( ‘Sports’, ‘Scientific’,'Health','Economy').</t>
-  </si>
-  <si>
-    <t>LH-CRS-NAVIGATION-002</t>
-  </si>
-  <si>
-    <t>LH-SRS-NAV-002</t>
-  </si>
-  <si>
-    <t>The system include a header navigation bar with tabs for each section and clickable dropdowns for subsections.</t>
-  </si>
-  <si>
-    <t>LH-CRS-NAVIGATION-003</t>
-  </si>
-  <si>
-    <t>LH-SRS-NAV-003</t>
-  </si>
-  <si>
-    <t>The system shall restrict content categories to exactly four (4) with no additions/deletions by users.</t>
   </si>
   <si>
     <t>Publish Article</t>
@@ -1199,11 +1159,17 @@
   <si>
     <t>Adjusted the [Publish video] after get comments</t>
   </si>
+  <si>
+    <t>v3.3</t>
+  </si>
+  <si>
+    <t>Removed out of scope features</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="15">
     <font>
       <sz val="11"/>
@@ -1454,7 +1420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1543,12 +1509,45 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1558,6 +1557,15 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1573,59 +1581,26 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1901,24 +1876,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G108"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="79" zoomScaleNormal="111" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:A51"/>
+    <sheetView topLeftCell="A94" zoomScale="79" zoomScaleNormal="111" workbookViewId="0">
+      <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="53.42578125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" style="7" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="7"/>
+    <col min="1" max="1" width="19.88671875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="29.5546875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="53.44140625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="23.109375" style="7" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5">
+    <row r="1" spans="1:5" ht="19.8">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1935,8 +1910,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="60">
-      <c r="A2" s="32" t="s">
+    <row r="2" spans="1:5" ht="57.6">
+      <c r="A2" s="43" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="14" t="s">
@@ -1946,14 +1921,14 @@
         <v>7</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30">
-      <c r="A3" s="33"/>
+    <row r="3" spans="1:5">
+      <c r="A3" s="44"/>
       <c r="B3" s="14" t="s">
         <v>9</v>
       </c>
@@ -1967,8 +1942,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30">
-      <c r="A4" s="33"/>
+    <row r="4" spans="1:5" ht="28.8">
+      <c r="A4" s="44"/>
       <c r="B4" s="14" t="s">
         <v>12</v>
       </c>
@@ -1983,7 +1958,7 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="33"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="14" t="s">
         <v>15</v>
       </c>
@@ -1997,8 +1972,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30">
-      <c r="A6" s="33"/>
+    <row r="6" spans="1:5" ht="28.8">
+      <c r="A6" s="44"/>
       <c r="B6" s="14" t="s">
         <v>18</v>
       </c>
@@ -2006,14 +1981,14 @@
         <v>19</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30">
-      <c r="A7" s="33"/>
+    <row r="7" spans="1:5" ht="28.8">
+      <c r="A7" s="44"/>
       <c r="B7" s="23" t="s">
         <v>20</v>
       </c>
@@ -2021,14 +1996,14 @@
         <v>21</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="33"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="23" t="s">
         <v>22</v>
       </c>
@@ -2043,7 +2018,7 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="33"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="14" t="s">
         <v>25</v>
       </c>
@@ -2051,14 +2026,14 @@
         <v>26</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="33"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="23" t="s">
         <v>27</v>
       </c>
@@ -2072,11 +2047,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30">
-      <c r="A11" s="32" t="s">
+    <row r="11" spans="1:5" ht="28.8">
+      <c r="A11" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="39" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="14" t="s">
@@ -2089,9 +2064,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30">
-      <c r="A12" s="33"/>
-      <c r="B12" s="45"/>
+    <row r="12" spans="1:5" ht="28.8">
+      <c r="A12" s="44"/>
+      <c r="B12" s="40"/>
       <c r="C12" s="14" t="s">
         <v>35</v>
       </c>
@@ -2103,8 +2078,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="28.5" customHeight="1">
-      <c r="A13" s="33"/>
-      <c r="B13" s="45"/>
+      <c r="A13" s="44"/>
+      <c r="B13" s="40"/>
       <c r="C13" s="14" t="s">
         <v>37</v>
       </c>
@@ -2116,8 +2091,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="28.5" customHeight="1">
-      <c r="A14" s="33"/>
-      <c r="B14" s="45"/>
+      <c r="A14" s="44"/>
+      <c r="B14" s="40"/>
       <c r="C14" s="14" t="s">
         <v>39</v>
       </c>
@@ -2128,9 +2103,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30">
-      <c r="A15" s="33"/>
-      <c r="B15" s="45"/>
+    <row r="15" spans="1:5" ht="28.8">
+      <c r="A15" s="44"/>
+      <c r="B15" s="40"/>
       <c r="C15" s="14" t="s">
         <v>41</v>
       </c>
@@ -2141,9 +2116,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30">
-      <c r="A16" s="33"/>
-      <c r="B16" s="31"/>
+    <row r="16" spans="1:5" ht="28.8">
+      <c r="A16" s="44"/>
+      <c r="B16" s="41"/>
       <c r="C16" s="14" t="s">
         <v>43</v>
       </c>
@@ -2154,9 +2129,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="45">
-      <c r="A17" s="33"/>
-      <c r="B17" s="30" t="s">
+    <row r="17" spans="1:7" ht="43.2">
+      <c r="A17" s="44"/>
+      <c r="B17" s="39" t="s">
         <v>45</v>
       </c>
       <c r="C17" s="14" t="s">
@@ -2169,9 +2144,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30">
-      <c r="A18" s="33"/>
-      <c r="B18" s="31"/>
+    <row r="18" spans="1:7" ht="28.8">
+      <c r="A18" s="44"/>
+      <c r="B18" s="41"/>
       <c r="C18" s="14" t="s">
         <v>48</v>
       </c>
@@ -2182,9 +2157,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="30">
-      <c r="A19" s="33"/>
-      <c r="B19" s="30" t="s">
+    <row r="19" spans="1:7" ht="28.8">
+      <c r="A19" s="44"/>
+      <c r="B19" s="39" t="s">
         <v>50</v>
       </c>
       <c r="C19" s="14" t="s">
@@ -2197,9 +2172,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="30">
-      <c r="A20" s="33"/>
-      <c r="B20" s="45"/>
+    <row r="20" spans="1:7" ht="28.8">
+      <c r="A20" s="44"/>
+      <c r="B20" s="40"/>
       <c r="C20" s="14" t="s">
         <v>53</v>
       </c>
@@ -2210,9 +2185,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="30">
-      <c r="A21" s="34"/>
-      <c r="B21" s="31"/>
+    <row r="21" spans="1:7" ht="28.8">
+      <c r="A21" s="45"/>
+      <c r="B21" s="41"/>
       <c r="C21" s="14" t="s">
         <v>55</v>
       </c>
@@ -2223,8 +2198,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="30">
-      <c r="A22" s="40" t="s">
+    <row r="22" spans="1:7" ht="28.8">
+      <c r="A22" s="46" t="s">
         <v>57</v>
       </c>
       <c r="B22" s="15" t="s">
@@ -2240,8 +2215,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="30">
-      <c r="A23" s="41"/>
+    <row r="23" spans="1:7" ht="28.8">
+      <c r="A23" s="47"/>
       <c r="B23" s="15" t="s">
         <v>61</v>
       </c>
@@ -2256,7 +2231,7 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="41"/>
+      <c r="A24" s="47"/>
       <c r="B24" s="15" t="s">
         <v>64</v>
       </c>
@@ -2270,8 +2245,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="30">
-      <c r="A25" s="41"/>
+    <row r="25" spans="1:7" ht="28.8">
+      <c r="A25" s="47"/>
       <c r="B25" s="15" t="s">
         <v>67</v>
       </c>
@@ -2285,8 +2260,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="30">
-      <c r="A26" s="41"/>
+    <row r="26" spans="1:7" ht="28.8">
+      <c r="A26" s="47"/>
       <c r="B26" s="15" t="s">
         <v>70</v>
       </c>
@@ -2300,8 +2275,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="30">
-      <c r="A27" s="41"/>
+    <row r="27" spans="1:7" ht="28.8">
+      <c r="A27" s="47"/>
       <c r="B27" s="15" t="s">
         <v>73</v>
       </c>
@@ -2315,8 +2290,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="30">
-      <c r="A28" s="41"/>
+    <row r="28" spans="1:7" ht="28.8">
+      <c r="A28" s="47"/>
       <c r="B28" s="15" t="s">
         <v>76</v>
       </c>
@@ -2324,14 +2299,14 @@
         <v>77</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="E28" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="30">
-      <c r="A29" s="41"/>
+    <row r="29" spans="1:7" ht="28.8">
+      <c r="A29" s="47"/>
       <c r="B29" s="15" t="s">
         <v>78</v>
       </c>
@@ -2345,8 +2320,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="30">
-      <c r="A30" s="41"/>
+    <row r="30" spans="1:7" ht="28.8">
+      <c r="A30" s="47"/>
       <c r="B30" s="15" t="s">
         <v>81</v>
       </c>
@@ -2360,8 +2335,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="30">
-      <c r="A31" s="42"/>
+    <row r="31" spans="1:7" ht="28.8">
+      <c r="A31" s="48"/>
       <c r="B31" s="15" t="s">
         <v>84</v>
       </c>
@@ -2375,8 +2350,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="30">
-      <c r="A32" s="32" t="s">
+    <row r="32" spans="1:7" ht="28.8">
+      <c r="A32" s="43" t="s">
         <v>87</v>
       </c>
       <c r="B32" s="14" t="s">
@@ -2395,38 +2370,38 @@
       <c r="G32" s="16"/>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1">
-      <c r="A33" s="33"/>
+      <c r="A33" s="44"/>
       <c r="B33" s="14" t="s">
-        <v>296</v>
-      </c>
-      <c r="C33" s="30" t="s">
-        <v>295</v>
-      </c>
-      <c r="D33" s="30" t="s">
-        <v>298</v>
-      </c>
-      <c r="E33" s="30" t="s">
-        <v>225</v>
+        <v>286</v>
+      </c>
+      <c r="C33" s="39" t="s">
+        <v>285</v>
+      </c>
+      <c r="D33" s="39" t="s">
+        <v>288</v>
+      </c>
+      <c r="E33" s="39" t="s">
+        <v>215</v>
       </c>
       <c r="F33" s="16"/>
       <c r="G33" s="16"/>
     </row>
     <row r="34" spans="1:7" ht="75" customHeight="1">
-      <c r="A34" s="34"/>
+      <c r="A34" s="45"/>
       <c r="B34" s="14" t="s">
-        <v>297</v>
-      </c>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
+        <v>287</v>
+      </c>
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="41"/>
       <c r="F34" s="16"/>
       <c r="G34" s="16"/>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1">
-      <c r="A35" s="40" t="s">
+      <c r="A35" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="B35" s="46" t="s">
+      <c r="B35" s="42" t="s">
         <v>93</v>
       </c>
       <c r="C35" s="15" t="s">
@@ -2440,8 +2415,8 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1">
-      <c r="A36" s="41"/>
-      <c r="B36" s="46"/>
+      <c r="A36" s="47"/>
+      <c r="B36" s="42"/>
       <c r="C36" s="15" t="s">
         <v>96</v>
       </c>
@@ -2453,8 +2428,8 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1">
-      <c r="A37" s="41"/>
-      <c r="B37" s="46" t="s">
+      <c r="A37" s="47"/>
+      <c r="B37" s="42" t="s">
         <v>98</v>
       </c>
       <c r="C37" s="15" t="s">
@@ -2468,8 +2443,8 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1">
-      <c r="A38" s="41"/>
-      <c r="B38" s="46"/>
+      <c r="A38" s="47"/>
+      <c r="B38" s="42"/>
       <c r="C38" s="15" t="s">
         <v>101</v>
       </c>
@@ -2481,7 +2456,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1">
-      <c r="A39" s="41"/>
+      <c r="A39" s="47"/>
       <c r="B39" s="24" t="s">
         <v>103</v>
       </c>
@@ -2496,7 +2471,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1">
-      <c r="A40" s="41"/>
+      <c r="A40" s="47"/>
       <c r="B40" s="24" t="s">
         <v>106</v>
       </c>
@@ -2510,8 +2485,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="30">
-      <c r="A41" s="41"/>
+    <row r="41" spans="1:7" ht="28.8">
+      <c r="A41" s="47"/>
       <c r="B41" s="24" t="s">
         <v>109</v>
       </c>
@@ -2525,9 +2500,9 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="30">
-      <c r="A42" s="41"/>
-      <c r="B42" s="47" t="s">
+    <row r="42" spans="1:7" ht="28.8">
+      <c r="A42" s="47"/>
+      <c r="B42" s="56" t="s">
         <v>112</v>
       </c>
       <c r="C42" s="15" t="s">
@@ -2540,9 +2515,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="45">
-      <c r="A43" s="41"/>
-      <c r="B43" s="48"/>
+    <row r="43" spans="1:7" ht="28.8">
+      <c r="A43" s="47"/>
+      <c r="B43" s="57"/>
       <c r="C43" s="15" t="s">
         <v>115</v>
       </c>
@@ -2553,9 +2528,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="30">
-      <c r="A44" s="41"/>
-      <c r="B44" s="47" t="s">
+    <row r="44" spans="1:7" ht="28.8">
+      <c r="A44" s="47"/>
+      <c r="B44" s="56" t="s">
         <v>117</v>
       </c>
       <c r="C44" s="15" t="s">
@@ -2568,9 +2543,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="30">
-      <c r="A45" s="41"/>
-      <c r="B45" s="48"/>
+    <row r="45" spans="1:7" ht="28.8">
+      <c r="A45" s="47"/>
+      <c r="B45" s="57"/>
       <c r="C45" s="15" t="s">
         <v>120</v>
       </c>
@@ -2581,8 +2556,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="30">
-      <c r="A46" s="41"/>
+    <row r="46" spans="1:7" ht="28.8">
+      <c r="A46" s="47"/>
       <c r="B46" s="24" t="s">
         <v>122</v>
       </c>
@@ -2596,8 +2571,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="30">
-      <c r="A47" s="41"/>
+    <row r="47" spans="1:7" ht="28.8">
+      <c r="A47" s="47"/>
       <c r="B47" s="24" t="s">
         <v>125</v>
       </c>
@@ -2611,8 +2586,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="30">
-      <c r="A48" s="41"/>
+    <row r="48" spans="1:7" ht="28.8">
+      <c r="A48" s="47"/>
       <c r="B48" s="24" t="s">
         <v>128</v>
       </c>
@@ -2626,8 +2601,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="30">
-      <c r="A49" s="41"/>
+    <row r="49" spans="1:5" ht="28.8">
+      <c r="A49" s="47"/>
       <c r="B49" s="24" t="s">
         <v>131</v>
       </c>
@@ -2641,9 +2616,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="45">
-      <c r="A50" s="41"/>
-      <c r="B50" s="47" t="s">
+    <row r="50" spans="1:5" ht="28.8">
+      <c r="A50" s="47"/>
+      <c r="B50" s="56" t="s">
         <v>134</v>
       </c>
       <c r="C50" s="15" t="s">
@@ -2656,9 +2631,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="60">
-      <c r="A51" s="41"/>
-      <c r="B51" s="48"/>
+    <row r="51" spans="1:5" ht="57.6">
+      <c r="A51" s="47"/>
+      <c r="B51" s="57"/>
       <c r="C51" s="15" t="s">
         <v>137</v>
       </c>
@@ -2669,841 +2644,794 @@
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="45">
-      <c r="A52" s="32" t="s">
+    <row r="52" spans="1:5" ht="28.8">
+      <c r="A52" s="46" t="s">
         <v>139</v>
       </c>
-      <c r="B52" s="14" t="s">
+      <c r="B52" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="C52" s="14" t="s">
+      <c r="C52" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="D52" s="14" t="s">
+      <c r="D52" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="E52" s="14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="30">
-      <c r="A53" s="33"/>
-      <c r="B53" s="14" t="s">
+      <c r="E52" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="28.8">
+      <c r="A53" s="47"/>
+      <c r="B53" s="34"/>
+      <c r="C53" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="C53" s="14" t="s">
+      <c r="D53" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="D53" s="14" t="s">
+      <c r="E53" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="28.8">
+      <c r="A54" s="47"/>
+      <c r="B54" s="34"/>
+      <c r="C54" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="E53" s="14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="30">
-      <c r="A54" s="33"/>
-      <c r="B54" s="14" t="s">
+      <c r="D54" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="C54" s="14" t="s">
+      <c r="E54" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="28.8">
+      <c r="A55" s="47"/>
+      <c r="B55" s="35"/>
+      <c r="C55" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="D54" s="14" t="s">
+      <c r="D55" s="15" t="s">
         <v>148</v>
-      </c>
-      <c r="E54" s="14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="30">
-      <c r="A55" s="40" t="s">
-        <v>149</v>
-      </c>
-      <c r="B55" s="49" t="s">
-        <v>150</v>
-      </c>
-      <c r="C55" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="D55" s="15" t="s">
-        <v>152</v>
       </c>
       <c r="E55" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="30">
-      <c r="A56" s="41"/>
-      <c r="B56" s="50"/>
+    <row r="56" spans="1:5" ht="28.8">
+      <c r="A56" s="47"/>
+      <c r="B56" s="33" t="s">
+        <v>149</v>
+      </c>
       <c r="C56" s="15" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E56" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="30">
-      <c r="A57" s="41"/>
-      <c r="B57" s="50"/>
+    <row r="57" spans="1:5" ht="28.8">
+      <c r="A57" s="47"/>
+      <c r="B57" s="34"/>
       <c r="C57" s="15" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D57" s="15" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E57" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="30">
-      <c r="A58" s="41"/>
-      <c r="B58" s="51"/>
+    <row r="58" spans="1:5" ht="43.2">
+      <c r="A58" s="47"/>
+      <c r="B58" s="34"/>
       <c r="C58" s="15" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D58" s="15" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E58" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="30">
-      <c r="A59" s="41"/>
-      <c r="B59" s="49" t="s">
-        <v>159</v>
-      </c>
+    <row r="59" spans="1:5" ht="28.8">
+      <c r="A59" s="47"/>
+      <c r="B59" s="35"/>
       <c r="C59" s="15" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D59" s="15" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E59" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="30">
-      <c r="A60" s="41"/>
-      <c r="B60" s="50"/>
+    <row r="60" spans="1:5" ht="43.2">
+      <c r="A60" s="47"/>
+      <c r="B60" s="25" t="s">
+        <v>158</v>
+      </c>
       <c r="C60" s="15" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D60" s="15" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E60" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="45">
-      <c r="A61" s="41"/>
-      <c r="B61" s="50"/>
+    <row r="61" spans="1:5" ht="43.2">
+      <c r="A61" s="47"/>
+      <c r="B61" s="25" t="s">
+        <v>161</v>
+      </c>
       <c r="C61" s="15" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D61" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E61" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="45">
-      <c r="A62" s="41"/>
-      <c r="B62" s="51"/>
+    <row r="62" spans="1:5" ht="28.8">
+      <c r="A62" s="47"/>
+      <c r="B62" s="33" t="s">
+        <v>164</v>
+      </c>
       <c r="C62" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="D62" s="15" t="s">
         <v>166</v>
-      </c>
-      <c r="D62" s="15" t="s">
-        <v>167</v>
       </c>
       <c r="E62" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="45">
-      <c r="A63" s="41"/>
-      <c r="B63" s="25" t="s">
+    <row r="63" spans="1:5" ht="43.2">
+      <c r="A63" s="48"/>
+      <c r="B63" s="35"/>
+      <c r="C63" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="D63" s="15" t="s">
         <v>168</v>
-      </c>
-      <c r="C63" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="D63" s="15" t="s">
-        <v>170</v>
       </c>
       <c r="E63" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="45">
-      <c r="A64" s="41"/>
-      <c r="B64" s="25" t="s">
+    <row r="64" spans="1:5" ht="28.8">
+      <c r="A64" s="43" t="s">
+        <v>169</v>
+      </c>
+      <c r="B64" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="C64" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="C64" s="15" t="s">
+      <c r="D64" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="D64" s="15" t="s">
+      <c r="E64" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="28.8">
+      <c r="A65" s="44"/>
+      <c r="B65" s="38"/>
+      <c r="C65" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="E64" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="30">
-      <c r="A65" s="41"/>
-      <c r="B65" s="49" t="s">
+      <c r="D65" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="C65" s="15" t="s">
+      <c r="E65" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="28.8">
+      <c r="A66" s="44"/>
+      <c r="B66" s="30" t="s">
         <v>175</v>
       </c>
-      <c r="D65" s="15" t="s">
+      <c r="C66" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="E65" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="45">
-      <c r="A66" s="42"/>
-      <c r="B66" s="51"/>
-      <c r="C66" s="15" t="s">
+      <c r="D66" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="D66" s="15" t="s">
+      <c r="E66" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="28.8">
+      <c r="A67" s="44"/>
+      <c r="B67" s="38"/>
+      <c r="C67" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="E66" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="30">
-      <c r="A67" s="32" t="s">
+      <c r="D67" s="14" t="s">
         <v>179</v>
-      </c>
-      <c r="B67" s="52" t="s">
-        <v>180</v>
-      </c>
-      <c r="C67" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="D67" s="14" t="s">
-        <v>182</v>
       </c>
       <c r="E67" s="14" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="30">
-      <c r="A68" s="33"/>
-      <c r="B68" s="53"/>
+    <row r="68" spans="1:5" ht="28.8">
+      <c r="A68" s="44"/>
+      <c r="B68" s="30" t="s">
+        <v>180</v>
+      </c>
       <c r="C68" s="14" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E68" s="14" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="30">
-      <c r="A69" s="33"/>
-      <c r="B69" s="52" t="s">
-        <v>185</v>
-      </c>
+    <row r="69" spans="1:5" ht="28.8">
+      <c r="A69" s="44"/>
+      <c r="B69" s="31"/>
       <c r="C69" s="14" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E69" s="14" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="30">
-      <c r="A70" s="33"/>
-      <c r="B70" s="53"/>
+    <row r="70" spans="1:5" ht="28.8">
+      <c r="A70" s="44"/>
+      <c r="B70" s="31"/>
       <c r="C70" s="14" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E70" s="14" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="30">
-      <c r="A71" s="33"/>
-      <c r="B71" s="52" t="s">
-        <v>190</v>
+    <row r="71" spans="1:5" ht="28.8">
+      <c r="A71" s="44"/>
+      <c r="B71" s="30" t="s">
+        <v>187</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E71" s="14" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="30">
-      <c r="A72" s="33"/>
-      <c r="B72" s="54"/>
+    <row r="72" spans="1:5" ht="28.8">
+      <c r="A72" s="44"/>
+      <c r="B72" s="38"/>
       <c r="C72" s="14" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E72" s="14" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="30">
-      <c r="A73" s="33"/>
-      <c r="B73" s="54"/>
-      <c r="C73" s="14" t="s">
+    <row r="73" spans="1:5" ht="28.8">
+      <c r="A73" s="54" t="s">
+        <v>192</v>
+      </c>
+      <c r="B73" s="33" t="s">
+        <v>193</v>
+      </c>
+      <c r="C73" s="22" t="s">
+        <v>307</v>
+      </c>
+      <c r="D73" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="E73" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="D73" s="14" t="s">
+    </row>
+    <row r="74" spans="1:5" ht="28.8">
+      <c r="A74" s="54"/>
+      <c r="B74" s="34"/>
+      <c r="C74" s="22" t="s">
+        <v>308</v>
+      </c>
+      <c r="D74" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="E74" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="28.8">
+      <c r="A75" s="54"/>
+      <c r="B75" s="34"/>
+      <c r="C75" s="22" t="s">
+        <v>309</v>
+      </c>
+      <c r="D75" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="E73" s="14" t="s">
+      <c r="E75" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="28.8">
+      <c r="A76" s="54"/>
+      <c r="B76" s="34"/>
+      <c r="C76" s="22" t="s">
+        <v>310</v>
+      </c>
+      <c r="D76" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="E76" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="43.2">
+      <c r="A77" s="54"/>
+      <c r="B77" s="34"/>
+      <c r="C77" s="22" t="s">
+        <v>311</v>
+      </c>
+      <c r="D77" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="E77" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="43.2">
+      <c r="A78" s="54"/>
+      <c r="B78" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="C78" s="22" t="s">
+        <v>312</v>
+      </c>
+      <c r="D78" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E78" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="43.2">
+      <c r="A79" s="54"/>
+      <c r="B79" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="C79" s="22" t="s">
+        <v>313</v>
+      </c>
+      <c r="D79" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E79" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="43.2">
+      <c r="A80" s="54"/>
+      <c r="B80" s="35"/>
+      <c r="C80" s="22" t="s">
+        <v>314</v>
+      </c>
+      <c r="D80" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="E80" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="43.2">
+      <c r="A81" s="54"/>
+      <c r="B81" s="33" t="s">
+        <v>204</v>
+      </c>
+      <c r="C81" s="22" t="s">
+        <v>315</v>
+      </c>
+      <c r="D81" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="E81" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="54"/>
+      <c r="B82" s="34"/>
+      <c r="C82" s="22" t="s">
+        <v>316</v>
+      </c>
+      <c r="D82" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="E82" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="28.8">
+      <c r="A83" s="54"/>
+      <c r="B83" s="35"/>
+      <c r="C83" s="22" t="s">
+        <v>317</v>
+      </c>
+      <c r="D83" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="E83" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="28.8">
+      <c r="A84" s="54"/>
+      <c r="B84" s="36" t="s">
+        <v>208</v>
+      </c>
+      <c r="C84" s="22" t="s">
+        <v>318</v>
+      </c>
+      <c r="D84" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="E84" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="28.8">
+      <c r="A85" s="54"/>
+      <c r="B85" s="37"/>
+      <c r="C85" s="22" t="s">
+        <v>319</v>
+      </c>
+      <c r="D85" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="E85" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="69.900000000000006" customHeight="1">
+      <c r="A86" s="43" t="s">
+        <v>211</v>
+      </c>
+      <c r="B86" s="30" t="s">
+        <v>212</v>
+      </c>
+      <c r="C86" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="D86" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="E86" s="14" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="43.2">
+      <c r="A87" s="44"/>
+      <c r="B87" s="31"/>
+      <c r="C87" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="D87" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="E87" s="14" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="43.2">
+      <c r="A88" s="44"/>
+      <c r="B88" s="31"/>
+      <c r="C88" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="D88" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="E88" s="14" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="28.8">
+      <c r="A89" s="44"/>
+      <c r="B89" s="38"/>
+      <c r="C89" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="D89" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="E89" s="14" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="50.1" customHeight="1">
+      <c r="A90" s="44"/>
+      <c r="B90" s="58" t="s">
+        <v>222</v>
+      </c>
+      <c r="C90" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="D90" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="E90" s="14" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="28.8">
+      <c r="A91" s="44"/>
+      <c r="B91" s="59"/>
+      <c r="C91" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="D91" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="E91" s="14" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="63.9" customHeight="1">
+      <c r="A92" s="44"/>
+      <c r="B92" s="60" t="s">
+        <v>227</v>
+      </c>
+      <c r="C92" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="D92" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="E92" s="14" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="43.2">
+      <c r="A93" s="44"/>
+      <c r="B93" s="60"/>
+      <c r="C93" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="D93" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="E93" s="23" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="33.6">
+      <c r="A94" s="55" t="s">
+        <v>232</v>
+      </c>
+      <c r="B94" s="32" t="s">
+        <v>233</v>
+      </c>
+      <c r="C94" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="D94" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="E94" s="17" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="30">
-      <c r="A74" s="33"/>
-      <c r="B74" s="52" t="s">
-        <v>197</v>
-      </c>
-      <c r="C74" s="14" t="s">
-        <v>198</v>
-      </c>
-      <c r="D74" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="E74" s="14" t="s">
+    <row r="95" spans="1:5" ht="33.6">
+      <c r="A95" s="55"/>
+      <c r="B95" s="32"/>
+      <c r="C95" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="D95" s="26" t="s">
+        <v>237</v>
+      </c>
+      <c r="E95" s="17" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="45">
-      <c r="A75" s="33"/>
-      <c r="B75" s="53"/>
-      <c r="C75" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="D75" s="14" t="s">
-        <v>201</v>
-      </c>
-      <c r="E75" s="14" t="s">
+    <row r="96" spans="1:5" ht="33.6">
+      <c r="A96" s="55"/>
+      <c r="B96" s="32" t="s">
+        <v>238</v>
+      </c>
+      <c r="C96" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="D96" s="26" t="s">
+        <v>240</v>
+      </c>
+      <c r="E96" s="17" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="30">
-      <c r="A76" s="43" t="s">
-        <v>202</v>
-      </c>
-      <c r="B76" s="49" t="s">
-        <v>203</v>
-      </c>
-      <c r="C76" s="22" t="s">
-        <v>317</v>
-      </c>
-      <c r="D76" s="15" t="s">
-        <v>204</v>
-      </c>
-      <c r="E76" s="15" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="30">
-      <c r="A77" s="43"/>
-      <c r="B77" s="50"/>
-      <c r="C77" s="22" t="s">
-        <v>318</v>
-      </c>
-      <c r="D77" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="E77" s="15" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="30">
-      <c r="A78" s="43"/>
-      <c r="B78" s="50"/>
-      <c r="C78" s="22" t="s">
-        <v>319</v>
-      </c>
-      <c r="D78" s="15" t="s">
-        <v>206</v>
-      </c>
-      <c r="E78" s="15" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="30">
-      <c r="A79" s="43"/>
-      <c r="B79" s="50"/>
-      <c r="C79" s="22" t="s">
-        <v>320</v>
-      </c>
-      <c r="D79" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E79" s="15" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="45">
-      <c r="A80" s="43"/>
-      <c r="B80" s="50"/>
-      <c r="C80" s="22" t="s">
-        <v>321</v>
-      </c>
-      <c r="D80" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="E80" s="15" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="45">
-      <c r="A81" s="43"/>
-      <c r="B81" s="15" t="s">
-        <v>209</v>
-      </c>
-      <c r="C81" s="22" t="s">
-        <v>322</v>
-      </c>
-      <c r="D81" s="15" t="s">
-        <v>210</v>
-      </c>
-      <c r="E81" s="15" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="45">
-      <c r="A82" s="43"/>
-      <c r="B82" s="49" t="s">
-        <v>211</v>
-      </c>
-      <c r="C82" s="22" t="s">
-        <v>323</v>
-      </c>
-      <c r="D82" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="E82" s="15" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="45">
-      <c r="A83" s="43"/>
-      <c r="B83" s="51"/>
-      <c r="C83" s="22" t="s">
-        <v>324</v>
-      </c>
-      <c r="D83" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="E83" s="15" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="45">
-      <c r="A84" s="43"/>
-      <c r="B84" s="49" t="s">
-        <v>214</v>
-      </c>
-      <c r="C84" s="22" t="s">
-        <v>325</v>
-      </c>
-      <c r="D84" s="15" t="s">
-        <v>215</v>
-      </c>
-      <c r="E84" s="15" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" ht="30">
-      <c r="A85" s="43"/>
-      <c r="B85" s="50"/>
-      <c r="C85" s="22" t="s">
-        <v>326</v>
-      </c>
-      <c r="D85" s="15" t="s">
-        <v>216</v>
-      </c>
-      <c r="E85" s="15" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="30">
-      <c r="A86" s="43"/>
-      <c r="B86" s="51"/>
-      <c r="C86" s="22" t="s">
-        <v>327</v>
-      </c>
-      <c r="D86" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="E86" s="15" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="30">
-      <c r="A87" s="43"/>
-      <c r="B87" s="56" t="s">
-        <v>218</v>
-      </c>
-      <c r="C87" s="22" t="s">
-        <v>328</v>
-      </c>
-      <c r="D87" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="E87" s="15" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="30">
-      <c r="A88" s="43"/>
-      <c r="B88" s="57"/>
-      <c r="C88" s="22" t="s">
-        <v>329</v>
-      </c>
-      <c r="D88" s="15" t="s">
-        <v>220</v>
-      </c>
-      <c r="E88" s="15" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="69.95" customHeight="1">
-      <c r="A89" s="32" t="s">
-        <v>221</v>
-      </c>
-      <c r="B89" s="52" t="s">
-        <v>222</v>
-      </c>
-      <c r="C89" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="D89" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="E89" s="14" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="45">
-      <c r="A90" s="33"/>
-      <c r="B90" s="54"/>
-      <c r="C90" s="14" t="s">
-        <v>226</v>
-      </c>
-      <c r="D90" s="21" t="s">
-        <v>227</v>
-      </c>
-      <c r="E90" s="14" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="45">
-      <c r="A91" s="33"/>
-      <c r="B91" s="54"/>
-      <c r="C91" s="14" t="s">
-        <v>228</v>
-      </c>
-      <c r="D91" s="21" t="s">
-        <v>229</v>
-      </c>
-      <c r="E91" s="14" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="30">
-      <c r="A92" s="33"/>
-      <c r="B92" s="53"/>
-      <c r="C92" s="14" t="s">
-        <v>230</v>
-      </c>
-      <c r="D92" s="21" t="s">
-        <v>231</v>
-      </c>
-      <c r="E92" s="14" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="50.1" customHeight="1">
-      <c r="A93" s="33"/>
-      <c r="B93" s="52" t="s">
-        <v>232</v>
-      </c>
-      <c r="C93" s="14" t="s">
-        <v>233</v>
-      </c>
-      <c r="D93" s="14" t="s">
-        <v>234</v>
-      </c>
-      <c r="E93" s="14" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="30">
-      <c r="A94" s="33"/>
-      <c r="B94" s="54"/>
-      <c r="C94" s="14" t="s">
-        <v>235</v>
-      </c>
-      <c r="D94" s="14" t="s">
-        <v>236</v>
-      </c>
-      <c r="E94" s="14" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" ht="63.95" customHeight="1">
-      <c r="A95" s="33"/>
-      <c r="B95" s="54" t="s">
-        <v>237</v>
-      </c>
-      <c r="C95" s="14" t="s">
-        <v>238</v>
-      </c>
-      <c r="D95" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="E95" s="14" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="45">
-      <c r="A96" s="33"/>
-      <c r="B96" s="54"/>
-      <c r="C96" s="23" t="s">
-        <v>240</v>
-      </c>
-      <c r="D96" s="23" t="s">
+    <row r="97" spans="1:5" ht="33.6">
+      <c r="A97" s="55"/>
+      <c r="B97" s="32"/>
+      <c r="C97" s="22" t="s">
         <v>241</v>
       </c>
-      <c r="E96" s="23" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="33">
-      <c r="A97" s="44" t="s">
+      <c r="D97" s="26" t="s">
         <v>242</v>
-      </c>
-      <c r="B97" s="55" t="s">
-        <v>243</v>
-      </c>
-      <c r="C97" s="22" t="s">
-        <v>244</v>
-      </c>
-      <c r="D97" s="26" t="s">
-        <v>245</v>
       </c>
       <c r="E97" s="17" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="33">
-      <c r="A98" s="44"/>
-      <c r="B98" s="55"/>
+    <row r="98" spans="1:5">
+      <c r="A98" s="55"/>
+      <c r="B98" s="32"/>
       <c r="C98" s="22" t="s">
-        <v>246</v>
-      </c>
-      <c r="D98" s="26" t="s">
-        <v>247</v>
+        <v>243</v>
+      </c>
+      <c r="D98" s="15" t="s">
+        <v>244</v>
       </c>
       <c r="E98" s="17" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="33">
-      <c r="A99" s="44"/>
-      <c r="B99" s="55" t="s">
-        <v>248</v>
-      </c>
-      <c r="C99" s="22" t="s">
-        <v>249</v>
-      </c>
-      <c r="D99" s="26" t="s">
-        <v>250</v>
-      </c>
-      <c r="E99" s="17" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" ht="33">
-      <c r="A100" s="44"/>
-      <c r="B100" s="55"/>
-      <c r="C100" s="22" t="s">
-        <v>251</v>
-      </c>
-      <c r="D100" s="26" t="s">
-        <v>252</v>
-      </c>
-      <c r="E100" s="17" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" ht="30">
-      <c r="A101" s="44"/>
-      <c r="B101" s="55"/>
-      <c r="C101" s="22" t="s">
-        <v>253</v>
-      </c>
-      <c r="D101" s="15" t="s">
-        <v>254</v>
-      </c>
-      <c r="E101" s="17" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" ht="60">
-      <c r="A102" s="37" t="s">
+    <row r="99" spans="1:5" ht="57.6">
+      <c r="A99" s="51" t="s">
+        <v>292</v>
+      </c>
+      <c r="B99" s="49" t="s">
+        <v>293</v>
+      </c>
+      <c r="C99" s="27" t="s">
+        <v>294</v>
+      </c>
+      <c r="D99" s="27" t="s">
+        <v>296</v>
+      </c>
+      <c r="E99" s="27" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="43.2">
+      <c r="A100" s="52"/>
+      <c r="B100" s="50"/>
+      <c r="C100" s="27" t="s">
+        <v>295</v>
+      </c>
+      <c r="D100" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="E100" s="27" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="57.6">
+      <c r="A101" s="52"/>
+      <c r="B101" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="C101" s="27" t="s">
+        <v>298</v>
+      </c>
+      <c r="D101" s="27" t="s">
+        <v>306</v>
+      </c>
+      <c r="E101" s="27" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="43.2">
+      <c r="A102" s="52"/>
+      <c r="B102" s="29" t="s">
         <v>302</v>
       </c>
-      <c r="B102" s="35" t="s">
+      <c r="C102" s="27" t="s">
+        <v>301</v>
+      </c>
+      <c r="D102" s="27" t="s">
+        <v>300</v>
+      </c>
+      <c r="E102" s="27" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="15" customHeight="1">
+      <c r="A103" s="53"/>
+      <c r="B103" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="C103" s="27" t="s">
         <v>303</v>
       </c>
-      <c r="C102" s="27" t="s">
+      <c r="D103" s="27" t="s">
         <v>304</v>
       </c>
-      <c r="D102" s="27" t="s">
-        <v>306</v>
-      </c>
-      <c r="E102" s="27" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" ht="60">
-      <c r="A103" s="38"/>
-      <c r="B103" s="36"/>
-      <c r="C103" s="27" t="s">
-        <v>305</v>
-      </c>
-      <c r="D103" s="28" t="s">
-        <v>307</v>
-      </c>
       <c r="E103" s="27" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" ht="60">
-      <c r="A104" s="38"/>
-      <c r="B104" s="29" t="s">
-        <v>309</v>
-      </c>
-      <c r="C104" s="27" t="s">
-        <v>308</v>
-      </c>
-      <c r="D104" s="27" t="s">
-        <v>316</v>
-      </c>
-      <c r="E104" s="27" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" ht="45">
-      <c r="A105" s="38"/>
-      <c r="B105" s="29" t="s">
-        <v>312</v>
-      </c>
-      <c r="C105" s="27" t="s">
-        <v>311</v>
-      </c>
-      <c r="D105" s="27" t="s">
-        <v>310</v>
-      </c>
-      <c r="E105" s="27" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" ht="15" customHeight="1">
-      <c r="A106" s="39"/>
-      <c r="B106" s="29" t="s">
-        <v>315</v>
-      </c>
-      <c r="C106" s="27" t="s">
-        <v>313</v>
-      </c>
-      <c r="D106" s="27" t="s">
-        <v>314</v>
-      </c>
-      <c r="E106" s="27" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" ht="15" customHeight="1">
-      <c r="A107" s="18"/>
-      <c r="B107" s="19"/>
-      <c r="C107" s="19"/>
-      <c r="D107" s="20"/>
-      <c r="E107" s="19"/>
-    </row>
-    <row r="108" spans="1:5">
-      <c r="A108" s="19"/>
+        <v>215</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="15" customHeight="1">
+      <c r="A104" s="18"/>
+      <c r="B104" s="19"/>
+      <c r="C104" s="19"/>
+      <c r="D104" s="20"/>
+      <c r="E104" s="19"/>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="B93:B96"/>
-    <mergeCell ref="B97:B98"/>
-    <mergeCell ref="B99:B101"/>
-    <mergeCell ref="B76:B80"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="B84:B86"/>
-    <mergeCell ref="B87:B88"/>
-    <mergeCell ref="B89:B92"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="B71:B73"/>
-    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="B99:B100"/>
+    <mergeCell ref="A99:A103"/>
+    <mergeCell ref="A52:A63"/>
+    <mergeCell ref="A64:A72"/>
+    <mergeCell ref="A73:A85"/>
+    <mergeCell ref="A86:A93"/>
+    <mergeCell ref="A94:A98"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B52:B55"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A11:A21"/>
+    <mergeCell ref="A22:A31"/>
+    <mergeCell ref="A35:A51"/>
     <mergeCell ref="B11:B16"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B35:B36"/>
     <mergeCell ref="B37:B38"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="A11:A21"/>
-    <mergeCell ref="A22:A31"/>
-    <mergeCell ref="A35:A51"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="B102:B103"/>
-    <mergeCell ref="A102:A106"/>
-    <mergeCell ref="A55:A66"/>
-    <mergeCell ref="A67:A75"/>
-    <mergeCell ref="A76:A88"/>
-    <mergeCell ref="A89:A96"/>
-    <mergeCell ref="A97:A101"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="B59:B62"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="B68:B70"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="B94:B95"/>
+    <mergeCell ref="B96:B98"/>
+    <mergeCell ref="B73:B77"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="B81:B83"/>
+    <mergeCell ref="B84:B85"/>
+    <mergeCell ref="B86:B89"/>
+    <mergeCell ref="B90:B91"/>
+    <mergeCell ref="B92:B93"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" sqref="A35:A40"/>
+    <dataValidation allowBlank="1" sqref="A35:A40" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -3511,284 +3439,298 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
     <col min="3" max="3" width="45" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="40.5">
+    <row r="1" spans="1:4" ht="42">
       <c r="A1" s="1" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="56.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="55.8">
       <c r="A2" s="3" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="D2" s="5">
         <v>45760</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="56.25">
+    <row r="3" spans="1:4" ht="55.8">
       <c r="A3" s="3" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="D3" s="5">
         <v>45765</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="37.5">
+    <row r="4" spans="1:4" ht="37.200000000000003">
       <c r="A4" s="3" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="D4" s="5">
         <v>45766</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="75">
+    <row r="5" spans="1:4" ht="74.400000000000006">
       <c r="A5" s="3" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="D5" s="5">
         <v>45773</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="37.5">
+    <row r="6" spans="1:4" ht="37.200000000000003">
       <c r="A6" s="3" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="D6" s="5">
         <v>45773</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="37.5">
+    <row r="7" spans="1:4" ht="37.200000000000003">
       <c r="A7" s="3" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="D7" s="5">
         <v>45780</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="37.5">
+    <row r="8" spans="1:4" ht="37.200000000000003">
       <c r="A8" s="3" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="D8" s="5">
         <v>45781</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="37.5">
+    <row r="9" spans="1:4" ht="37.200000000000003">
       <c r="A9" s="3" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="D9" s="5">
         <v>45784</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="37.5">
+    <row r="10" spans="1:4" ht="37.200000000000003">
       <c r="A10" s="3" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="D10" s="5">
         <v>45785</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="37.5">
+    <row r="11" spans="1:4" ht="37.200000000000003">
       <c r="A11" s="3" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="D11" s="5">
         <v>45786</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="37.5">
+    <row r="12" spans="1:4" ht="37.200000000000003">
       <c r="A12" s="3" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="D12" s="5">
         <v>45786</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="18.75">
+    <row r="13" spans="1:4" ht="18.600000000000001">
       <c r="A13" s="3" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="D13" s="5">
         <v>45786</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="18.75">
+    <row r="14" spans="1:4" ht="18.600000000000001">
       <c r="A14" s="3" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="D14" s="5">
         <v>45786</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="37.5">
+    <row r="15" spans="1:4" ht="37.200000000000003">
       <c r="A15" s="3" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="D15" s="5">
         <v>45787</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="37.5">
+    <row r="16" spans="1:4" ht="37.200000000000003">
       <c r="A16" s="3" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="D16" s="5">
         <v>45787</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="37.5">
+    <row r="17" spans="1:4" ht="37.200000000000003">
       <c r="A17" s="3" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="D17" s="5">
         <v>45787</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="37.5">
+    <row r="18" spans="1:4" ht="37.200000000000003">
       <c r="A18" s="3" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="D18" s="5">
         <v>45787</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="37.5">
+    <row r="19" spans="1:4" ht="37.200000000000003">
       <c r="A19" s="3" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="D19" s="5">
+        <v>45787</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="37.200000000000003">
+      <c r="A20" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="D20" s="5">
         <v>45787</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v3.5 edited a mistake
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_SRS.xlsx
+++ b/LH_REQUIREMENTS/LH_SRS.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="335">
   <si>
     <t>Feature</t>
   </si>
@@ -318,7 +318,7 @@
     <t>LH-SRS-CATEGORIES-008</t>
   </si>
   <si>
-    <t>Include a second dropdown list at the bottom of the page for publishing options.</t>
+    <t>Include a second dropdown list in the same page for publishing options.</t>
   </si>
   <si>
     <t>LH-CRS-CATEGORIES-009</t>
@@ -1200,6 +1200,12 @@
   <si>
     <t>Removed out of scope SRS</t>
   </si>
+  <si>
+    <t>v3.6</t>
+  </si>
+  <si>
+    <t>Edited a small mistake in Categories feature</t>
+  </si>
 </sst>
 </file>
 
@@ -1211,7 +1217,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="35">
+  <fonts count="34">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1285,13 +1291,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF404040"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1454,13 +1453,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -1468,8 +1460,15 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="39">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1557,12 +1556,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1932,136 +1925,136 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2119,19 +2112,19 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="49" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="49" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="49" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="49" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="49" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="49" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="49" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="49" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2164,19 +2157,19 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2200,13 +2193,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2215,7 +2208,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2224,19 +2217,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2582,8 +2575,8 @@
   <sheetPr/>
   <dimension ref="A1:G109"/>
   <sheetViews>
-    <sheetView zoomScale="82" zoomScaleNormal="82" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:A22"/>
+    <sheetView zoomScale="82" zoomScaleNormal="82" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.87619047619048" defaultRowHeight="15" outlineLevelCol="6"/>
@@ -4195,10 +4188,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="B26" sqref="B25:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -4517,6 +4510,20 @@
         <v>45792</v>
       </c>
     </row>
+    <row r="23" ht="37.5" spans="1:4">
+      <c r="A23" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="D23" s="5">
+        <v>45792</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
v3.7 Added SRS to match the change request
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_SRS.xlsx
+++ b/LH_REQUIREMENTS/LH_SRS.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halae\OneDrive\Desktop\Group-3-Learning-hub-dev\LH_REQUIREMENTS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7620" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LH_SRS" sheetId="1" r:id="rId1"/>
     <sheet name="LH_SRS_VERSION_HISTORY" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -28,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="356">
   <si>
     <t>Feature</t>
   </si>
@@ -1206,18 +1211,75 @@
   <si>
     <t>Edited a small mistake in Categories feature</t>
   </si>
+  <si>
+    <t>v3.7</t>
+  </si>
+  <si>
+    <t>Added SRS to match the change request</t>
+  </si>
+  <si>
+    <t>LH-CRS-PUBLISHARTICLE-006</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUBART-013</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUBART-014</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUBART-015</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUBART-016</t>
+  </si>
+  <si>
+    <t>if the title exceeds 40 characters show error message: title too long</t>
+  </si>
+  <si>
+    <t>each of these combined spaces counts as one char</t>
+  </si>
+  <si>
+    <t>LH-CRS-PUBLISHAUDIO-005</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUBLISHAUDIO-012</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUBLISHAUDIO-013</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUBLISHAUDIO-014</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUBLISHAUDIO-015</t>
+  </si>
+  <si>
+    <t>the title should be less than or equal 40 characters</t>
+  </si>
+  <si>
+    <t>all consecutive spaces will count and show up as one</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUBLISHVIDEO-014</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUBLISHVIDEO-015</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUBLISHVIDEO-016</t>
+  </si>
+  <si>
+    <t>LH-SRS-PUBLISHVIDEO-017</t>
+  </si>
+  <si>
+    <t>LH-CRS-PUBLISHVIDEO-006</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="34">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1309,150 +1371,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -1467,8 +1385,15 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="38">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1501,198 +1426,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.79995117038483843"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799920651875362"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.79989013336588644"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1809,254 +1554,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="50">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2100,115 +1603,34 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="49" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="49" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="49" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="49" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2223,9 +1645,6 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2253,63 +1672,118 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="50">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
-    <cellStyle name="Normal 2" xfId="49"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2567,29 +2041,29 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:G109"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView zoomScale="82" zoomScaleNormal="82" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView topLeftCell="A81" zoomScale="62" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="H90" sqref="H90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87619047619048" defaultRowHeight="15" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.5047619047619" style="9" customWidth="1"/>
-    <col min="2" max="2" width="52.3714285714286" style="9" customWidth="1"/>
-    <col min="3" max="3" width="24.8761904761905" style="9" customWidth="1"/>
-    <col min="4" max="4" width="106.12380952381" style="10" customWidth="1"/>
-    <col min="5" max="5" width="21.3714285714286" style="9" customWidth="1"/>
-    <col min="6" max="16384" width="8.87619047619048" style="9"/>
+    <col min="1" max="1" width="17.5703125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="52.42578125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="106.140625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" style="9" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" ht="19.5" spans="1:5">
+    <row r="1" spans="1:5" ht="19.5">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -2606,1545 +2080,1715 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="86.45" customHeight="1" spans="1:5">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:5" ht="86.45" customHeight="1">
+      <c r="A2" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="18"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="17" t="s">
+      <c r="A3" s="39"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" ht="45" spans="1:5">
-      <c r="A4" s="18"/>
-      <c r="B4" s="20" t="s">
+    <row r="4" spans="1:5" ht="45">
+      <c r="A4" s="39"/>
+      <c r="B4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" ht="43.15" customHeight="1" spans="1:5">
-      <c r="A5" s="18"/>
-      <c r="B5" s="21" t="s">
+    <row r="5" spans="1:5" ht="43.15" customHeight="1">
+      <c r="A5" s="39"/>
+      <c r="B5" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="18"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="17" t="s">
+      <c r="A6" s="39"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="18"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="17" t="s">
+      <c r="A7" s="39"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" ht="30" spans="1:5">
-      <c r="A8" s="18"/>
-      <c r="B8" s="23" t="s">
+    <row r="8" spans="1:5" ht="30">
+      <c r="A8" s="39"/>
+      <c r="B8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="18"/>
-      <c r="B9" s="23" t="s">
+      <c r="A9" s="39"/>
+      <c r="B9" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" ht="28.9" customHeight="1" spans="1:5">
-      <c r="A10" s="18"/>
-      <c r="B10" s="23" t="s">
+    <row r="10" spans="1:5" ht="28.9" customHeight="1">
+      <c r="A10" s="39"/>
+      <c r="B10" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="18"/>
-      <c r="B11" s="23" t="s">
+      <c r="A11" s="39"/>
+      <c r="B11" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="18"/>
-      <c r="B12" s="21" t="s">
+      <c r="A12" s="39"/>
+      <c r="B12" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="18"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="17" t="s">
+      <c r="A13" s="39"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="18"/>
-      <c r="B14" s="23" t="s">
+      <c r="A14" s="39"/>
+      <c r="B14" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" s="7" customFormat="1" spans="1:5">
-      <c r="A15" s="24" t="s">
+    <row r="15" spans="1:5" s="7" customFormat="1">
+      <c r="A15" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="D15" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="E15" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" s="7" customFormat="1" spans="1:5">
-      <c r="A16" s="27"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="26" t="s">
+    <row r="16" spans="1:5" s="7" customFormat="1">
+      <c r="A16" s="41"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="26" t="s">
+      <c r="E16" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" s="7" customFormat="1" ht="28.5" customHeight="1" spans="1:5">
-      <c r="A17" s="27"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="26" t="s">
+    <row r="17" spans="1:5" s="7" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A17" s="41"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="26" t="s">
+      <c r="D17" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="26" t="s">
+      <c r="E17" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" s="7" customFormat="1" ht="28.5" customHeight="1" spans="1:5">
-      <c r="A18" s="27"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="26" t="s">
+    <row r="18" spans="1:5" s="7" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A18" s="41"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="26" t="s">
+      <c r="D18" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="26" t="s">
+      <c r="E18" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" s="7" customFormat="1" spans="1:5">
-      <c r="A19" s="27"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="26" t="s">
+    <row r="19" spans="1:5" s="7" customFormat="1">
+      <c r="A19" s="41"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="26" t="s">
+      <c r="D19" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="E19" s="26" t="s">
+      <c r="E19" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" s="7" customFormat="1" spans="1:5">
-      <c r="A20" s="27"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="26" t="s">
+    <row r="20" spans="1:5" s="7" customFormat="1">
+      <c r="A20" s="41"/>
+      <c r="B20" s="56"/>
+      <c r="C20" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="26" t="s">
+      <c r="D20" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="E20" s="26" t="s">
+      <c r="E20" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" s="7" customFormat="1" ht="30" spans="1:5">
-      <c r="A21" s="27"/>
-      <c r="B21" s="25" t="s">
+    <row r="21" spans="1:5" s="7" customFormat="1" ht="30">
+      <c r="A21" s="41"/>
+      <c r="B21" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="D21" s="26" t="s">
+      <c r="D21" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="E21" s="26" t="s">
+      <c r="E21" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" s="7" customFormat="1" spans="1:5">
-      <c r="A22" s="27"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="26" t="s">
+    <row r="22" spans="1:5" s="7" customFormat="1">
+      <c r="A22" s="41"/>
+      <c r="B22" s="56"/>
+      <c r="C22" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="D22" s="26" t="s">
+      <c r="D22" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="E22" s="26" t="s">
+      <c r="E22" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" s="8" customFormat="1" spans="1:5">
-      <c r="A23" s="30" t="s">
+    <row r="23" spans="1:5" s="8" customFormat="1">
+      <c r="A23" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C23" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="E23" s="31" t="s">
+      <c r="E23" s="19" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" s="8" customFormat="1" spans="1:5">
-      <c r="A24" s="32"/>
-      <c r="B24" s="31" t="s">
+    <row r="24" spans="1:5" s="8" customFormat="1">
+      <c r="A24" s="43"/>
+      <c r="B24" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C24" s="31" t="s">
+      <c r="C24" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="31" t="s">
+      <c r="D24" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="31" t="s">
+      <c r="E24" s="19" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" s="8" customFormat="1" spans="1:5">
-      <c r="A25" s="32"/>
-      <c r="B25" s="31" t="s">
+    <row r="25" spans="1:5" s="8" customFormat="1">
+      <c r="A25" s="43"/>
+      <c r="B25" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C25" s="31" t="s">
+      <c r="C25" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="D25" s="31" t="s">
+      <c r="D25" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E25" s="19" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" s="8" customFormat="1" spans="1:5">
-      <c r="A26" s="32"/>
-      <c r="B26" s="31" t="s">
+    <row r="26" spans="1:5" s="8" customFormat="1">
+      <c r="A26" s="43"/>
+      <c r="B26" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="C26" s="31" t="s">
+      <c r="C26" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="D26" s="31" t="s">
+      <c r="D26" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="E26" s="31" t="s">
+      <c r="E26" s="19" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" s="8" customFormat="1" spans="1:5">
-      <c r="A27" s="32"/>
-      <c r="B27" s="31" t="s">
+    <row r="27" spans="1:5" s="8" customFormat="1">
+      <c r="A27" s="43"/>
+      <c r="B27" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="31" t="s">
+      <c r="C27" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="D27" s="31" t="s">
+      <c r="D27" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E27" s="31" t="s">
+      <c r="E27" s="19" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" s="8" customFormat="1" spans="1:5">
-      <c r="A28" s="32"/>
-      <c r="B28" s="31" t="s">
+    <row r="28" spans="1:5" s="8" customFormat="1">
+      <c r="A28" s="43"/>
+      <c r="B28" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="C28" s="31" t="s">
+      <c r="C28" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="D28" s="31" t="s">
+      <c r="D28" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="E28" s="31" t="s">
+      <c r="E28" s="19" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" s="8" customFormat="1" spans="1:5">
-      <c r="A29" s="32"/>
-      <c r="B29" s="31" t="s">
+    <row r="29" spans="1:5" s="8" customFormat="1">
+      <c r="A29" s="43"/>
+      <c r="B29" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="C29" s="31" t="s">
+      <c r="C29" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="D29" s="31" t="s">
+      <c r="D29" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="E29" s="31" t="s">
+      <c r="E29" s="19" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" s="8" customFormat="1" spans="1:5">
-      <c r="A30" s="32"/>
-      <c r="B30" s="31" t="s">
+    <row r="30" spans="1:5" s="8" customFormat="1">
+      <c r="A30" s="43"/>
+      <c r="B30" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="C30" s="31" t="s">
+      <c r="C30" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="D30" s="31" t="s">
+      <c r="D30" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="E30" s="31" t="s">
+      <c r="E30" s="19" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="31" s="8" customFormat="1" spans="1:5">
-      <c r="A31" s="32"/>
-      <c r="B31" s="31" t="s">
+    <row r="31" spans="1:5" s="8" customFormat="1">
+      <c r="A31" s="43"/>
+      <c r="B31" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="C31" s="31" t="s">
+      <c r="C31" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="D31" s="31" t="s">
+      <c r="D31" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="E31" s="31" t="s">
+      <c r="E31" s="19" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="32" s="8" customFormat="1" spans="1:5">
-      <c r="A32" s="33"/>
-      <c r="B32" s="31" t="s">
+    <row r="32" spans="1:5" s="8" customFormat="1">
+      <c r="A32" s="44"/>
+      <c r="B32" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C32" s="31" t="s">
+      <c r="C32" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="D32" s="31" t="s">
+      <c r="D32" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="E32" s="31" t="s">
+      <c r="E32" s="19" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="33" s="7" customFormat="1" ht="16.5" spans="1:7">
-      <c r="A33" s="24" t="s">
+    <row r="33" spans="1:7" s="7" customFormat="1" ht="16.5">
+      <c r="A33" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="B33" s="26" t="s">
+      <c r="B33" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="C33" s="26" t="s">
+      <c r="C33" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="D33" s="26" t="s">
+      <c r="D33" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E33" s="26" t="s">
+      <c r="E33" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="F33" s="34"/>
-      <c r="G33" s="34"/>
-    </row>
-    <row r="34" s="7" customFormat="1" ht="30" customHeight="1" spans="1:7">
-      <c r="A34" s="27"/>
-      <c r="B34" s="26" t="s">
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+    </row>
+    <row r="34" spans="1:7" s="7" customFormat="1" ht="30" customHeight="1">
+      <c r="A34" s="41"/>
+      <c r="B34" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C34" s="25" t="s">
+      <c r="C34" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="D34" s="25" t="s">
+      <c r="D34" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="E34" s="25" t="s">
+      <c r="E34" s="54" t="s">
         <v>101</v>
       </c>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-    </row>
-    <row r="35" s="7" customFormat="1" ht="75" customHeight="1" spans="1:7">
-      <c r="A35" s="35"/>
-      <c r="B35" s="26" t="s">
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+    </row>
+    <row r="35" spans="1:7" s="7" customFormat="1" ht="75" customHeight="1">
+      <c r="A35" s="45"/>
+      <c r="B35" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="34"/>
-    </row>
-    <row r="36" s="8" customFormat="1" ht="30" customHeight="1" spans="1:5">
-      <c r="A36" s="30" t="s">
+      <c r="C35" s="56"/>
+      <c r="D35" s="56"/>
+      <c r="E35" s="56"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+    </row>
+    <row r="36" spans="1:7" s="8" customFormat="1" ht="30" customHeight="1">
+      <c r="A36" s="42" t="s">
         <v>103</v>
       </c>
-      <c r="B36" s="36" t="s">
+      <c r="B36" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="C36" s="31" t="s">
+      <c r="C36" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="D36" s="31" t="s">
+      <c r="D36" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="E36" s="31" t="s">
+      <c r="E36" s="19" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="37" s="8" customFormat="1" ht="30" customHeight="1" spans="1:5">
-      <c r="A37" s="32"/>
-      <c r="B37" s="36"/>
-      <c r="C37" s="31" t="s">
+    <row r="37" spans="1:7" s="8" customFormat="1" ht="30" customHeight="1">
+      <c r="A37" s="43"/>
+      <c r="B37" s="57"/>
+      <c r="C37" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="D37" s="31" t="s">
+      <c r="D37" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="E37" s="31" t="s">
+      <c r="E37" s="19" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="38" s="8" customFormat="1" ht="30" customHeight="1" spans="1:5">
-      <c r="A38" s="32"/>
-      <c r="B38" s="36" t="s">
+    <row r="38" spans="1:7" s="8" customFormat="1" ht="30" customHeight="1">
+      <c r="A38" s="43"/>
+      <c r="B38" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="C38" s="31" t="s">
+      <c r="C38" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="D38" s="31" t="s">
+      <c r="D38" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="E38" s="31" t="s">
+      <c r="E38" s="19" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="39" s="8" customFormat="1" ht="30" customHeight="1" spans="1:5">
-      <c r="A39" s="32"/>
-      <c r="B39" s="36"/>
-      <c r="C39" s="31" t="s">
+    <row r="39" spans="1:7" s="8" customFormat="1" ht="30" customHeight="1">
+      <c r="A39" s="43"/>
+      <c r="B39" s="57"/>
+      <c r="C39" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="D39" s="31" t="s">
+      <c r="D39" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="E39" s="31" t="s">
+      <c r="E39" s="19" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="40" s="8" customFormat="1" ht="30" customHeight="1" spans="1:5">
-      <c r="A40" s="32"/>
-      <c r="B40" s="36" t="s">
+    <row r="40" spans="1:7" s="8" customFormat="1" ht="30" customHeight="1">
+      <c r="A40" s="43"/>
+      <c r="B40" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="C40" s="31" t="s">
+      <c r="C40" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="D40" s="31" t="s">
+      <c r="D40" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="E40" s="31" t="s">
+      <c r="E40" s="19" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="41" s="8" customFormat="1" ht="30" customHeight="1" spans="1:5">
-      <c r="A41" s="32"/>
-      <c r="B41" s="36" t="s">
+    <row r="41" spans="1:7" s="8" customFormat="1" ht="30" customHeight="1">
+      <c r="A41" s="43"/>
+      <c r="B41" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="C41" s="31" t="s">
+      <c r="C41" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="D41" s="31" t="s">
+      <c r="D41" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="E41" s="31" t="s">
+      <c r="E41" s="19" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="42" s="8" customFormat="1" ht="15.75" spans="1:5">
-      <c r="A42" s="32"/>
-      <c r="B42" s="36" t="s">
+    <row r="42" spans="1:7" s="8" customFormat="1" ht="15.75">
+      <c r="A42" s="43"/>
+      <c r="B42" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="C42" s="31" t="s">
+      <c r="C42" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="D42" s="31" t="s">
+      <c r="D42" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="E42" s="31" t="s">
+      <c r="E42" s="19" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="43" s="8" customFormat="1" spans="1:5">
-      <c r="A43" s="32"/>
-      <c r="B43" s="37" t="s">
+    <row r="43" spans="1:7" s="8" customFormat="1">
+      <c r="A43" s="43"/>
+      <c r="B43" s="58" t="s">
         <v>123</v>
       </c>
-      <c r="C43" s="31" t="s">
+      <c r="C43" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="D43" s="31" t="s">
+      <c r="D43" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="E43" s="31" t="s">
+      <c r="E43" s="19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="44" s="8" customFormat="1" spans="1:5">
-      <c r="A44" s="32"/>
-      <c r="B44" s="38"/>
-      <c r="C44" s="31" t="s">
+    <row r="44" spans="1:7" s="8" customFormat="1">
+      <c r="A44" s="43"/>
+      <c r="B44" s="59"/>
+      <c r="C44" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="D44" s="31" t="s">
+      <c r="D44" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="E44" s="31" t="s">
+      <c r="E44" s="19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="45" s="8" customFormat="1" spans="1:5">
-      <c r="A45" s="32"/>
-      <c r="B45" s="37" t="s">
+    <row r="45" spans="1:7" s="8" customFormat="1">
+      <c r="A45" s="43"/>
+      <c r="B45" s="58" t="s">
         <v>128</v>
       </c>
-      <c r="C45" s="31" t="s">
+      <c r="C45" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="D45" s="31" t="s">
+      <c r="D45" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="E45" s="31" t="s">
+      <c r="E45" s="19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="46" s="8" customFormat="1" spans="1:5">
-      <c r="A46" s="32"/>
-      <c r="B46" s="38"/>
-      <c r="C46" s="31" t="s">
+    <row r="46" spans="1:7" s="8" customFormat="1">
+      <c r="A46" s="43"/>
+      <c r="B46" s="59"/>
+      <c r="C46" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="D46" s="31" t="s">
+      <c r="D46" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="E46" s="31" t="s">
+      <c r="E46" s="19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="47" s="8" customFormat="1" ht="15.75" spans="1:5">
-      <c r="A47" s="32"/>
-      <c r="B47" s="36" t="s">
+    <row r="47" spans="1:7" s="8" customFormat="1" ht="15.75">
+      <c r="A47" s="43"/>
+      <c r="B47" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="C47" s="31" t="s">
+      <c r="C47" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="D47" s="31" t="s">
+      <c r="D47" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="E47" s="31" t="s">
+      <c r="E47" s="19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" s="8" customFormat="1" ht="15.75" spans="1:5">
-      <c r="A48" s="32"/>
-      <c r="B48" s="36" t="s">
+    <row r="48" spans="1:7" s="8" customFormat="1" ht="15.75">
+      <c r="A48" s="43"/>
+      <c r="B48" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="C48" s="31" t="s">
+      <c r="C48" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="D48" s="31" t="s">
+      <c r="D48" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="E48" s="31" t="s">
+      <c r="E48" s="19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" s="8" customFormat="1" ht="15.75" spans="1:5">
-      <c r="A49" s="32"/>
-      <c r="B49" s="36" t="s">
+    <row r="49" spans="1:5" s="8" customFormat="1" ht="15.75">
+      <c r="A49" s="43"/>
+      <c r="B49" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="C49" s="31" t="s">
+      <c r="C49" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="D49" s="31" t="s">
+      <c r="D49" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="E49" s="31" t="s">
+      <c r="E49" s="19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" s="8" customFormat="1" ht="15.75" spans="1:5">
-      <c r="A50" s="32"/>
-      <c r="B50" s="36" t="s">
+    <row r="50" spans="1:5" s="8" customFormat="1" ht="15.75">
+      <c r="A50" s="43"/>
+      <c r="B50" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="C50" s="31" t="s">
+      <c r="C50" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="D50" s="31" t="s">
+      <c r="D50" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="E50" s="36" t="s">
+      <c r="E50" s="21" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="51" s="8" customFormat="1" ht="15.75" spans="1:5">
-      <c r="A51" s="32"/>
-      <c r="B51" s="37" t="s">
+    <row r="51" spans="1:5" s="8" customFormat="1" ht="30">
+      <c r="A51" s="43"/>
+      <c r="B51" s="58" t="s">
         <v>145</v>
       </c>
-      <c r="C51" s="31" t="s">
+      <c r="C51" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="D51" s="31" t="s">
+      <c r="D51" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="E51" s="36" t="s">
+      <c r="E51" s="21" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="52" s="8" customFormat="1" ht="30" spans="1:5">
-      <c r="A52" s="32"/>
-      <c r="B52" s="38"/>
-      <c r="C52" s="31" t="s">
+    <row r="52" spans="1:5" s="8" customFormat="1" ht="30">
+      <c r="A52" s="43"/>
+      <c r="B52" s="59"/>
+      <c r="C52" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="D52" s="31" t="s">
+      <c r="D52" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="E52" s="36" t="s">
+      <c r="E52" s="21" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="39" t="s">
+      <c r="A53" s="46" t="s">
         <v>150</v>
       </c>
-      <c r="B53" s="40" t="s">
+      <c r="B53" s="60" t="s">
         <v>151</v>
       </c>
-      <c r="C53" s="41" t="s">
+      <c r="C53" s="22" t="s">
         <v>152</v>
       </c>
-      <c r="D53" s="41" t="s">
+      <c r="D53" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="E53" s="41" t="s">
+      <c r="E53" s="22" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="54" spans="1:5">
-      <c r="A54" s="42"/>
-      <c r="B54" s="43"/>
-      <c r="C54" s="41" t="s">
+      <c r="A54" s="47"/>
+      <c r="B54" s="61"/>
+      <c r="C54" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="D54" s="41" t="s">
+      <c r="D54" s="22" t="s">
         <v>155</v>
       </c>
-      <c r="E54" s="41" t="s">
+      <c r="E54" s="22" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="42"/>
-      <c r="B55" s="43"/>
-      <c r="C55" s="41" t="s">
+      <c r="A55" s="47"/>
+      <c r="B55" s="61"/>
+      <c r="C55" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="D55" s="41" t="s">
+      <c r="D55" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="E55" s="41" t="s">
+      <c r="E55" s="22" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="42"/>
-      <c r="B56" s="44"/>
-      <c r="C56" s="41" t="s">
+      <c r="A56" s="47"/>
+      <c r="B56" s="62"/>
+      <c r="C56" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="D56" s="41" t="s">
+      <c r="D56" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="E56" s="41" t="s">
+      <c r="E56" s="22" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="42"/>
-      <c r="B57" s="40" t="s">
+      <c r="A57" s="47"/>
+      <c r="B57" s="60" t="s">
         <v>160</v>
       </c>
-      <c r="C57" s="41" t="s">
+      <c r="C57" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="D57" s="41" t="s">
+      <c r="D57" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="E57" s="41" t="s">
+      <c r="E57" s="22" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="42"/>
-      <c r="B58" s="43"/>
-      <c r="C58" s="41" t="s">
+      <c r="A58" s="47"/>
+      <c r="B58" s="61"/>
+      <c r="C58" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="D58" s="41" t="s">
+      <c r="D58" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="E58" s="41" t="s">
+      <c r="E58" s="22" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="59" ht="30" spans="1:5">
-      <c r="A59" s="42"/>
-      <c r="B59" s="43"/>
-      <c r="C59" s="41" t="s">
+    <row r="59" spans="1:5" ht="30">
+      <c r="A59" s="47"/>
+      <c r="B59" s="61"/>
+      <c r="C59" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="D59" s="41" t="s">
+      <c r="D59" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="E59" s="41" t="s">
+      <c r="E59" s="22" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="42"/>
-      <c r="B60" s="44"/>
-      <c r="C60" s="41" t="s">
+    <row r="60" spans="1:5" ht="30">
+      <c r="A60" s="47"/>
+      <c r="B60" s="62"/>
+      <c r="C60" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="D60" s="41" t="s">
+      <c r="D60" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="E60" s="41" t="s">
+      <c r="E60" s="22" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="61" ht="30" spans="1:5">
-      <c r="A61" s="42"/>
-      <c r="B61" s="44" t="s">
+    <row r="61" spans="1:5" ht="30">
+      <c r="A61" s="47"/>
+      <c r="B61" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="C61" s="41" t="s">
+      <c r="C61" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="D61" s="41" t="s">
+      <c r="D61" s="22" t="s">
         <v>171</v>
       </c>
-      <c r="E61" s="41" t="s">
+      <c r="E61" s="22" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="62" ht="30" spans="1:5">
-      <c r="A62" s="42"/>
-      <c r="B62" s="44" t="s">
+    <row r="62" spans="1:5" ht="30">
+      <c r="A62" s="47"/>
+      <c r="B62" s="23" t="s">
         <v>172</v>
       </c>
-      <c r="C62" s="41" t="s">
+      <c r="C62" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="D62" s="41" t="s">
+      <c r="D62" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="E62" s="41" t="s">
+      <c r="E62" s="22" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="42"/>
-      <c r="B63" s="40" t="s">
+      <c r="A63" s="47"/>
+      <c r="B63" s="60" t="s">
         <v>175</v>
       </c>
-      <c r="C63" s="41" t="s">
+      <c r="C63" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="D63" s="41" t="s">
+      <c r="D63" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="E63" s="41" t="s">
+      <c r="E63" s="22" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="64" ht="30" spans="1:5">
-      <c r="A64" s="45"/>
-      <c r="B64" s="44"/>
-      <c r="C64" s="41" t="s">
+    <row r="64" spans="1:5" ht="30">
+      <c r="A64" s="47"/>
+      <c r="B64" s="62"/>
+      <c r="C64" s="22" t="s">
         <v>178</v>
       </c>
-      <c r="D64" s="41" t="s">
+      <c r="D64" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="E64" s="41" t="s">
+      <c r="E64" s="22" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="65" ht="16.5" customHeight="1" spans="1:5">
-      <c r="A65" s="15" t="s">
+    <row r="65" spans="1:5">
+      <c r="A65" s="47"/>
+      <c r="B65" s="60" t="s">
+        <v>337</v>
+      </c>
+      <c r="C65" s="22" t="s">
+        <v>338</v>
+      </c>
+      <c r="D65" s="22" t="s">
+        <v>349</v>
+      </c>
+      <c r="E65" s="22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="47"/>
+      <c r="B66" s="61"/>
+      <c r="C66" s="22" t="s">
+        <v>339</v>
+      </c>
+      <c r="D66" s="22" t="s">
+        <v>342</v>
+      </c>
+      <c r="E66" s="22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="47"/>
+      <c r="B67" s="61"/>
+      <c r="C67" s="22" t="s">
+        <v>340</v>
+      </c>
+      <c r="D67" s="22" t="s">
+        <v>350</v>
+      </c>
+      <c r="E67" s="22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="48"/>
+      <c r="B68" s="62"/>
+      <c r="C68" s="22" t="s">
+        <v>341</v>
+      </c>
+      <c r="D68" s="22" t="s">
+        <v>343</v>
+      </c>
+      <c r="E68" s="22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A69" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="B65" s="46" t="s">
+      <c r="B69" s="63" t="s">
         <v>181</v>
       </c>
-      <c r="C65" s="17" t="s">
+      <c r="C69" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="D65" s="17" t="s">
+      <c r="D69" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="E65" s="17" t="s">
+      <c r="E69" s="15" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
-      <c r="A66" s="18"/>
-      <c r="B66" s="47"/>
-      <c r="C66" s="17" t="s">
+    <row r="70" spans="1:5" ht="30">
+      <c r="A70" s="39"/>
+      <c r="B70" s="64"/>
+      <c r="C70" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="D66" s="17" t="s">
+      <c r="D70" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="E66" s="17" t="s">
+      <c r="E70" s="15" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="67" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A67" s="18"/>
-      <c r="B67" s="47"/>
-      <c r="C67" s="17" t="s">
+    <row r="71" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A71" s="39"/>
+      <c r="B71" s="64"/>
+      <c r="C71" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="D67" s="17" t="s">
+      <c r="D71" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="E67" s="17" t="s">
+      <c r="E71" s="15" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="68" ht="14.25" customHeight="1" spans="1:5">
-      <c r="A68" s="18"/>
-      <c r="B68" s="48"/>
-      <c r="C68" s="17" t="s">
+    <row r="72" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A72" s="39"/>
+      <c r="B72" s="65"/>
+      <c r="C72" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="D68" s="17" t="s">
+      <c r="D72" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="E68" s="17" t="s">
+      <c r="E72" s="15" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
-      <c r="A69" s="18"/>
-      <c r="B69" s="46" t="s">
+    <row r="73" spans="1:5" ht="30">
+      <c r="A73" s="39"/>
+      <c r="B73" s="63" t="s">
         <v>190</v>
       </c>
-      <c r="C69" s="17" t="s">
+      <c r="C73" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="D69" s="17" t="s">
+      <c r="D73" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="E69" s="17" t="s">
+      <c r="E73" s="15" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
-      <c r="A70" s="18"/>
-      <c r="B70" s="48"/>
-      <c r="C70" s="17" t="s">
+    <row r="74" spans="1:5" ht="30">
+      <c r="A74" s="39"/>
+      <c r="B74" s="65"/>
+      <c r="C74" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="D70" s="17" t="s">
+      <c r="D74" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="E70" s="17" t="s">
+      <c r="E74" s="15" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
-      <c r="A71" s="18"/>
-      <c r="B71" s="46" t="s">
+    <row r="75" spans="1:5" ht="30">
+      <c r="A75" s="39"/>
+      <c r="B75" s="63" t="s">
         <v>195</v>
       </c>
-      <c r="C71" s="17" t="s">
+      <c r="C75" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="D71" s="17" t="s">
+      <c r="D75" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="E71" s="17" t="s">
+      <c r="E75" s="15" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
-      <c r="A72" s="18"/>
-      <c r="B72" s="47"/>
-      <c r="C72" s="17" t="s">
+    <row r="76" spans="1:5" ht="30">
+      <c r="A76" s="39"/>
+      <c r="B76" s="64"/>
+      <c r="C76" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="D72" s="17" t="s">
+      <c r="D76" s="15" t="s">
         <v>199</v>
       </c>
-      <c r="E72" s="17" t="s">
+      <c r="E76" s="15" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
-      <c r="A73" s="18"/>
-      <c r="B73" s="47"/>
-      <c r="C73" s="17" t="s">
+    <row r="77" spans="1:5" ht="30">
+      <c r="A77" s="39"/>
+      <c r="B77" s="64"/>
+      <c r="C77" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="D73" s="17" t="s">
+      <c r="D77" s="15" t="s">
         <v>201</v>
       </c>
-      <c r="E73" s="17" t="s">
+      <c r="E77" s="15" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
-      <c r="A74" s="18"/>
-      <c r="B74" s="46" t="s">
+    <row r="78" spans="1:5" ht="30">
+      <c r="A78" s="39"/>
+      <c r="B78" s="63" t="s">
         <v>202</v>
       </c>
-      <c r="C74" s="17" t="s">
+      <c r="C78" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="D74" s="17" t="s">
+      <c r="D78" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="E74" s="17" t="s">
+      <c r="E78" s="15" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
-      <c r="A75" s="18"/>
-      <c r="B75" s="48"/>
-      <c r="C75" s="17" t="s">
+    <row r="79" spans="1:5" ht="30">
+      <c r="A79" s="39"/>
+      <c r="B79" s="65"/>
+      <c r="C79" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="D75" s="17" t="s">
+      <c r="D79" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="E75" s="17" t="s">
+      <c r="E79" s="15" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="76" ht="30" spans="1:5">
-      <c r="A76" s="49" t="s">
+    <row r="80" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A80" s="39"/>
+      <c r="B80" s="63" t="s">
+        <v>344</v>
+      </c>
+      <c r="C80" s="15" t="s">
+        <v>345</v>
+      </c>
+      <c r="D80" s="22" t="s">
+        <v>349</v>
+      </c>
+      <c r="E80" s="22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A81" s="39"/>
+      <c r="B81" s="64"/>
+      <c r="C81" s="15" t="s">
+        <v>346</v>
+      </c>
+      <c r="D81" s="22" t="s">
+        <v>342</v>
+      </c>
+      <c r="E81" s="22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A82" s="39"/>
+      <c r="B82" s="64"/>
+      <c r="C82" s="15" t="s">
+        <v>347</v>
+      </c>
+      <c r="D82" s="22" t="s">
+        <v>350</v>
+      </c>
+      <c r="E82" s="22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A83" s="70"/>
+      <c r="B83" s="65"/>
+      <c r="C83" s="15" t="s">
+        <v>348</v>
+      </c>
+      <c r="D83" s="22" t="s">
+        <v>343</v>
+      </c>
+      <c r="E83" s="22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="30">
+      <c r="A84" s="46" t="s">
         <v>207</v>
       </c>
-      <c r="B76" s="40" t="s">
+      <c r="B84" s="60" t="s">
         <v>208</v>
       </c>
-      <c r="C76" s="26" t="s">
+      <c r="C84" s="18" t="s">
         <v>209</v>
       </c>
-      <c r="D76" s="41" t="s">
+      <c r="D84" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="E76" s="41" t="s">
+      <c r="E84" s="22" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="77" ht="30" spans="1:5">
-      <c r="A77" s="49"/>
-      <c r="B77" s="43"/>
-      <c r="C77" s="26" t="s">
+    <row r="85" spans="1:5" ht="30">
+      <c r="A85" s="47"/>
+      <c r="B85" s="61"/>
+      <c r="C85" s="18" t="s">
         <v>212</v>
       </c>
-      <c r="D77" s="41" t="s">
+      <c r="D85" s="22" t="s">
         <v>155</v>
       </c>
-      <c r="E77" s="41" t="s">
+      <c r="E85" s="22" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="78" ht="30" spans="1:5">
-      <c r="A78" s="49"/>
-      <c r="B78" s="43"/>
-      <c r="C78" s="26" t="s">
+    <row r="86" spans="1:5" ht="30">
+      <c r="A86" s="47"/>
+      <c r="B86" s="61"/>
+      <c r="C86" s="18" t="s">
         <v>213</v>
       </c>
-      <c r="D78" s="41" t="s">
+      <c r="D86" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="E78" s="41" t="s">
+      <c r="E86" s="22" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="79" ht="30" spans="1:5">
-      <c r="A79" s="49"/>
-      <c r="B79" s="43"/>
-      <c r="C79" s="26" t="s">
+    <row r="87" spans="1:5" ht="30">
+      <c r="A87" s="47"/>
+      <c r="B87" s="61"/>
+      <c r="C87" s="18" t="s">
         <v>215</v>
       </c>
-      <c r="D79" s="41" t="s">
+      <c r="D87" s="22" t="s">
         <v>216</v>
       </c>
-      <c r="E79" s="41" t="s">
+      <c r="E87" s="22" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="80" ht="30" spans="1:5">
-      <c r="A80" s="49"/>
-      <c r="B80" s="43"/>
-      <c r="C80" s="26" t="s">
+    <row r="88" spans="1:5" ht="30">
+      <c r="A88" s="47"/>
+      <c r="B88" s="61"/>
+      <c r="C88" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="D80" s="41" t="s">
+      <c r="D88" s="22" t="s">
         <v>218</v>
       </c>
-      <c r="E80" s="41" t="s">
+      <c r="E88" s="22" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="81" ht="30" spans="1:5">
-      <c r="A81" s="49"/>
-      <c r="B81" s="41" t="s">
+    <row r="89" spans="1:5" ht="30">
+      <c r="A89" s="47"/>
+      <c r="B89" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C81" s="26" t="s">
+      <c r="C89" s="18" t="s">
         <v>220</v>
       </c>
-      <c r="D81" s="41" t="s">
+      <c r="D89" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="E81" s="41" t="s">
+      <c r="E89" s="22" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="82" ht="45" spans="1:5">
-      <c r="A82" s="49"/>
-      <c r="B82" s="40" t="s">
+    <row r="90" spans="1:5" ht="45">
+      <c r="A90" s="47"/>
+      <c r="B90" s="60" t="s">
         <v>222</v>
       </c>
-      <c r="C82" s="26" t="s">
+      <c r="C90" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="D82" s="41" t="s">
+      <c r="D90" s="22" t="s">
         <v>224</v>
       </c>
-      <c r="E82" s="41" t="s">
+      <c r="E90" s="22" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="83" ht="30" spans="1:5">
-      <c r="A83" s="49"/>
-      <c r="B83" s="44"/>
-      <c r="C83" s="26" t="s">
+    <row r="91" spans="1:5" ht="30">
+      <c r="A91" s="47"/>
+      <c r="B91" s="62"/>
+      <c r="C91" s="18" t="s">
         <v>225</v>
       </c>
-      <c r="D83" s="41" t="s">
+      <c r="D91" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="E83" s="41" t="s">
+      <c r="E91" s="22" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="84" ht="30" spans="1:5">
-      <c r="A84" s="49"/>
-      <c r="B84" s="40" t="s">
+    <row r="92" spans="1:5" ht="30">
+      <c r="A92" s="47"/>
+      <c r="B92" s="60" t="s">
         <v>227</v>
       </c>
-      <c r="C84" s="26" t="s">
+      <c r="C92" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="D84" s="41" t="s">
+      <c r="D92" s="22" t="s">
         <v>229</v>
       </c>
-      <c r="E84" s="41" t="s">
+      <c r="E92" s="22" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="85" ht="30" spans="1:5">
-      <c r="A85" s="49"/>
-      <c r="B85" s="43"/>
-      <c r="C85" s="26" t="s">
+    <row r="93" spans="1:5" ht="30">
+      <c r="A93" s="47"/>
+      <c r="B93" s="61"/>
+      <c r="C93" s="18" t="s">
         <v>230</v>
       </c>
-      <c r="D85" s="41" t="s">
+      <c r="D93" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="E85" s="41" t="s">
+      <c r="E93" s="22" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="86" ht="30" spans="1:5">
-      <c r="A86" s="49"/>
-      <c r="B86" s="44"/>
-      <c r="C86" s="26" t="s">
+    <row r="94" spans="1:5" ht="30">
+      <c r="A94" s="47"/>
+      <c r="B94" s="62"/>
+      <c r="C94" s="18" t="s">
         <v>232</v>
       </c>
-      <c r="D86" s="41" t="s">
+      <c r="D94" s="22" t="s">
         <v>233</v>
       </c>
-      <c r="E86" s="41" t="s">
+      <c r="E94" s="22" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="87" ht="30" spans="1:5">
-      <c r="A87" s="49"/>
-      <c r="B87" s="25" t="s">
+    <row r="95" spans="1:5" ht="30">
+      <c r="A95" s="47"/>
+      <c r="B95" s="54" t="s">
         <v>234</v>
       </c>
-      <c r="C87" s="26" t="s">
+      <c r="C95" s="18" t="s">
         <v>235</v>
       </c>
-      <c r="D87" s="41" t="s">
+      <c r="D95" s="22" t="s">
         <v>236</v>
       </c>
-      <c r="E87" s="41" t="s">
+      <c r="E95" s="22" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="88" ht="30" spans="1:5">
-      <c r="A88" s="49"/>
-      <c r="B88" s="29"/>
-      <c r="C88" s="26" t="s">
+    <row r="96" spans="1:5" ht="30">
+      <c r="A96" s="47"/>
+      <c r="B96" s="56"/>
+      <c r="C96" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="D88" s="41" t="s">
+      <c r="D96" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="E88" s="41" t="s">
+      <c r="E96" s="22" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="89" ht="69.95" customHeight="1" spans="1:5">
-      <c r="A89" s="15" t="s">
+    <row r="97" spans="1:5">
+      <c r="A97" s="47"/>
+      <c r="B97" s="54" t="s">
+        <v>355</v>
+      </c>
+      <c r="C97" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="D97" s="22" t="s">
+        <v>349</v>
+      </c>
+      <c r="E97" s="22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="47"/>
+      <c r="B98" s="55"/>
+      <c r="C98" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="D98" s="22" t="s">
+        <v>342</v>
+      </c>
+      <c r="E98" s="22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" s="47"/>
+      <c r="B99" s="55"/>
+      <c r="C99" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="D99" s="22" t="s">
+        <v>350</v>
+      </c>
+      <c r="E99" s="22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" s="48"/>
+      <c r="B100" s="56"/>
+      <c r="C100" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="D100" s="22" t="s">
+        <v>343</v>
+      </c>
+      <c r="E100" s="22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="69.95" customHeight="1">
+      <c r="A101" s="38" t="s">
         <v>239</v>
       </c>
-      <c r="B89" s="46" t="s">
+      <c r="B101" s="63" t="s">
         <v>240</v>
       </c>
-      <c r="C89" s="17" t="s">
+      <c r="C101" s="15" t="s">
         <v>241</v>
       </c>
-      <c r="D89" s="17" t="s">
+      <c r="D101" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="E89" s="17" t="s">
+      <c r="E101" s="15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="90" ht="45" spans="1:5">
-      <c r="A90" s="18"/>
-      <c r="B90" s="47"/>
-      <c r="C90" s="17" t="s">
+    <row r="102" spans="1:5" ht="45">
+      <c r="A102" s="39"/>
+      <c r="B102" s="64"/>
+      <c r="C102" s="15" t="s">
         <v>243</v>
       </c>
-      <c r="D90" s="50" t="s">
+      <c r="D102" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="E90" s="17" t="s">
+      <c r="E102" s="15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="91" ht="45" spans="1:5">
-      <c r="A91" s="18"/>
-      <c r="B91" s="47"/>
-      <c r="C91" s="17" t="s">
+    <row r="103" spans="1:5" ht="45">
+      <c r="A103" s="39"/>
+      <c r="B103" s="64"/>
+      <c r="C103" s="15" t="s">
         <v>245</v>
       </c>
-      <c r="D91" s="50" t="s">
+      <c r="D103" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="E91" s="17" t="s">
+      <c r="E103" s="15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="92" ht="30" spans="1:5">
-      <c r="A92" s="18"/>
-      <c r="B92" s="48"/>
-      <c r="C92" s="17" t="s">
+    <row r="104" spans="1:5" ht="30">
+      <c r="A104" s="39"/>
+      <c r="B104" s="65"/>
+      <c r="C104" s="15" t="s">
         <v>247</v>
       </c>
-      <c r="D92" s="50" t="s">
+      <c r="D104" s="24" t="s">
         <v>248</v>
       </c>
-      <c r="E92" s="17" t="s">
+      <c r="E104" s="15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="93" ht="50.1" customHeight="1" spans="1:5">
-      <c r="A93" s="18"/>
-      <c r="B93" s="46" t="s">
+    <row r="105" spans="1:5" ht="50.1" customHeight="1">
+      <c r="A105" s="39"/>
+      <c r="B105" s="63" t="s">
         <v>249</v>
       </c>
-      <c r="C93" s="17" t="s">
+      <c r="C105" s="15" t="s">
         <v>250</v>
       </c>
-      <c r="D93" s="17" t="s">
+      <c r="D105" s="15" t="s">
         <v>251</v>
       </c>
-      <c r="E93" s="17" t="s">
+      <c r="E105" s="15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="94" ht="30" spans="1:5">
-      <c r="A94" s="18"/>
-      <c r="B94" s="47"/>
-      <c r="C94" s="17" t="s">
+    <row r="106" spans="1:5" ht="30">
+      <c r="A106" s="39"/>
+      <c r="B106" s="64"/>
+      <c r="C106" s="15" t="s">
         <v>252</v>
       </c>
-      <c r="D94" s="17" t="s">
+      <c r="D106" s="15" t="s">
         <v>253</v>
       </c>
-      <c r="E94" s="17" t="s">
+      <c r="E106" s="15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="95" ht="63.95" customHeight="1" spans="1:5">
-      <c r="A95" s="18"/>
-      <c r="B95" s="51" t="s">
+    <row r="107" spans="1:5" ht="63.95" customHeight="1">
+      <c r="A107" s="39"/>
+      <c r="B107" s="66" t="s">
         <v>254</v>
       </c>
-      <c r="C95" s="17" t="s">
+      <c r="C107" s="15" t="s">
         <v>255</v>
       </c>
-      <c r="D95" s="17" t="s">
+      <c r="D107" s="15" t="s">
         <v>256</v>
       </c>
-      <c r="E95" s="17" t="s">
+      <c r="E107" s="15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="96" ht="30" spans="1:5">
-      <c r="A96" s="18"/>
-      <c r="B96" s="51"/>
-      <c r="C96" s="52" t="s">
+    <row r="108" spans="1:5" ht="30">
+      <c r="A108" s="39"/>
+      <c r="B108" s="66"/>
+      <c r="C108" s="25" t="s">
         <v>257</v>
       </c>
-      <c r="D96" s="52" t="s">
+      <c r="D108" s="25" t="s">
         <v>258</v>
       </c>
-      <c r="E96" s="52" t="s">
+      <c r="E108" s="25" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="97" ht="30" spans="1:5">
-      <c r="A97" s="53" t="s">
+    <row r="109" spans="1:5" ht="30">
+      <c r="A109" s="49" t="s">
         <v>259</v>
       </c>
-      <c r="B97" s="54" t="s">
+      <c r="B109" s="67" t="s">
         <v>260</v>
       </c>
-      <c r="C97" s="26" t="s">
+      <c r="C109" s="18" t="s">
         <v>261</v>
       </c>
-      <c r="D97" s="54" t="s">
+      <c r="D109" s="27" t="s">
         <v>262</v>
       </c>
-      <c r="E97" s="53" t="s">
+      <c r="E109" s="26" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="98" ht="30" spans="1:5">
-      <c r="A98" s="53"/>
-      <c r="B98" s="54"/>
-      <c r="C98" s="26" t="s">
+    <row r="110" spans="1:5" ht="30">
+      <c r="A110" s="49"/>
+      <c r="B110" s="67"/>
+      <c r="C110" s="18" t="s">
         <v>263</v>
       </c>
-      <c r="D98" s="54" t="s">
+      <c r="D110" s="27" t="s">
         <v>264</v>
       </c>
-      <c r="E98" s="53" t="s">
+      <c r="E110" s="26" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="99" ht="30" spans="1:5">
-      <c r="A99" s="53"/>
-      <c r="B99" s="54" t="s">
+    <row r="111" spans="1:5" ht="30">
+      <c r="A111" s="49"/>
+      <c r="B111" s="67" t="s">
         <v>265</v>
       </c>
-      <c r="C99" s="26" t="s">
+      <c r="C111" s="18" t="s">
         <v>266</v>
       </c>
-      <c r="D99" s="54" t="s">
+      <c r="D111" s="27" t="s">
         <v>267</v>
       </c>
-      <c r="E99" s="53" t="s">
+      <c r="E111" s="26" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="100" ht="30" spans="1:5">
-      <c r="A100" s="53"/>
-      <c r="B100" s="54"/>
-      <c r="C100" s="26" t="s">
+    <row r="112" spans="1:5" ht="30">
+      <c r="A112" s="49"/>
+      <c r="B112" s="67"/>
+      <c r="C112" s="18" t="s">
         <v>268</v>
       </c>
-      <c r="D100" s="54" t="s">
+      <c r="D112" s="27" t="s">
         <v>269</v>
       </c>
-      <c r="E100" s="53" t="s">
+      <c r="E112" s="26" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="101" ht="30" spans="1:5">
-      <c r="A101" s="53"/>
-      <c r="B101" s="54"/>
-      <c r="C101" s="26" t="s">
+    <row r="113" spans="1:5" ht="30">
+      <c r="A113" s="49"/>
+      <c r="B113" s="67"/>
+      <c r="C113" s="18" t="s">
         <v>270</v>
       </c>
-      <c r="D101" s="41" t="s">
+      <c r="D113" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="E101" s="53" t="s">
+      <c r="E113" s="26" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="102" ht="45" spans="1:5">
-      <c r="A102" s="30" t="s">
+    <row r="114" spans="1:5" ht="45">
+      <c r="A114" s="42" t="s">
         <v>272</v>
       </c>
-      <c r="B102" s="55" t="s">
+      <c r="B114" s="68" t="s">
         <v>273</v>
       </c>
-      <c r="C102" s="31" t="s">
+      <c r="C114" s="19" t="s">
         <v>274</v>
       </c>
-      <c r="D102" s="31" t="s">
+      <c r="D114" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="E102" s="31" t="s">
+      <c r="E114" s="19" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="103" ht="30" spans="1:5">
-      <c r="A103" s="32"/>
-      <c r="B103" s="56"/>
-      <c r="C103" s="31" t="s">
+    <row r="115" spans="1:5" ht="45">
+      <c r="A115" s="43"/>
+      <c r="B115" s="69"/>
+      <c r="C115" s="19" t="s">
         <v>276</v>
       </c>
-      <c r="D103" s="57" t="s">
+      <c r="D115" s="29" t="s">
         <v>277</v>
       </c>
-      <c r="E103" s="31" t="s">
+      <c r="E115" s="19" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="104" ht="45" spans="1:5">
-      <c r="A104" s="32"/>
-      <c r="B104" s="58" t="s">
+    <row r="116" spans="1:5" ht="45">
+      <c r="A116" s="43"/>
+      <c r="B116" s="30" t="s">
         <v>278</v>
       </c>
-      <c r="C104" s="31" t="s">
+      <c r="C116" s="19" t="s">
         <v>279</v>
       </c>
-      <c r="D104" s="31" t="s">
+      <c r="D116" s="19" t="s">
         <v>280</v>
       </c>
-      <c r="E104" s="31" t="s">
+      <c r="E116" s="19" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="105" ht="30" spans="1:5">
-      <c r="A105" s="32"/>
-      <c r="B105" s="58" t="s">
+    <row r="117" spans="1:5" ht="30">
+      <c r="A117" s="43"/>
+      <c r="B117" s="30" t="s">
         <v>281</v>
       </c>
-      <c r="C105" s="31" t="s">
+      <c r="C117" s="19" t="s">
         <v>282</v>
       </c>
-      <c r="D105" s="31" t="s">
+      <c r="D117" s="19" t="s">
         <v>283</v>
       </c>
-      <c r="E105" s="31" t="s">
+      <c r="E117" s="19" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="106" customHeight="1" spans="1:5">
-      <c r="A106" s="32"/>
-      <c r="B106" s="55" t="s">
+    <row r="118" spans="1:5" ht="15" customHeight="1">
+      <c r="A118" s="43"/>
+      <c r="B118" s="28" t="s">
         <v>284</v>
       </c>
-      <c r="C106" s="59" t="s">
+      <c r="C118" s="31" t="s">
         <v>285</v>
       </c>
-      <c r="D106" s="59" t="s">
+      <c r="D118" s="31" t="s">
         <v>286</v>
       </c>
-      <c r="E106" s="59" t="s">
+      <c r="E118" s="31" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="107" customHeight="1" spans="1:5">
-      <c r="A107" s="60"/>
-      <c r="B107" s="61"/>
-      <c r="C107" s="61"/>
-      <c r="D107" s="62"/>
-      <c r="E107" s="61"/>
-    </row>
-    <row r="108" spans="1:5">
-      <c r="A108" s="63"/>
-      <c r="B108" s="64"/>
-      <c r="C108" s="64"/>
-      <c r="D108" s="65"/>
-      <c r="E108" s="64"/>
-    </row>
-    <row r="109" spans="1:5">
-      <c r="A109" s="64"/>
-      <c r="B109" s="64"/>
-      <c r="C109" s="64"/>
-      <c r="D109" s="65"/>
-      <c r="E109" s="64"/>
+    <row r="119" spans="1:5" ht="15" customHeight="1">
+      <c r="A119" s="32"/>
+      <c r="B119" s="33"/>
+      <c r="C119" s="33"/>
+      <c r="D119" s="34"/>
+      <c r="E119" s="33"/>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120" s="35"/>
+      <c r="B120" s="36"/>
+      <c r="C120" s="36"/>
+      <c r="D120" s="37"/>
+      <c r="E120" s="36"/>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121" s="36"/>
+      <c r="B121" s="36"/>
+      <c r="C121" s="36"/>
+      <c r="D121" s="37"/>
+      <c r="E121" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="A2:A14"/>
-    <mergeCell ref="A15:A22"/>
-    <mergeCell ref="A23:A32"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A36:A52"/>
-    <mergeCell ref="A53:A64"/>
-    <mergeCell ref="A65:A75"/>
-    <mergeCell ref="A76:A88"/>
-    <mergeCell ref="A89:A96"/>
-    <mergeCell ref="A97:A101"/>
-    <mergeCell ref="A102:A106"/>
+  <mergeCells count="44">
+    <mergeCell ref="B111:B113"/>
+    <mergeCell ref="B114:B115"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B80:B83"/>
+    <mergeCell ref="B97:B100"/>
+    <mergeCell ref="B95:B96"/>
+    <mergeCell ref="B101:B104"/>
+    <mergeCell ref="B105:B106"/>
+    <mergeCell ref="B107:B108"/>
+    <mergeCell ref="B109:B110"/>
+    <mergeCell ref="B75:B77"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="B84:B88"/>
+    <mergeCell ref="B90:B91"/>
+    <mergeCell ref="B92:B94"/>
+    <mergeCell ref="A114:A118"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="B12:B13"/>
@@ -4158,51 +3802,44 @@
     <mergeCell ref="B53:B56"/>
     <mergeCell ref="B57:B60"/>
     <mergeCell ref="B63:B64"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="B71:B73"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="B76:B80"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="B84:B86"/>
-    <mergeCell ref="B87:B88"/>
-    <mergeCell ref="B89:B92"/>
-    <mergeCell ref="B93:B94"/>
-    <mergeCell ref="B95:B96"/>
-    <mergeCell ref="B97:B98"/>
-    <mergeCell ref="B99:B101"/>
-    <mergeCell ref="B102:B103"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="B69:B72"/>
+    <mergeCell ref="B73:B74"/>
+    <mergeCell ref="A101:A108"/>
+    <mergeCell ref="A109:A113"/>
+    <mergeCell ref="A53:A68"/>
+    <mergeCell ref="A69:A83"/>
+    <mergeCell ref="A84:A100"/>
+    <mergeCell ref="A2:A14"/>
+    <mergeCell ref="A15:A22"/>
+    <mergeCell ref="A23:A32"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A36:A52"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" sqref="A36:A41"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:D23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B26" sqref="B25:B26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.6285714285714" customWidth="1"/>
-    <col min="2" max="2" width="20.6285714285714" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="45" customWidth="1"/>
-    <col min="4" max="4" width="19.3714285714286" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="40.5" spans="1:4">
+    <row r="1" spans="1:4" ht="40.5">
       <c r="A1" s="1" t="s">
         <v>287</v>
       </c>
@@ -4216,7 +3853,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="2" ht="37.5" spans="1:4">
+    <row r="2" spans="1:4" ht="56.25">
       <c r="A2" s="3" t="s">
         <v>291</v>
       </c>
@@ -4230,7 +3867,7 @@
         <v>45760</v>
       </c>
     </row>
-    <row r="3" ht="56.25" spans="1:4">
+    <row r="3" spans="1:4" ht="56.25">
       <c r="A3" s="3" t="s">
         <v>293</v>
       </c>
@@ -4244,7 +3881,7 @@
         <v>45765</v>
       </c>
     </row>
-    <row r="4" ht="37.5" spans="1:4">
+    <row r="4" spans="1:4" ht="37.5">
       <c r="A4" s="3" t="s">
         <v>295</v>
       </c>
@@ -4258,7 +3895,7 @@
         <v>45766</v>
       </c>
     </row>
-    <row r="5" ht="75" spans="1:4">
+    <row r="5" spans="1:4" ht="75">
       <c r="A5" s="3" t="s">
         <v>297</v>
       </c>
@@ -4272,7 +3909,7 @@
         <v>45773</v>
       </c>
     </row>
-    <row r="6" ht="37.5" spans="1:4">
+    <row r="6" spans="1:4" ht="37.5">
       <c r="A6" s="3" t="s">
         <v>299</v>
       </c>
@@ -4286,7 +3923,7 @@
         <v>45773</v>
       </c>
     </row>
-    <row r="7" ht="37.5" spans="1:4">
+    <row r="7" spans="1:4" ht="37.5">
       <c r="A7" s="3" t="s">
         <v>301</v>
       </c>
@@ -4300,7 +3937,7 @@
         <v>45780</v>
       </c>
     </row>
-    <row r="8" ht="37.5" spans="1:4">
+    <row r="8" spans="1:4" ht="37.5">
       <c r="A8" s="3" t="s">
         <v>303</v>
       </c>
@@ -4314,7 +3951,7 @@
         <v>45781</v>
       </c>
     </row>
-    <row r="9" ht="37.5" spans="1:4">
+    <row r="9" spans="1:4" ht="37.5">
       <c r="A9" s="3" t="s">
         <v>305</v>
       </c>
@@ -4328,7 +3965,7 @@
         <v>45784</v>
       </c>
     </row>
-    <row r="10" ht="37.5" spans="1:4">
+    <row r="10" spans="1:4" ht="37.5">
       <c r="A10" s="3" t="s">
         <v>307</v>
       </c>
@@ -4342,7 +3979,7 @@
         <v>45785</v>
       </c>
     </row>
-    <row r="11" ht="37.5" spans="1:4">
+    <row r="11" spans="1:4" ht="37.5">
       <c r="A11" s="3" t="s">
         <v>309</v>
       </c>
@@ -4356,7 +3993,7 @@
         <v>45786</v>
       </c>
     </row>
-    <row r="12" ht="37.5" spans="1:4">
+    <row r="12" spans="1:4" ht="37.5">
       <c r="A12" s="3" t="s">
         <v>311</v>
       </c>
@@ -4370,7 +4007,7 @@
         <v>45786</v>
       </c>
     </row>
-    <row r="13" ht="18.75" spans="1:4">
+    <row r="13" spans="1:4" ht="18.75">
       <c r="A13" s="3" t="s">
         <v>313</v>
       </c>
@@ -4384,7 +4021,7 @@
         <v>45786</v>
       </c>
     </row>
-    <row r="14" ht="18.75" spans="1:4">
+    <row r="14" spans="1:4" ht="18.75">
       <c r="A14" s="3" t="s">
         <v>315</v>
       </c>
@@ -4398,7 +4035,7 @@
         <v>45786</v>
       </c>
     </row>
-    <row r="15" ht="37.5" spans="1:4">
+    <row r="15" spans="1:4" ht="37.5">
       <c r="A15" s="3" t="s">
         <v>317</v>
       </c>
@@ -4412,7 +4049,7 @@
         <v>45787</v>
       </c>
     </row>
-    <row r="16" ht="37.5" spans="1:4">
+    <row r="16" spans="1:4" ht="37.5">
       <c r="A16" s="3" t="s">
         <v>319</v>
       </c>
@@ -4426,7 +4063,7 @@
         <v>45787</v>
       </c>
     </row>
-    <row r="17" ht="37.5" spans="1:4">
+    <row r="17" spans="1:4" ht="37.5">
       <c r="A17" s="3" t="s">
         <v>321</v>
       </c>
@@ -4440,7 +4077,7 @@
         <v>45787</v>
       </c>
     </row>
-    <row r="18" ht="37.5" spans="1:4">
+    <row r="18" spans="1:4" ht="37.5">
       <c r="A18" s="3" t="s">
         <v>323</v>
       </c>
@@ -4454,7 +4091,7 @@
         <v>45787</v>
       </c>
     </row>
-    <row r="19" ht="37.5" spans="1:4">
+    <row r="19" spans="1:4" ht="37.5">
       <c r="A19" s="3" t="s">
         <v>325</v>
       </c>
@@ -4468,7 +4105,7 @@
         <v>45787</v>
       </c>
     </row>
-    <row r="20" ht="37.5" spans="1:4">
+    <row r="20" spans="1:4" ht="37.5">
       <c r="A20" s="3" t="s">
         <v>327</v>
       </c>
@@ -4482,7 +4119,7 @@
         <v>45787</v>
       </c>
     </row>
-    <row r="21" ht="18.75" spans="1:4">
+    <row r="21" spans="1:4" ht="37.5">
       <c r="A21" s="3" t="s">
         <v>329</v>
       </c>
@@ -4496,7 +4133,7 @@
         <v>45790</v>
       </c>
     </row>
-    <row r="22" ht="18.75" spans="1:4">
+    <row r="22" spans="1:4" ht="18.75">
       <c r="A22" s="3" t="s">
         <v>331</v>
       </c>
@@ -4510,7 +4147,7 @@
         <v>45792</v>
       </c>
     </row>
-    <row r="23" ht="37.5" spans="1:4">
+    <row r="23" spans="1:4" ht="37.5">
       <c r="A23" s="3" t="s">
         <v>333</v>
       </c>
@@ -4524,8 +4161,21 @@
         <v>45792</v>
       </c>
     </row>
+    <row r="24" spans="1:4" ht="37.5">
+      <c r="A24" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="D24" s="5">
+        <v>45794</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
v3.8 Added SRS to match the change request
</commit_message>
<xml_diff>
--- a/LH_REQUIREMENTS/LH_SRS.xlsx
+++ b/LH_REQUIREMENTS/LH_SRS.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="349">
   <si>
     <t>Feature</t>
   </si>
@@ -1227,18 +1227,6 @@
     <t>LH-SRS-PUBART-014</t>
   </si>
   <si>
-    <t>LH-SRS-PUBART-015</t>
-  </si>
-  <si>
-    <t>LH-SRS-PUBART-016</t>
-  </si>
-  <si>
-    <t>if the title exceeds 40 characters show error message: title too long</t>
-  </si>
-  <si>
-    <t>each of these combined spaces counts as one char</t>
-  </si>
-  <si>
     <t>LH-CRS-PUBLISHAUDIO-005</t>
   </si>
   <si>
@@ -1248,31 +1236,22 @@
     <t>LH-SRS-PUBLISHAUDIO-013</t>
   </si>
   <si>
-    <t>LH-SRS-PUBLISHAUDIO-014</t>
-  </si>
-  <si>
-    <t>LH-SRS-PUBLISHAUDIO-015</t>
-  </si>
-  <si>
-    <t>the title should be less than or equal 40 characters</t>
-  </si>
-  <si>
-    <t>all consecutive spaces will count and show up as one</t>
-  </si>
-  <si>
     <t>LH-SRS-PUBLISHVIDEO-014</t>
   </si>
   <si>
     <t>LH-SRS-PUBLISHVIDEO-015</t>
   </si>
   <si>
-    <t>LH-SRS-PUBLISHVIDEO-016</t>
-  </si>
-  <si>
-    <t>LH-SRS-PUBLISHVIDEO-017</t>
-  </si>
-  <si>
     <t>LH-CRS-PUBLISHVIDEO-006</t>
+  </si>
+  <si>
+    <t>the title should be less than or equal 40 characters , if the title exceeds 40 characters show error message: title too long</t>
+  </si>
+  <si>
+    <t>v3.8</t>
+  </si>
+  <si>
+    <t>all consecutive spaces will count as one character and show up as one</t>
   </si>
 </sst>
 </file>
@@ -1559,7 +1538,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1672,103 +1651,97 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2047,10 +2020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G121"/>
+  <dimension ref="A1:G115"/>
   <sheetViews>
-    <sheetView topLeftCell="A81" zoomScale="62" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="H90" sqref="H90"/>
+    <sheetView topLeftCell="A57" zoomScale="79" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2081,10 +2054,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="86.45" customHeight="1">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="53" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -2098,8 +2071,8 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="39"/>
-      <c r="B3" s="51"/>
+      <c r="A3" s="61"/>
+      <c r="B3" s="54"/>
       <c r="C3" s="15" t="s">
         <v>10</v>
       </c>
@@ -2111,7 +2084,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="45">
-      <c r="A4" s="39"/>
+      <c r="A4" s="61"/>
       <c r="B4" s="16" t="s">
         <v>12</v>
       </c>
@@ -2126,8 +2099,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="43.15" customHeight="1">
-      <c r="A5" s="39"/>
-      <c r="B5" s="52" t="s">
+      <c r="A5" s="61"/>
+      <c r="B5" s="55" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="15" t="s">
@@ -2141,8 +2114,8 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="39"/>
-      <c r="B6" s="53"/>
+      <c r="A6" s="61"/>
+      <c r="B6" s="56"/>
       <c r="C6" s="15" t="s">
         <v>18</v>
       </c>
@@ -2154,8 +2127,8 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="39"/>
-      <c r="B7" s="53"/>
+      <c r="A7" s="61"/>
+      <c r="B7" s="56"/>
       <c r="C7" s="15" t="s">
         <v>20</v>
       </c>
@@ -2167,7 +2140,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="30">
-      <c r="A8" s="39"/>
+      <c r="A8" s="61"/>
       <c r="B8" s="17" t="s">
         <v>22</v>
       </c>
@@ -2182,7 +2155,7 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="39"/>
+      <c r="A9" s="61"/>
       <c r="B9" s="17" t="s">
         <v>25</v>
       </c>
@@ -2197,7 +2170,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="28.9" customHeight="1">
-      <c r="A10" s="39"/>
+      <c r="A10" s="61"/>
       <c r="B10" s="17" t="s">
         <v>28</v>
       </c>
@@ -2212,7 +2185,7 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="39"/>
+      <c r="A11" s="61"/>
       <c r="B11" s="17" t="s">
         <v>31</v>
       </c>
@@ -2227,8 +2200,8 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="39"/>
-      <c r="B12" s="52" t="s">
+      <c r="A12" s="61"/>
+      <c r="B12" s="55" t="s">
         <v>34</v>
       </c>
       <c r="C12" s="15" t="s">
@@ -2242,8 +2215,8 @@
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="39"/>
-      <c r="B13" s="53"/>
+      <c r="A13" s="61"/>
+      <c r="B13" s="56"/>
       <c r="C13" s="15" t="s">
         <v>37</v>
       </c>
@@ -2255,7 +2228,7 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="39"/>
+      <c r="A14" s="61"/>
       <c r="B14" s="17" t="s">
         <v>39</v>
       </c>
@@ -2270,10 +2243,10 @@
       </c>
     </row>
     <row r="15" spans="1:5" s="7" customFormat="1">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="54" t="s">
+      <c r="B15" s="41" t="s">
         <v>43</v>
       </c>
       <c r="C15" s="18" t="s">
@@ -2287,8 +2260,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" s="7" customFormat="1">
-      <c r="A16" s="41"/>
-      <c r="B16" s="55"/>
+      <c r="A16" s="66"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="18" t="s">
         <v>47</v>
       </c>
@@ -2300,8 +2273,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" s="7" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A17" s="41"/>
-      <c r="B17" s="55"/>
+      <c r="A17" s="66"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="18" t="s">
         <v>49</v>
       </c>
@@ -2313,8 +2286,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" s="7" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A18" s="41"/>
-      <c r="B18" s="55"/>
+      <c r="A18" s="66"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="18" t="s">
         <v>51</v>
       </c>
@@ -2326,8 +2299,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" s="7" customFormat="1">
-      <c r="A19" s="41"/>
-      <c r="B19" s="55"/>
+      <c r="A19" s="66"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="18" t="s">
         <v>53</v>
       </c>
@@ -2339,8 +2312,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" s="7" customFormat="1">
-      <c r="A20" s="41"/>
-      <c r="B20" s="56"/>
+      <c r="A20" s="66"/>
+      <c r="B20" s="42"/>
       <c r="C20" s="18" t="s">
         <v>55</v>
       </c>
@@ -2352,8 +2325,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" s="7" customFormat="1" ht="30">
-      <c r="A21" s="41"/>
-      <c r="B21" s="54" t="s">
+      <c r="A21" s="66"/>
+      <c r="B21" s="41" t="s">
         <v>57</v>
       </c>
       <c r="C21" s="18" t="s">
@@ -2367,8 +2340,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" s="7" customFormat="1">
-      <c r="A22" s="41"/>
-      <c r="B22" s="56"/>
+      <c r="A22" s="66"/>
+      <c r="B22" s="42"/>
       <c r="C22" s="18" t="s">
         <v>60</v>
       </c>
@@ -2380,7 +2353,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" s="8" customFormat="1">
-      <c r="A23" s="42" t="s">
+      <c r="A23" s="51" t="s">
         <v>62</v>
       </c>
       <c r="B23" s="19" t="s">
@@ -2397,7 +2370,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" s="8" customFormat="1">
-      <c r="A24" s="43"/>
+      <c r="A24" s="52"/>
       <c r="B24" s="19" t="s">
         <v>66</v>
       </c>
@@ -2412,7 +2385,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" s="8" customFormat="1">
-      <c r="A25" s="43"/>
+      <c r="A25" s="52"/>
       <c r="B25" s="19" t="s">
         <v>69</v>
       </c>
@@ -2427,7 +2400,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" s="8" customFormat="1">
-      <c r="A26" s="43"/>
+      <c r="A26" s="52"/>
       <c r="B26" s="19" t="s">
         <v>72</v>
       </c>
@@ -2442,7 +2415,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" s="8" customFormat="1">
-      <c r="A27" s="43"/>
+      <c r="A27" s="52"/>
       <c r="B27" s="19" t="s">
         <v>75</v>
       </c>
@@ -2457,7 +2430,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" s="8" customFormat="1">
-      <c r="A28" s="43"/>
+      <c r="A28" s="52"/>
       <c r="B28" s="19" t="s">
         <v>78</v>
       </c>
@@ -2472,7 +2445,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" s="8" customFormat="1">
-      <c r="A29" s="43"/>
+      <c r="A29" s="52"/>
       <c r="B29" s="19" t="s">
         <v>81</v>
       </c>
@@ -2487,7 +2460,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" s="8" customFormat="1">
-      <c r="A30" s="43"/>
+      <c r="A30" s="52"/>
       <c r="B30" s="19" t="s">
         <v>84</v>
       </c>
@@ -2502,7 +2475,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" s="8" customFormat="1">
-      <c r="A31" s="43"/>
+      <c r="A31" s="52"/>
       <c r="B31" s="19" t="s">
         <v>87</v>
       </c>
@@ -2517,7 +2490,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" s="8" customFormat="1">
-      <c r="A32" s="44"/>
+      <c r="A32" s="67"/>
       <c r="B32" s="19" t="s">
         <v>90</v>
       </c>
@@ -2532,7 +2505,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" s="7" customFormat="1" ht="16.5">
-      <c r="A33" s="40" t="s">
+      <c r="A33" s="65" t="s">
         <v>93</v>
       </c>
       <c r="B33" s="18" t="s">
@@ -2551,35 +2524,35 @@
       <c r="G33" s="20"/>
     </row>
     <row r="34" spans="1:7" s="7" customFormat="1" ht="30" customHeight="1">
-      <c r="A34" s="41"/>
+      <c r="A34" s="66"/>
       <c r="B34" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C34" s="54" t="s">
+      <c r="C34" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="D34" s="54" t="s">
+      <c r="D34" s="41" t="s">
         <v>100</v>
       </c>
-      <c r="E34" s="54" t="s">
+      <c r="E34" s="41" t="s">
         <v>101</v>
       </c>
       <c r="F34" s="20"/>
       <c r="G34" s="20"/>
     </row>
     <row r="35" spans="1:7" s="7" customFormat="1" ht="75" customHeight="1">
-      <c r="A35" s="45"/>
+      <c r="A35" s="68"/>
       <c r="B35" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="C35" s="56"/>
-      <c r="D35" s="56"/>
-      <c r="E35" s="56"/>
+      <c r="C35" s="42"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="42"/>
       <c r="F35" s="20"/>
       <c r="G35" s="20"/>
     </row>
     <row r="36" spans="1:7" s="8" customFormat="1" ht="30" customHeight="1">
-      <c r="A36" s="42" t="s">
+      <c r="A36" s="51" t="s">
         <v>103</v>
       </c>
       <c r="B36" s="57" t="s">
@@ -2596,7 +2569,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" s="8" customFormat="1" ht="30" customHeight="1">
-      <c r="A37" s="43"/>
+      <c r="A37" s="52"/>
       <c r="B37" s="57"/>
       <c r="C37" s="19" t="s">
         <v>107</v>
@@ -2609,7 +2582,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" s="8" customFormat="1" ht="30" customHeight="1">
-      <c r="A38" s="43"/>
+      <c r="A38" s="52"/>
       <c r="B38" s="57" t="s">
         <v>109</v>
       </c>
@@ -2624,7 +2597,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" s="8" customFormat="1" ht="30" customHeight="1">
-      <c r="A39" s="43"/>
+      <c r="A39" s="52"/>
       <c r="B39" s="57"/>
       <c r="C39" s="19" t="s">
         <v>112</v>
@@ -2637,7 +2610,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" s="8" customFormat="1" ht="30" customHeight="1">
-      <c r="A40" s="43"/>
+      <c r="A40" s="52"/>
       <c r="B40" s="21" t="s">
         <v>114</v>
       </c>
@@ -2652,7 +2625,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" s="8" customFormat="1" ht="30" customHeight="1">
-      <c r="A41" s="43"/>
+      <c r="A41" s="52"/>
       <c r="B41" s="21" t="s">
         <v>117</v>
       </c>
@@ -2667,7 +2640,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" s="8" customFormat="1" ht="15.75">
-      <c r="A42" s="43"/>
+      <c r="A42" s="52"/>
       <c r="B42" s="21" t="s">
         <v>120</v>
       </c>
@@ -2682,7 +2655,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" s="8" customFormat="1">
-      <c r="A43" s="43"/>
+      <c r="A43" s="52"/>
       <c r="B43" s="58" t="s">
         <v>123</v>
       </c>
@@ -2697,7 +2670,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" s="8" customFormat="1">
-      <c r="A44" s="43"/>
+      <c r="A44" s="52"/>
       <c r="B44" s="59"/>
       <c r="C44" s="19" t="s">
         <v>126</v>
@@ -2710,7 +2683,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" s="8" customFormat="1">
-      <c r="A45" s="43"/>
+      <c r="A45" s="52"/>
       <c r="B45" s="58" t="s">
         <v>128</v>
       </c>
@@ -2725,7 +2698,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" s="8" customFormat="1">
-      <c r="A46" s="43"/>
+      <c r="A46" s="52"/>
       <c r="B46" s="59"/>
       <c r="C46" s="19" t="s">
         <v>131</v>
@@ -2738,7 +2711,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" s="8" customFormat="1" ht="15.75">
-      <c r="A47" s="43"/>
+      <c r="A47" s="52"/>
       <c r="B47" s="21" t="s">
         <v>133</v>
       </c>
@@ -2753,7 +2726,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" s="8" customFormat="1" ht="15.75">
-      <c r="A48" s="43"/>
+      <c r="A48" s="52"/>
       <c r="B48" s="21" t="s">
         <v>136</v>
       </c>
@@ -2768,7 +2741,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" s="8" customFormat="1" ht="15.75">
-      <c r="A49" s="43"/>
+      <c r="A49" s="52"/>
       <c r="B49" s="21" t="s">
         <v>139</v>
       </c>
@@ -2783,7 +2756,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" s="8" customFormat="1" ht="15.75">
-      <c r="A50" s="43"/>
+      <c r="A50" s="52"/>
       <c r="B50" s="21" t="s">
         <v>142</v>
       </c>
@@ -2798,7 +2771,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" s="8" customFormat="1" ht="30">
-      <c r="A51" s="43"/>
+      <c r="A51" s="52"/>
       <c r="B51" s="58" t="s">
         <v>145</v>
       </c>
@@ -2813,7 +2786,7 @@
       </c>
     </row>
     <row r="52" spans="1:5" s="8" customFormat="1" ht="30">
-      <c r="A52" s="43"/>
+      <c r="A52" s="52"/>
       <c r="B52" s="59"/>
       <c r="C52" s="19" t="s">
         <v>148</v>
@@ -2826,10 +2799,10 @@
       </c>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="46" t="s">
+      <c r="A53" s="63" t="s">
         <v>150</v>
       </c>
-      <c r="B53" s="60" t="s">
+      <c r="B53" s="43" t="s">
         <v>151</v>
       </c>
       <c r="C53" s="22" t="s">
@@ -2843,8 +2816,8 @@
       </c>
     </row>
     <row r="54" spans="1:5">
-      <c r="A54" s="47"/>
-      <c r="B54" s="61"/>
+      <c r="A54" s="64"/>
+      <c r="B54" s="44"/>
       <c r="C54" s="22" t="s">
         <v>154</v>
       </c>
@@ -2856,8 +2829,8 @@
       </c>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="47"/>
-      <c r="B55" s="61"/>
+      <c r="A55" s="64"/>
+      <c r="B55" s="44"/>
       <c r="C55" s="22" t="s">
         <v>156</v>
       </c>
@@ -2869,8 +2842,8 @@
       </c>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="47"/>
-      <c r="B56" s="62"/>
+      <c r="A56" s="64"/>
+      <c r="B56" s="45"/>
       <c r="C56" s="22" t="s">
         <v>158</v>
       </c>
@@ -2882,8 +2855,8 @@
       </c>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="47"/>
-      <c r="B57" s="60" t="s">
+      <c r="A57" s="64"/>
+      <c r="B57" s="43" t="s">
         <v>160</v>
       </c>
       <c r="C57" s="22" t="s">
@@ -2897,8 +2870,8 @@
       </c>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="47"/>
-      <c r="B58" s="61"/>
+      <c r="A58" s="64"/>
+      <c r="B58" s="44"/>
       <c r="C58" s="22" t="s">
         <v>163</v>
       </c>
@@ -2910,8 +2883,8 @@
       </c>
     </row>
     <row r="59" spans="1:5" ht="30">
-      <c r="A59" s="47"/>
-      <c r="B59" s="61"/>
+      <c r="A59" s="64"/>
+      <c r="B59" s="44"/>
       <c r="C59" s="22" t="s">
         <v>165</v>
       </c>
@@ -2923,8 +2896,8 @@
       </c>
     </row>
     <row r="60" spans="1:5" ht="30">
-      <c r="A60" s="47"/>
-      <c r="B60" s="62"/>
+      <c r="A60" s="64"/>
+      <c r="B60" s="45"/>
       <c r="C60" s="22" t="s">
         <v>167</v>
       </c>
@@ -2936,7 +2909,7 @@
       </c>
     </row>
     <row r="61" spans="1:5" ht="30">
-      <c r="A61" s="47"/>
+      <c r="A61" s="64"/>
       <c r="B61" s="23" t="s">
         <v>169</v>
       </c>
@@ -2951,7 +2924,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" ht="30">
-      <c r="A62" s="47"/>
+      <c r="A62" s="64"/>
       <c r="B62" s="23" t="s">
         <v>172</v>
       </c>
@@ -2966,8 +2939,8 @@
       </c>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="47"/>
-      <c r="B63" s="60" t="s">
+      <c r="A63" s="64"/>
+      <c r="B63" s="43" t="s">
         <v>175</v>
       </c>
       <c r="C63" s="22" t="s">
@@ -2981,8 +2954,8 @@
       </c>
     </row>
     <row r="64" spans="1:5" ht="30">
-      <c r="A64" s="47"/>
-      <c r="B64" s="62"/>
+      <c r="A64" s="64"/>
+      <c r="B64" s="45"/>
       <c r="C64" s="22" t="s">
         <v>178</v>
       </c>
@@ -2993,802 +2966,720 @@
         <v>46</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
-      <c r="A65" s="47"/>
-      <c r="B65" s="60" t="s">
+    <row r="65" spans="1:5" ht="30">
+      <c r="A65" s="64"/>
+      <c r="B65" s="43" t="s">
         <v>337</v>
       </c>
       <c r="C65" s="22" t="s">
         <v>338</v>
       </c>
       <c r="D65" s="22" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E65" s="22" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
-      <c r="A66" s="47"/>
-      <c r="B66" s="61"/>
+    <row r="66" spans="1:5" ht="24.75" customHeight="1">
+      <c r="A66" s="64"/>
+      <c r="B66" s="44"/>
       <c r="C66" s="22" t="s">
         <v>339</v>
       </c>
       <c r="D66" s="22" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="E66" s="22" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
-      <c r="A67" s="47"/>
-      <c r="B67" s="61"/>
-      <c r="C67" s="22" t="s">
-        <v>340</v>
-      </c>
-      <c r="D67" s="22" t="s">
-        <v>350</v>
-      </c>
-      <c r="E67" s="22" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
-      <c r="A68" s="48"/>
-      <c r="B68" s="62"/>
-      <c r="C68" s="22" t="s">
-        <v>341</v>
-      </c>
-      <c r="D68" s="22" t="s">
-        <v>343</v>
-      </c>
-      <c r="E68" s="22" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A69" s="38" t="s">
+    <row r="67" spans="1:5" ht="40.5" customHeight="1">
+      <c r="A67" s="60" t="s">
         <v>180</v>
       </c>
-      <c r="B69" s="63" t="s">
+      <c r="B67" s="46" t="s">
         <v>181</v>
       </c>
+      <c r="C67" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="D67" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="E67" s="15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="30">
+      <c r="A68" s="61"/>
+      <c r="B68" s="47"/>
+      <c r="C68" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="D68" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="E68" s="15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A69" s="61"/>
+      <c r="B69" s="47"/>
       <c r="C69" s="15" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="D69" s="15" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E69" s="15" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="30">
-      <c r="A70" s="39"/>
-      <c r="B70" s="64"/>
+    <row r="70" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A70" s="61"/>
+      <c r="B70" s="48"/>
       <c r="C70" s="15" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="D70" s="15" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E70" s="15" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A71" s="39"/>
-      <c r="B71" s="64"/>
+    <row r="71" spans="1:5" ht="30">
+      <c r="A71" s="61"/>
+      <c r="B71" s="46" t="s">
+        <v>190</v>
+      </c>
       <c r="C71" s="15" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="D71" s="15" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="E71" s="15" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A72" s="39"/>
-      <c r="B72" s="65"/>
+    <row r="72" spans="1:5" ht="30">
+      <c r="A72" s="61"/>
+      <c r="B72" s="48"/>
       <c r="C72" s="15" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="D72" s="15" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="E72" s="15" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="30">
-      <c r="A73" s="39"/>
-      <c r="B73" s="63" t="s">
-        <v>190</v>
+      <c r="A73" s="61"/>
+      <c r="B73" s="46" t="s">
+        <v>195</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="D73" s="15" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="E73" s="15" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="30">
-      <c r="A74" s="39"/>
-      <c r="B74" s="65"/>
+      <c r="A74" s="61"/>
+      <c r="B74" s="47"/>
       <c r="C74" s="15" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="D74" s="15" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="E74" s="15" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="30">
-      <c r="A75" s="39"/>
-      <c r="B75" s="63" t="s">
-        <v>195</v>
-      </c>
+      <c r="A75" s="61"/>
+      <c r="B75" s="47"/>
       <c r="C75" s="15" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="D75" s="15" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="E75" s="15" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="30">
-      <c r="A76" s="39"/>
-      <c r="B76" s="64"/>
+      <c r="A76" s="61"/>
+      <c r="B76" s="46" t="s">
+        <v>202</v>
+      </c>
       <c r="C76" s="15" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="D76" s="15" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="E76" s="15" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="30">
-      <c r="A77" s="39"/>
-      <c r="B77" s="64"/>
+    <row r="77" spans="1:5" ht="32.25" customHeight="1">
+      <c r="A77" s="61"/>
+      <c r="B77" s="48"/>
       <c r="C77" s="15" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="D77" s="15" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="E77" s="15" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="30">
-      <c r="A78" s="39"/>
-      <c r="B78" s="63" t="s">
-        <v>202</v>
+    <row r="78" spans="1:5" ht="34.5" customHeight="1">
+      <c r="A78" s="61"/>
+      <c r="B78" s="46" t="s">
+        <v>340</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="D78" s="15" t="s">
-        <v>204</v>
-      </c>
-      <c r="E78" s="15" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="30">
-      <c r="A79" s="39"/>
-      <c r="B79" s="65"/>
+        <v>341</v>
+      </c>
+      <c r="D78" s="22" t="s">
+        <v>346</v>
+      </c>
+      <c r="E78" s="22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="32.25" customHeight="1">
+      <c r="A79" s="61"/>
+      <c r="B79" s="47"/>
       <c r="C79" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="D79" s="15" t="s">
-        <v>206</v>
-      </c>
-      <c r="E79" s="15" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A80" s="39"/>
-      <c r="B80" s="63" t="s">
-        <v>344</v>
-      </c>
-      <c r="C80" s="15" t="s">
-        <v>345</v>
+        <v>342</v>
+      </c>
+      <c r="D79" s="22" t="s">
+        <v>348</v>
+      </c>
+      <c r="E79" s="22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="30">
+      <c r="A80" s="63" t="s">
+        <v>207</v>
+      </c>
+      <c r="B80" s="43" t="s">
+        <v>208</v>
+      </c>
+      <c r="C80" s="18" t="s">
+        <v>209</v>
       </c>
       <c r="D80" s="22" t="s">
-        <v>349</v>
+        <v>210</v>
       </c>
       <c r="E80" s="22" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A81" s="39"/>
-      <c r="B81" s="64"/>
-      <c r="C81" s="15" t="s">
-        <v>346</v>
+        <v>211</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="30">
+      <c r="A81" s="64"/>
+      <c r="B81" s="44"/>
+      <c r="C81" s="18" t="s">
+        <v>212</v>
       </c>
       <c r="D81" s="22" t="s">
-        <v>342</v>
+        <v>155</v>
       </c>
       <c r="E81" s="22" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A82" s="39"/>
-      <c r="B82" s="64"/>
-      <c r="C82" s="15" t="s">
-        <v>347</v>
+        <v>211</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="30">
+      <c r="A82" s="64"/>
+      <c r="B82" s="44"/>
+      <c r="C82" s="18" t="s">
+        <v>213</v>
       </c>
       <c r="D82" s="22" t="s">
-        <v>350</v>
+        <v>214</v>
       </c>
       <c r="E82" s="22" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A83" s="70"/>
-      <c r="B83" s="65"/>
-      <c r="C83" s="15" t="s">
-        <v>348</v>
+        <v>211</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="30">
+      <c r="A83" s="64"/>
+      <c r="B83" s="44"/>
+      <c r="C83" s="18" t="s">
+        <v>215</v>
       </c>
       <c r="D83" s="22" t="s">
-        <v>343</v>
+        <v>216</v>
       </c>
       <c r="E83" s="22" t="s">
-        <v>101</v>
+        <v>211</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="30">
-      <c r="A84" s="46" t="s">
-        <v>207</v>
-      </c>
-      <c r="B84" s="60" t="s">
-        <v>208</v>
-      </c>
+      <c r="A84" s="64"/>
+      <c r="B84" s="44"/>
       <c r="C84" s="18" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="D84" s="22" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="E84" s="22" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="30">
-      <c r="A85" s="47"/>
-      <c r="B85" s="61"/>
+      <c r="A85" s="64"/>
+      <c r="B85" s="22" t="s">
+        <v>219</v>
+      </c>
       <c r="C85" s="18" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="D85" s="22" t="s">
-        <v>155</v>
+        <v>221</v>
       </c>
       <c r="E85" s="22" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="30">
-      <c r="A86" s="47"/>
-      <c r="B86" s="61"/>
+    <row r="86" spans="1:5" ht="45">
+      <c r="A86" s="64"/>
+      <c r="B86" s="43" t="s">
+        <v>222</v>
+      </c>
       <c r="C86" s="18" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="D86" s="22" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="E86" s="22" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="30">
-      <c r="A87" s="47"/>
-      <c r="B87" s="61"/>
+      <c r="A87" s="64"/>
+      <c r="B87" s="45"/>
       <c r="C87" s="18" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="D87" s="22" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="E87" s="22" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="30">
-      <c r="A88" s="47"/>
-      <c r="B88" s="61"/>
+      <c r="A88" s="64"/>
+      <c r="B88" s="43" t="s">
+        <v>227</v>
+      </c>
       <c r="C88" s="18" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
       <c r="D88" s="22" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="E88" s="22" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="30">
-      <c r="A89" s="47"/>
-      <c r="B89" s="22" t="s">
-        <v>219</v>
-      </c>
+      <c r="A89" s="64"/>
+      <c r="B89" s="44"/>
       <c r="C89" s="18" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="D89" s="22" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
       <c r="E89" s="22" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="45">
-      <c r="A90" s="47"/>
-      <c r="B90" s="60" t="s">
-        <v>222</v>
-      </c>
+    <row r="90" spans="1:5" ht="30">
+      <c r="A90" s="64"/>
+      <c r="B90" s="45"/>
       <c r="C90" s="18" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="D90" s="22" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="E90" s="22" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="30">
-      <c r="A91" s="47"/>
-      <c r="B91" s="62"/>
+      <c r="A91" s="64"/>
+      <c r="B91" s="41" t="s">
+        <v>234</v>
+      </c>
       <c r="C91" s="18" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="D91" s="22" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
       <c r="E91" s="22" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="30">
-      <c r="A92" s="47"/>
-      <c r="B92" s="60" t="s">
-        <v>227</v>
-      </c>
+      <c r="A92" s="64"/>
+      <c r="B92" s="42"/>
       <c r="C92" s="18" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="D92" s="22" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="E92" s="22" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="30">
-      <c r="A93" s="47"/>
-      <c r="B93" s="61"/>
+      <c r="A93" s="64"/>
+      <c r="B93" s="41" t="s">
+        <v>345</v>
+      </c>
       <c r="C93" s="18" t="s">
-        <v>230</v>
+        <v>343</v>
       </c>
       <c r="D93" s="22" t="s">
-        <v>231</v>
+        <v>346</v>
       </c>
       <c r="E93" s="22" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="30">
-      <c r="A94" s="47"/>
-      <c r="B94" s="62"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="33.75" customHeight="1">
+      <c r="A94" s="64"/>
+      <c r="B94" s="49"/>
       <c r="C94" s="18" t="s">
-        <v>232</v>
+        <v>344</v>
       </c>
       <c r="D94" s="22" t="s">
-        <v>233</v>
+        <v>348</v>
       </c>
       <c r="E94" s="22" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" ht="30">
-      <c r="A95" s="47"/>
-      <c r="B95" s="54" t="s">
-        <v>234</v>
-      </c>
-      <c r="C95" s="18" t="s">
-        <v>235</v>
-      </c>
-      <c r="D95" s="22" t="s">
-        <v>236</v>
-      </c>
-      <c r="E95" s="22" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="30">
-      <c r="A96" s="47"/>
-      <c r="B96" s="56"/>
-      <c r="C96" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="D96" s="22" t="s">
-        <v>238</v>
-      </c>
-      <c r="E96" s="22" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5">
-      <c r="A97" s="47"/>
-      <c r="B97" s="54" t="s">
-        <v>355</v>
-      </c>
-      <c r="C97" s="18" t="s">
-        <v>351</v>
-      </c>
-      <c r="D97" s="22" t="s">
-        <v>349</v>
-      </c>
-      <c r="E97" s="22" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="98" spans="1:5">
-      <c r="A98" s="47"/>
-      <c r="B98" s="55"/>
-      <c r="C98" s="18" t="s">
-        <v>352</v>
-      </c>
-      <c r="D98" s="22" t="s">
-        <v>342</v>
-      </c>
-      <c r="E98" s="22" t="s">
+    <row r="95" spans="1:5" ht="69.95" customHeight="1">
+      <c r="A95" s="60" t="s">
+        <v>239</v>
+      </c>
+      <c r="B95" s="46" t="s">
+        <v>240</v>
+      </c>
+      <c r="C95" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="D95" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="E95" s="15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="99" spans="1:5">
-      <c r="A99" s="47"/>
-      <c r="B99" s="55"/>
-      <c r="C99" s="18" t="s">
-        <v>353</v>
-      </c>
-      <c r="D99" s="22" t="s">
-        <v>350</v>
-      </c>
-      <c r="E99" s="22" t="s">
+    <row r="96" spans="1:5" ht="45">
+      <c r="A96" s="61"/>
+      <c r="B96" s="47"/>
+      <c r="C96" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="D96" s="24" t="s">
+        <v>244</v>
+      </c>
+      <c r="E96" s="15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="100" spans="1:5">
-      <c r="A100" s="48"/>
-      <c r="B100" s="56"/>
-      <c r="C100" s="18" t="s">
-        <v>354</v>
-      </c>
-      <c r="D100" s="22" t="s">
-        <v>343</v>
-      </c>
-      <c r="E100" s="22" t="s">
+    <row r="97" spans="1:5" ht="45">
+      <c r="A97" s="61"/>
+      <c r="B97" s="47"/>
+      <c r="C97" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="D97" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="E97" s="15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="69.95" customHeight="1">
-      <c r="A101" s="38" t="s">
-        <v>239</v>
-      </c>
-      <c r="B101" s="63" t="s">
-        <v>240</v>
+    <row r="98" spans="1:5" ht="30">
+      <c r="A98" s="61"/>
+      <c r="B98" s="48"/>
+      <c r="C98" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="D98" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="E98" s="15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="50.1" customHeight="1">
+      <c r="A99" s="61"/>
+      <c r="B99" s="46" t="s">
+        <v>249</v>
+      </c>
+      <c r="C99" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="D99" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="E99" s="15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="30">
+      <c r="A100" s="61"/>
+      <c r="B100" s="47"/>
+      <c r="C100" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="D100" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="E100" s="15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="63.95" customHeight="1">
+      <c r="A101" s="61"/>
+      <c r="B101" s="50" t="s">
+        <v>254</v>
       </c>
       <c r="C101" s="15" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="D101" s="15" t="s">
-        <v>242</v>
+        <v>256</v>
       </c>
       <c r="E101" s="15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="45">
-      <c r="A102" s="39"/>
-      <c r="B102" s="64"/>
-      <c r="C102" s="15" t="s">
-        <v>243</v>
-      </c>
-      <c r="D102" s="24" t="s">
-        <v>244</v>
-      </c>
-      <c r="E102" s="15" t="s">
+    <row r="102" spans="1:5" ht="30">
+      <c r="A102" s="61"/>
+      <c r="B102" s="50"/>
+      <c r="C102" s="25" t="s">
+        <v>257</v>
+      </c>
+      <c r="D102" s="25" t="s">
+        <v>258</v>
+      </c>
+      <c r="E102" s="25" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="45">
-      <c r="A103" s="39"/>
-      <c r="B103" s="64"/>
-      <c r="C103" s="15" t="s">
-        <v>245</v>
-      </c>
-      <c r="D103" s="24" t="s">
-        <v>246</v>
-      </c>
-      <c r="E103" s="15" t="s">
+    <row r="103" spans="1:5" ht="30">
+      <c r="A103" s="62" t="s">
+        <v>259</v>
+      </c>
+      <c r="B103" s="38" t="s">
+        <v>260</v>
+      </c>
+      <c r="C103" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="D103" s="27" t="s">
+        <v>262</v>
+      </c>
+      <c r="E103" s="26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="30">
+      <c r="A104" s="62"/>
+      <c r="B104" s="38"/>
+      <c r="C104" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="D104" s="27" t="s">
+        <v>264</v>
+      </c>
+      <c r="E104" s="26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="30">
+      <c r="A105" s="62"/>
+      <c r="B105" s="38" t="s">
+        <v>265</v>
+      </c>
+      <c r="C105" s="18" t="s">
+        <v>266</v>
+      </c>
+      <c r="D105" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="E105" s="26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="30">
+      <c r="A106" s="62"/>
+      <c r="B106" s="38"/>
+      <c r="C106" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="D106" s="27" t="s">
+        <v>269</v>
+      </c>
+      <c r="E106" s="26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="30">
+      <c r="A107" s="62"/>
+      <c r="B107" s="38"/>
+      <c r="C107" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="D107" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="E107" s="26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="45">
+      <c r="A108" s="51" t="s">
+        <v>272</v>
+      </c>
+      <c r="B108" s="39" t="s">
+        <v>273</v>
+      </c>
+      <c r="C108" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="D108" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="E108" s="19" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="30">
-      <c r="A104" s="39"/>
-      <c r="B104" s="65"/>
-      <c r="C104" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="D104" s="24" t="s">
-        <v>248</v>
-      </c>
-      <c r="E104" s="15" t="s">
+    <row r="109" spans="1:5" ht="45">
+      <c r="A109" s="52"/>
+      <c r="B109" s="40"/>
+      <c r="C109" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="D109" s="29" t="s">
+        <v>277</v>
+      </c>
+      <c r="E109" s="19" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="50.1" customHeight="1">
-      <c r="A105" s="39"/>
-      <c r="B105" s="63" t="s">
-        <v>249</v>
-      </c>
-      <c r="C105" s="15" t="s">
-        <v>250</v>
-      </c>
-      <c r="D105" s="15" t="s">
-        <v>251</v>
-      </c>
-      <c r="E105" s="15" t="s">
+    <row r="110" spans="1:5" ht="45">
+      <c r="A110" s="52"/>
+      <c r="B110" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="C110" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="D110" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="E110" s="19" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="30">
-      <c r="A106" s="39"/>
-      <c r="B106" s="64"/>
-      <c r="C106" s="15" t="s">
-        <v>252</v>
-      </c>
-      <c r="D106" s="15" t="s">
-        <v>253</v>
-      </c>
-      <c r="E106" s="15" t="s">
+    <row r="111" spans="1:5" ht="30">
+      <c r="A111" s="52"/>
+      <c r="B111" s="30" t="s">
+        <v>281</v>
+      </c>
+      <c r="C111" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="D111" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="E111" s="19" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="63.95" customHeight="1">
-      <c r="A107" s="39"/>
-      <c r="B107" s="66" t="s">
-        <v>254</v>
-      </c>
-      <c r="C107" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D107" s="15" t="s">
-        <v>256</v>
-      </c>
-      <c r="E107" s="15" t="s">
+    <row r="112" spans="1:5" ht="15" customHeight="1">
+      <c r="A112" s="52"/>
+      <c r="B112" s="28" t="s">
+        <v>284</v>
+      </c>
+      <c r="C112" s="31" t="s">
+        <v>285</v>
+      </c>
+      <c r="D112" s="31" t="s">
+        <v>286</v>
+      </c>
+      <c r="E112" s="31" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="30">
-      <c r="A108" s="39"/>
-      <c r="B108" s="66"/>
-      <c r="C108" s="25" t="s">
-        <v>257</v>
-      </c>
-      <c r="D108" s="25" t="s">
-        <v>258</v>
-      </c>
-      <c r="E108" s="25" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" ht="30">
-      <c r="A109" s="49" t="s">
-        <v>259</v>
-      </c>
-      <c r="B109" s="67" t="s">
-        <v>260</v>
-      </c>
-      <c r="C109" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="D109" s="27" t="s">
-        <v>262</v>
-      </c>
-      <c r="E109" s="26" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" ht="30">
-      <c r="A110" s="49"/>
-      <c r="B110" s="67"/>
-      <c r="C110" s="18" t="s">
-        <v>263</v>
-      </c>
-      <c r="D110" s="27" t="s">
-        <v>264</v>
-      </c>
-      <c r="E110" s="26" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" ht="30">
-      <c r="A111" s="49"/>
-      <c r="B111" s="67" t="s">
-        <v>265</v>
-      </c>
-      <c r="C111" s="18" t="s">
-        <v>266</v>
-      </c>
-      <c r="D111" s="27" t="s">
-        <v>267</v>
-      </c>
-      <c r="E111" s="26" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" ht="30">
-      <c r="A112" s="49"/>
-      <c r="B112" s="67"/>
-      <c r="C112" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="D112" s="27" t="s">
-        <v>269</v>
-      </c>
-      <c r="E112" s="26" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" ht="30">
-      <c r="A113" s="49"/>
-      <c r="B113" s="67"/>
-      <c r="C113" s="18" t="s">
-        <v>270</v>
-      </c>
-      <c r="D113" s="22" t="s">
-        <v>271</v>
-      </c>
-      <c r="E113" s="26" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" ht="45">
-      <c r="A114" s="42" t="s">
-        <v>272</v>
-      </c>
-      <c r="B114" s="68" t="s">
-        <v>273</v>
-      </c>
-      <c r="C114" s="19" t="s">
-        <v>274</v>
-      </c>
-      <c r="D114" s="19" t="s">
-        <v>275</v>
-      </c>
-      <c r="E114" s="19" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" ht="45">
-      <c r="A115" s="43"/>
-      <c r="B115" s="69"/>
-      <c r="C115" s="19" t="s">
-        <v>276</v>
-      </c>
-      <c r="D115" s="29" t="s">
-        <v>277</v>
-      </c>
-      <c r="E115" s="19" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" ht="45">
-      <c r="A116" s="43"/>
-      <c r="B116" s="30" t="s">
-        <v>278</v>
-      </c>
-      <c r="C116" s="19" t="s">
-        <v>279</v>
-      </c>
-      <c r="D116" s="19" t="s">
-        <v>280</v>
-      </c>
-      <c r="E116" s="19" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" ht="30">
-      <c r="A117" s="43"/>
-      <c r="B117" s="30" t="s">
-        <v>281</v>
-      </c>
-      <c r="C117" s="19" t="s">
-        <v>282</v>
-      </c>
-      <c r="D117" s="19" t="s">
-        <v>283</v>
-      </c>
-      <c r="E117" s="19" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" ht="15" customHeight="1">
-      <c r="A118" s="43"/>
-      <c r="B118" s="28" t="s">
-        <v>284</v>
-      </c>
-      <c r="C118" s="31" t="s">
-        <v>285</v>
-      </c>
-      <c r="D118" s="31" t="s">
-        <v>286</v>
-      </c>
-      <c r="E118" s="31" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" ht="15" customHeight="1">
-      <c r="A119" s="32"/>
-      <c r="B119" s="33"/>
-      <c r="C119" s="33"/>
-      <c r="D119" s="34"/>
-      <c r="E119" s="33"/>
-    </row>
-    <row r="120" spans="1:5">
-      <c r="A120" s="35"/>
-      <c r="B120" s="36"/>
-      <c r="C120" s="36"/>
-      <c r="D120" s="37"/>
-      <c r="E120" s="36"/>
-    </row>
-    <row r="121" spans="1:5">
-      <c r="A121" s="36"/>
-      <c r="B121" s="36"/>
-      <c r="C121" s="36"/>
-      <c r="D121" s="37"/>
-      <c r="E121" s="36"/>
+    <row r="113" spans="1:5" ht="15" customHeight="1">
+      <c r="A113" s="32"/>
+      <c r="B113" s="33"/>
+      <c r="C113" s="33"/>
+      <c r="D113" s="34"/>
+      <c r="E113" s="33"/>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114" s="35"/>
+      <c r="B114" s="36"/>
+      <c r="C114" s="36"/>
+      <c r="D114" s="37"/>
+      <c r="E114" s="36"/>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" s="36"/>
+      <c r="B115" s="36"/>
+      <c r="C115" s="36"/>
+      <c r="D115" s="37"/>
+      <c r="E115" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="B111:B113"/>
-    <mergeCell ref="B114:B115"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B80:B83"/>
-    <mergeCell ref="B97:B100"/>
-    <mergeCell ref="B95:B96"/>
-    <mergeCell ref="B101:B104"/>
-    <mergeCell ref="B105:B106"/>
-    <mergeCell ref="B107:B108"/>
-    <mergeCell ref="B109:B110"/>
-    <mergeCell ref="B75:B77"/>
-    <mergeCell ref="B78:B79"/>
-    <mergeCell ref="B84:B88"/>
-    <mergeCell ref="B90:B91"/>
-    <mergeCell ref="B92:B94"/>
-    <mergeCell ref="A114:A118"/>
+    <mergeCell ref="A2:A14"/>
+    <mergeCell ref="A15:A22"/>
+    <mergeCell ref="A23:A32"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A36:A52"/>
+    <mergeCell ref="B67:B70"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="A95:A102"/>
+    <mergeCell ref="A103:A107"/>
+    <mergeCell ref="A53:A66"/>
+    <mergeCell ref="A67:A79"/>
+    <mergeCell ref="A80:A94"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="B88:B90"/>
+    <mergeCell ref="A108:A112"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="B12:B13"/>
@@ -3802,18 +3693,22 @@
     <mergeCell ref="B53:B56"/>
     <mergeCell ref="B57:B60"/>
     <mergeCell ref="B63:B64"/>
-    <mergeCell ref="B69:B72"/>
-    <mergeCell ref="B73:B74"/>
-    <mergeCell ref="A101:A108"/>
-    <mergeCell ref="A109:A113"/>
-    <mergeCell ref="A53:A68"/>
-    <mergeCell ref="A69:A83"/>
-    <mergeCell ref="A84:A100"/>
-    <mergeCell ref="A2:A14"/>
-    <mergeCell ref="A15:A22"/>
-    <mergeCell ref="A23:A32"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A36:A52"/>
+    <mergeCell ref="B105:B107"/>
+    <mergeCell ref="B108:B109"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="B93:B94"/>
+    <mergeCell ref="B91:B92"/>
+    <mergeCell ref="B95:B98"/>
+    <mergeCell ref="B99:B100"/>
+    <mergeCell ref="B101:B102"/>
+    <mergeCell ref="B103:B104"/>
+    <mergeCell ref="B73:B75"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="B80:B84"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" sqref="A36:A41"/>
@@ -3825,10 +3720,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4175,6 +4070,20 @@
         <v>45794</v>
       </c>
     </row>
+    <row r="25" spans="1:4" ht="37.5">
+      <c r="A25" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="D25" s="5">
+        <v>45794</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>